<commit_message>
fix test data, small update to missed renamings on modules
</commit_message>
<xml_diff>
--- a/tests/data/_schema/conceptual/only_concepts.xlsx
+++ b/tests/data/_schema/conceptual/only_concepts.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10512"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AndersAlbert\Projects\internal\neat\tests\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nikola/Repos/neat/tests/data/_schema/conceptual/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B24E51D4-BDA2-4CB4-85AA-7439C45A42FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6686FB3-51CC-9A4D-B93E-56A519791CEC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="48520" windowHeight="27500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Metadata" sheetId="1" r:id="rId1"/>
@@ -106,183 +106,6 @@
     <t>Implements</t>
   </si>
   <si>
-    <t>http://purl.org/cognite/neat/data-model/verified/logical/neat_space/NeatInferredDataModel/v1/CircuitShare</t>
-  </si>
-  <si>
-    <t>http://purl.org/cognite/neat/data-model/verified/logical/neat_space/NeatInferredDataModel/v1/EnergyCongestionZone</t>
-  </si>
-  <si>
-    <t>http://purl.org/cognite/neat/data-model/verified/logical/neat_space/NeatInferredDataModel/v1/EnergySchedulingArea</t>
-  </si>
-  <si>
-    <t>http://purl.org/cognite/neat/data-model/verified/logical/neat_space/NeatInferredDataModel/v1/LineCircuit</t>
-  </si>
-  <si>
-    <t>http://purl.org/cognite/neat/data-model/verified/logical/neat_space/NeatInferredDataModel/v1/PowerTransferCorridor</t>
-  </si>
-  <si>
-    <t>http://purl.org/cognite/neat/data-model/verified/logical/neat_space/NeatInferredDataModel/v1/RateTemperature</t>
-  </si>
-  <si>
-    <t>http://purl.org/cognite/neat/data-model/verified/logical/neat_space/NeatInferredDataModel/v1/ACLineSegment</t>
-  </si>
-  <si>
-    <t>http://purl.org/cognite/neat/data-model/verified/logical/neat_space/NeatInferredDataModel/v1/ActivePowerLimit</t>
-  </si>
-  <si>
-    <t>http://purl.org/cognite/neat/data-model/verified/logical/neat_space/NeatInferredDataModel/v1/Analog</t>
-  </si>
-  <si>
-    <t>http://purl.org/cognite/neat/data-model/verified/logical/neat_space/NeatInferredDataModel/v1/AnalogValue</t>
-  </si>
-  <si>
-    <t>http://purl.org/cognite/neat/data-model/verified/logical/neat_space/NeatInferredDataModel/v1/BasePower</t>
-  </si>
-  <si>
-    <t>http://purl.org/cognite/neat/data-model/verified/logical/neat_space/NeatInferredDataModel/v1/BaseVoltage</t>
-  </si>
-  <si>
-    <t>http://purl.org/cognite/neat/data-model/verified/logical/neat_space/NeatInferredDataModel/v1/Bay</t>
-  </si>
-  <si>
-    <t>http://purl.org/cognite/neat/data-model/verified/logical/neat_space/NeatInferredDataModel/v1/Breaker</t>
-  </si>
-  <si>
-    <t>http://purl.org/cognite/neat/data-model/verified/logical/neat_space/NeatInferredDataModel/v1/BusbarSection</t>
-  </si>
-  <si>
-    <t>http://purl.org/cognite/neat/data-model/verified/logical/neat_space/NeatInferredDataModel/v1/ConformLoad</t>
-  </si>
-  <si>
-    <t>http://purl.org/cognite/neat/data-model/verified/logical/neat_space/NeatInferredDataModel/v1/ConformLoadGroup</t>
-  </si>
-  <si>
-    <t>http://purl.org/cognite/neat/data-model/verified/logical/neat_space/NeatInferredDataModel/v1/ConnectivityNode</t>
-  </si>
-  <si>
-    <t>http://purl.org/cognite/neat/data-model/verified/logical/neat_space/NeatInferredDataModel/v1/ControlArea</t>
-  </si>
-  <si>
-    <t>http://purl.org/cognite/neat/data-model/verified/logical/neat_space/NeatInferredDataModel/v1/ControlAreaGeneratingUnit</t>
-  </si>
-  <si>
-    <t>http://purl.org/cognite/neat/data-model/verified/logical/neat_space/NeatInferredDataModel/v1/CurrentLimit</t>
-  </si>
-  <si>
-    <t>http://purl.org/cognite/neat/data-model/verified/logical/neat_space/NeatInferredDataModel/v1/Disconnector</t>
-  </si>
-  <si>
-    <t>http://purl.org/cognite/neat/data-model/verified/logical/neat_space/NeatInferredDataModel/v1/GeneratingUnit</t>
-  </si>
-  <si>
-    <t>http://purl.org/cognite/neat/data-model/verified/logical/neat_space/NeatInferredDataModel/v1/GeographicalRegion</t>
-  </si>
-  <si>
-    <t>http://purl.org/cognite/neat/data-model/verified/logical/neat_space/NeatInferredDataModel/v1/Line</t>
-  </si>
-  <si>
-    <t>http://purl.org/cognite/neat/data-model/verified/logical/neat_space/NeatInferredDataModel/v1/LinearShuntCompensator</t>
-  </si>
-  <si>
-    <t>http://purl.org/cognite/neat/data-model/verified/logical/neat_space/NeatInferredDataModel/v1/LoadArea</t>
-  </si>
-  <si>
-    <t>http://purl.org/cognite/neat/data-model/verified/logical/neat_space/NeatInferredDataModel/v1/LoadResponseCharacteristic</t>
-  </si>
-  <si>
-    <t>http://purl.org/cognite/neat/data-model/verified/logical/neat_space/NeatInferredDataModel/v1/MeasurementValueSource</t>
-  </si>
-  <si>
-    <t>http://purl.org/cognite/neat/data-model/verified/logical/neat_space/NeatInferredDataModel/v1/NonConformLoad</t>
-  </si>
-  <si>
-    <t>http://purl.org/cognite/neat/data-model/verified/logical/neat_space/NeatInferredDataModel/v1/NonConformLoadGroup</t>
-  </si>
-  <si>
-    <t>http://purl.org/cognite/neat/data-model/verified/logical/neat_space/NeatInferredDataModel/v1/OperatingParticipant</t>
-  </si>
-  <si>
-    <t>http://purl.org/cognite/neat/data-model/verified/logical/neat_space/NeatInferredDataModel/v1/OperatingShare</t>
-  </si>
-  <si>
-    <t>http://purl.org/cognite/neat/data-model/verified/logical/neat_space/NeatInferredDataModel/v1/OperationalLimitSet</t>
-  </si>
-  <si>
-    <t>http://purl.org/cognite/neat/data-model/verified/logical/neat_space/NeatInferredDataModel/v1/OperationalLimitType</t>
-  </si>
-  <si>
-    <t>http://purl.org/cognite/neat/data-model/verified/logical/neat_space/NeatInferredDataModel/v1/PowerTransformer</t>
-  </si>
-  <si>
-    <t>http://purl.org/cognite/neat/data-model/verified/logical/neat_space/NeatInferredDataModel/v1/PowerTransformerEnd</t>
-  </si>
-  <si>
-    <t>http://purl.org/cognite/neat/data-model/verified/logical/neat_space/NeatInferredDataModel/v1/RatioTapChanger</t>
-  </si>
-  <si>
-    <t>http://purl.org/cognite/neat/data-model/verified/logical/neat_space/NeatInferredDataModel/v1/RegulatingControl</t>
-  </si>
-  <si>
-    <t>http://purl.org/cognite/neat/data-model/verified/logical/neat_space/NeatInferredDataModel/v1/SubGeographicalRegion</t>
-  </si>
-  <si>
-    <t>http://purl.org/cognite/neat/data-model/verified/logical/neat_space/NeatInferredDataModel/v1/SubLoadArea</t>
-  </si>
-  <si>
-    <t>http://purl.org/cognite/neat/data-model/verified/logical/neat_space/NeatInferredDataModel/v1/Substation</t>
-  </si>
-  <si>
-    <t>http://purl.org/cognite/neat/data-model/verified/logical/neat_space/NeatInferredDataModel/v1/SynchronousMachine</t>
-  </si>
-  <si>
-    <t>http://purl.org/cognite/neat/data-model/verified/logical/neat_space/NeatInferredDataModel/v1/TapChangerControl</t>
-  </si>
-  <si>
-    <t>http://purl.org/cognite/neat/data-model/verified/logical/neat_space/NeatInferredDataModel/v1/Terminal</t>
-  </si>
-  <si>
-    <t>http://purl.org/cognite/neat/data-model/verified/logical/neat_space/NeatInferredDataModel/v1/VoltageLevel</t>
-  </si>
-  <si>
-    <t>http://purl.org/cognite/neat/data-model/verified/logical/neat_space/NeatInferredDataModel/v1/VoltageLimit</t>
-  </si>
-  <si>
-    <t>http://purl.org/cognite/neat/data-model/verified/logical/neat_space/NeatInferredDataModel/v1/Gate</t>
-  </si>
-  <si>
-    <t>http://purl.org/cognite/neat/data-model/verified/logical/neat_space/NeatInferredDataModel/v1/PinEquipment</t>
-  </si>
-  <si>
-    <t>http://purl.org/cognite/neat/data-model/verified/logical/neat_space/NeatInferredDataModel/v1/PinGate</t>
-  </si>
-  <si>
-    <t>http://purl.org/cognite/neat/data-model/verified/logical/neat_space/NeatInferredDataModel/v1/PinTerminal</t>
-  </si>
-  <si>
-    <t>http://purl.org/cognite/neat/data-model/verified/logical/neat_space/NeatInferredDataModel/v1/ProtectiveActionAdjustment</t>
-  </si>
-  <si>
-    <t>http://purl.org/cognite/neat/data-model/verified/logical/neat_space/NeatInferredDataModel/v1/ProtectiveActionCollection</t>
-  </si>
-  <si>
-    <t>http://purl.org/cognite/neat/data-model/verified/logical/neat_space/NeatInferredDataModel/v1/ProtectiveActionEquipment</t>
-  </si>
-  <si>
-    <t>http://purl.org/cognite/neat/data-model/verified/logical/neat_space/NeatInferredDataModel/v1/RemedialActionScheme</t>
-  </si>
-  <si>
-    <t>http://purl.org/cognite/neat/data-model/verified/logical/neat_space/NeatInferredDataModel/v1/Stage</t>
-  </si>
-  <si>
-    <t>http://purl.org/cognite/neat/data-model/verified/logical/neat_space/NeatInferredDataModel/v1/StageTrigger</t>
-  </si>
-  <si>
-    <t>http://purl.org/cognite/neat/data-model/verified/logical/neat_space/NeatInferredDataModel/v1/FullModel</t>
-  </si>
-  <si>
-    <t>http://purl.org/cognite/neat/data-model/verified/logical/neat_space/NeatInferredDataModel/v1/ScheduleResourceGeneration</t>
-  </si>
-  <si>
     <t>Prefix</t>
   </si>
   <si>
@@ -437,6 +260,183 @@
   </si>
   <si>
     <t>WindTurbine</t>
+  </si>
+  <si>
+    <t>http://purl.org/cognite/neat/data-model/verified/conceptual/neat_space/NeatInferredDataModel/v1/CircuitShare</t>
+  </si>
+  <si>
+    <t>http://purl.org/cognite/neat/data-model/verified/conceptual/neat_space/NeatInferredDataModel/v1/EnergyCongestionZone</t>
+  </si>
+  <si>
+    <t>http://purl.org/cognite/neat/data-model/verified/conceptual/neat_space/NeatInferredDataModel/v1/EnergySchedulingArea</t>
+  </si>
+  <si>
+    <t>http://purl.org/cognite/neat/data-model/verified/conceptual/neat_space/NeatInferredDataModel/v1/LineCircuit</t>
+  </si>
+  <si>
+    <t>http://purl.org/cognite/neat/data-model/verified/conceptual/neat_space/NeatInferredDataModel/v1/PowerTransferCorridor</t>
+  </si>
+  <si>
+    <t>http://purl.org/cognite/neat/data-model/verified/conceptual/neat_space/NeatInferredDataModel/v1/RateTemperature</t>
+  </si>
+  <si>
+    <t>http://purl.org/cognite/neat/data-model/verified/conceptual/neat_space/NeatInferredDataModel/v1/ACLineSegment</t>
+  </si>
+  <si>
+    <t>http://purl.org/cognite/neat/data-model/verified/conceptual/neat_space/NeatInferredDataModel/v1/ActivePowerLimit</t>
+  </si>
+  <si>
+    <t>http://purl.org/cognite/neat/data-model/verified/conceptual/neat_space/NeatInferredDataModel/v1/Analog</t>
+  </si>
+  <si>
+    <t>http://purl.org/cognite/neat/data-model/verified/conceptual/neat_space/NeatInferredDataModel/v1/AnalogValue</t>
+  </si>
+  <si>
+    <t>http://purl.org/cognite/neat/data-model/verified/conceptual/neat_space/NeatInferredDataModel/v1/BasePower</t>
+  </si>
+  <si>
+    <t>http://purl.org/cognite/neat/data-model/verified/conceptual/neat_space/NeatInferredDataModel/v1/BaseVoltage</t>
+  </si>
+  <si>
+    <t>http://purl.org/cognite/neat/data-model/verified/conceptual/neat_space/NeatInferredDataModel/v1/Bay</t>
+  </si>
+  <si>
+    <t>http://purl.org/cognite/neat/data-model/verified/conceptual/neat_space/NeatInferredDataModel/v1/Breaker</t>
+  </si>
+  <si>
+    <t>http://purl.org/cognite/neat/data-model/verified/conceptual/neat_space/NeatInferredDataModel/v1/BusbarSection</t>
+  </si>
+  <si>
+    <t>http://purl.org/cognite/neat/data-model/verified/conceptual/neat_space/NeatInferredDataModel/v1/ConformLoad</t>
+  </si>
+  <si>
+    <t>http://purl.org/cognite/neat/data-model/verified/conceptual/neat_space/NeatInferredDataModel/v1/ConformLoadGroup</t>
+  </si>
+  <si>
+    <t>http://purl.org/cognite/neat/data-model/verified/conceptual/neat_space/NeatInferredDataModel/v1/ConnectivityNode</t>
+  </si>
+  <si>
+    <t>http://purl.org/cognite/neat/data-model/verified/conceptual/neat_space/NeatInferredDataModel/v1/ControlArea</t>
+  </si>
+  <si>
+    <t>http://purl.org/cognite/neat/data-model/verified/conceptual/neat_space/NeatInferredDataModel/v1/ControlAreaGeneratingUnit</t>
+  </si>
+  <si>
+    <t>http://purl.org/cognite/neat/data-model/verified/conceptual/neat_space/NeatInferredDataModel/v1/CurrentLimit</t>
+  </si>
+  <si>
+    <t>http://purl.org/cognite/neat/data-model/verified/conceptual/neat_space/NeatInferredDataModel/v1/Disconnector</t>
+  </si>
+  <si>
+    <t>http://purl.org/cognite/neat/data-model/verified/conceptual/neat_space/NeatInferredDataModel/v1/GeneratingUnit</t>
+  </si>
+  <si>
+    <t>http://purl.org/cognite/neat/data-model/verified/conceptual/neat_space/NeatInferredDataModel/v1/GeographicalRegion</t>
+  </si>
+  <si>
+    <t>http://purl.org/cognite/neat/data-model/verified/conceptual/neat_space/NeatInferredDataModel/v1/Line</t>
+  </si>
+  <si>
+    <t>http://purl.org/cognite/neat/data-model/verified/conceptual/neat_space/NeatInferredDataModel/v1/LinearShuntCompensator</t>
+  </si>
+  <si>
+    <t>http://purl.org/cognite/neat/data-model/verified/conceptual/neat_space/NeatInferredDataModel/v1/LoadArea</t>
+  </si>
+  <si>
+    <t>http://purl.org/cognite/neat/data-model/verified/conceptual/neat_space/NeatInferredDataModel/v1/LoadResponseCharacteristic</t>
+  </si>
+  <si>
+    <t>http://purl.org/cognite/neat/data-model/verified/conceptual/neat_space/NeatInferredDataModel/v1/MeasurementValueSource</t>
+  </si>
+  <si>
+    <t>http://purl.org/cognite/neat/data-model/verified/conceptual/neat_space/NeatInferredDataModel/v1/NonConformLoad</t>
+  </si>
+  <si>
+    <t>http://purl.org/cognite/neat/data-model/verified/conceptual/neat_space/NeatInferredDataModel/v1/NonConformLoadGroup</t>
+  </si>
+  <si>
+    <t>http://purl.org/cognite/neat/data-model/verified/conceptual/neat_space/NeatInferredDataModel/v1/OperatingParticipant</t>
+  </si>
+  <si>
+    <t>http://purl.org/cognite/neat/data-model/verified/conceptual/neat_space/NeatInferredDataModel/v1/OperatingShare</t>
+  </si>
+  <si>
+    <t>http://purl.org/cognite/neat/data-model/verified/conceptual/neat_space/NeatInferredDataModel/v1/OperationalLimitSet</t>
+  </si>
+  <si>
+    <t>http://purl.org/cognite/neat/data-model/verified/conceptual/neat_space/NeatInferredDataModel/v1/OperationalLimitType</t>
+  </si>
+  <si>
+    <t>http://purl.org/cognite/neat/data-model/verified/conceptual/neat_space/NeatInferredDataModel/v1/PowerTransformer</t>
+  </si>
+  <si>
+    <t>http://purl.org/cognite/neat/data-model/verified/conceptual/neat_space/NeatInferredDataModel/v1/PowerTransformerEnd</t>
+  </si>
+  <si>
+    <t>http://purl.org/cognite/neat/data-model/verified/conceptual/neat_space/NeatInferredDataModel/v1/RatioTapChanger</t>
+  </si>
+  <si>
+    <t>http://purl.org/cognite/neat/data-model/verified/conceptual/neat_space/NeatInferredDataModel/v1/RegulatingControl</t>
+  </si>
+  <si>
+    <t>http://purl.org/cognite/neat/data-model/verified/conceptual/neat_space/NeatInferredDataModel/v1/SubGeographicalRegion</t>
+  </si>
+  <si>
+    <t>http://purl.org/cognite/neat/data-model/verified/conceptual/neat_space/NeatInferredDataModel/v1/SubLoadArea</t>
+  </si>
+  <si>
+    <t>http://purl.org/cognite/neat/data-model/verified/conceptual/neat_space/NeatInferredDataModel/v1/Substation</t>
+  </si>
+  <si>
+    <t>http://purl.org/cognite/neat/data-model/verified/conceptual/neat_space/NeatInferredDataModel/v1/SynchronousMachine</t>
+  </si>
+  <si>
+    <t>http://purl.org/cognite/neat/data-model/verified/conceptual/neat_space/NeatInferredDataModel/v1/TapChangerControl</t>
+  </si>
+  <si>
+    <t>http://purl.org/cognite/neat/data-model/verified/conceptual/neat_space/NeatInferredDataModel/v1/Terminal</t>
+  </si>
+  <si>
+    <t>http://purl.org/cognite/neat/data-model/verified/conceptual/neat_space/NeatInferredDataModel/v1/VoltageLevel</t>
+  </si>
+  <si>
+    <t>http://purl.org/cognite/neat/data-model/verified/conceptual/neat_space/NeatInferredDataModel/v1/VoltageLimit</t>
+  </si>
+  <si>
+    <t>http://purl.org/cognite/neat/data-model/verified/conceptual/neat_space/NeatInferredDataModel/v1/Gate</t>
+  </si>
+  <si>
+    <t>http://purl.org/cognite/neat/data-model/verified/conceptual/neat_space/NeatInferredDataModel/v1/PinEquipment</t>
+  </si>
+  <si>
+    <t>http://purl.org/cognite/neat/data-model/verified/conceptual/neat_space/NeatInferredDataModel/v1/PinGate</t>
+  </si>
+  <si>
+    <t>http://purl.org/cognite/neat/data-model/verified/conceptual/neat_space/NeatInferredDataModel/v1/PinTerminal</t>
+  </si>
+  <si>
+    <t>http://purl.org/cognite/neat/data-model/verified/conceptual/neat_space/NeatInferredDataModel/v1/ProtectiveActionAdjustment</t>
+  </si>
+  <si>
+    <t>http://purl.org/cognite/neat/data-model/verified/conceptual/neat_space/NeatInferredDataModel/v1/ProtectiveActionCollection</t>
+  </si>
+  <si>
+    <t>http://purl.org/cognite/neat/data-model/verified/conceptual/neat_space/NeatInferredDataModel/v1/ProtectiveActionEquipment</t>
+  </si>
+  <si>
+    <t>http://purl.org/cognite/neat/data-model/verified/conceptual/neat_space/NeatInferredDataModel/v1/RemedialActionScheme</t>
+  </si>
+  <si>
+    <t>http://purl.org/cognite/neat/data-model/verified/conceptual/neat_space/NeatInferredDataModel/v1/Stage</t>
+  </si>
+  <si>
+    <t>http://purl.org/cognite/neat/data-model/verified/conceptual/neat_space/NeatInferredDataModel/v1/StageTrigger</t>
+  </si>
+  <si>
+    <t>http://purl.org/cognite/neat/data-model/verified/conceptual/neat_space/NeatInferredDataModel/v1/FullModel</t>
+  </si>
+  <si>
+    <t>http://purl.org/cognite/neat/data-model/verified/conceptual/neat_space/NeatInferredDataModel/v1/ScheduleResourceGeneration</t>
   </si>
 </sst>
 </file>
@@ -446,7 +446,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd\ h:mm:ss"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -458,16 +458,25 @@
       <b/>
       <sz val="12"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="20"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="14"/>
       <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF839496"/>
+      <name val="Menlo"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="5">
@@ -520,7 +529,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -531,6 +540,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -839,13 +849,13 @@
       <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="13" customWidth="1"/>
     <col min="2" max="2" width="70" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -853,23 +863,23 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
@@ -877,31 +887,31 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B5" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B6" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B7" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>9</v>
       </c>
@@ -909,7 +919,7 @@
         <v>45728.612507300008</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>10</v>
       </c>
@@ -917,17 +927,17 @@
         <v>45728.612507300008</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="12" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>13</v>
       </c>
@@ -941,15 +951,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:L334"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="26.44140625" customWidth="1"/>
-    <col min="2" max="2" width="45.44140625" customWidth="1"/>
+    <col min="1" max="1" width="26.5" customWidth="1"/>
+    <col min="2" max="2" width="45.5" customWidth="1"/>
     <col min="3" max="4" width="13" customWidth="1"/>
     <col min="5" max="5" width="70" customWidth="1"/>
     <col min="6" max="8" width="13" customWidth="1"/>
@@ -958,7 +968,7 @@
     <col min="12" max="12" width="70" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="25.8" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:12" ht="26" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>14</v>
       </c>
@@ -974,7 +984,7 @@
       <c r="K1" s="4"/>
       <c r="L1" s="4"/>
     </row>
-    <row r="2" spans="1:12" ht="18" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:12" ht="19" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>15</v>
       </c>
@@ -1012,7 +1022,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3" s="6"/>
       <c r="B3" s="6"/>
       <c r="C3" s="6"/>
@@ -1026,7 +1036,7 @@
       <c r="K3" s="6"/>
       <c r="L3" s="6"/>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4" s="6"/>
       <c r="B4" s="6"/>
       <c r="C4" s="6"/>
@@ -1040,7 +1050,7 @@
       <c r="K4" s="6"/>
       <c r="L4" s="6"/>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5" s="6"/>
       <c r="B5" s="6"/>
       <c r="C5" s="6"/>
@@ -1054,7 +1064,7 @@
       <c r="K5" s="6"/>
       <c r="L5" s="6"/>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A6" s="6"/>
       <c r="B6" s="6"/>
       <c r="C6" s="6"/>
@@ -1068,7 +1078,7 @@
       <c r="K6" s="6"/>
       <c r="L6" s="6"/>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A7" s="7"/>
       <c r="B7" s="7"/>
       <c r="C7" s="7"/>
@@ -1082,7 +1092,7 @@
       <c r="K7" s="7"/>
       <c r="L7" s="7"/>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A8" s="7"/>
       <c r="B8" s="7"/>
       <c r="C8" s="7"/>
@@ -1096,7 +1106,7 @@
       <c r="K8" s="7"/>
       <c r="L8" s="7"/>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A9" s="7"/>
       <c r="B9" s="7"/>
       <c r="C9" s="7"/>
@@ -1110,7 +1120,7 @@
       <c r="K9" s="7"/>
       <c r="L9" s="7"/>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A10" s="7"/>
       <c r="B10" s="7"/>
       <c r="C10" s="7"/>
@@ -1124,7 +1134,7 @@
       <c r="K10" s="7"/>
       <c r="L10" s="7"/>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A11" s="6"/>
       <c r="B11" s="6"/>
       <c r="C11" s="6"/>
@@ -1138,7 +1148,7 @@
       <c r="K11" s="6"/>
       <c r="L11" s="6"/>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
@@ -1152,7 +1162,7 @@
       <c r="K12" s="6"/>
       <c r="L12" s="6"/>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A13" s="6"/>
       <c r="B13" s="6"/>
       <c r="C13" s="6"/>
@@ -1166,7 +1176,7 @@
       <c r="K13" s="6"/>
       <c r="L13" s="6"/>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A14" s="6"/>
       <c r="B14" s="6"/>
       <c r="C14" s="6"/>
@@ -1180,7 +1190,7 @@
       <c r="K14" s="6"/>
       <c r="L14" s="6"/>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A15" s="6"/>
       <c r="B15" s="6"/>
       <c r="C15" s="6"/>
@@ -1194,7 +1204,7 @@
       <c r="K15" s="6"/>
       <c r="L15" s="6"/>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A16" s="7"/>
       <c r="B16" s="7"/>
       <c r="C16" s="7"/>
@@ -1208,7 +1218,7 @@
       <c r="K16" s="7"/>
       <c r="L16" s="7"/>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A17" s="7"/>
       <c r="B17" s="7"/>
       <c r="C17" s="7"/>
@@ -1222,7 +1232,7 @@
       <c r="K17" s="7"/>
       <c r="L17" s="7"/>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A18" s="7"/>
       <c r="B18" s="7"/>
       <c r="C18" s="7"/>
@@ -1236,7 +1246,7 @@
       <c r="K18" s="7"/>
       <c r="L18" s="7"/>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A19" s="7"/>
       <c r="B19" s="7"/>
       <c r="C19" s="7"/>
@@ -1250,7 +1260,7 @@
       <c r="K19" s="7"/>
       <c r="L19" s="7"/>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A20" s="6"/>
       <c r="B20" s="6"/>
       <c r="C20" s="6"/>
@@ -1264,7 +1274,7 @@
       <c r="K20" s="6"/>
       <c r="L20" s="6"/>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A21" s="6"/>
       <c r="B21" s="6"/>
       <c r="C21" s="6"/>
@@ -1278,7 +1288,7 @@
       <c r="K21" s="6"/>
       <c r="L21" s="6"/>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A22" s="7"/>
       <c r="B22" s="7"/>
       <c r="C22" s="7"/>
@@ -1292,7 +1302,7 @@
       <c r="K22" s="7"/>
       <c r="L22" s="7"/>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A23" s="7"/>
       <c r="B23" s="7"/>
       <c r="C23" s="7"/>
@@ -1306,7 +1316,7 @@
       <c r="K23" s="7"/>
       <c r="L23" s="7"/>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A24" s="7"/>
       <c r="B24" s="7"/>
       <c r="C24" s="7"/>
@@ -1320,7 +1330,7 @@
       <c r="K24" s="7"/>
       <c r="L24" s="7"/>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A25" s="6"/>
       <c r="B25" s="6"/>
       <c r="C25" s="6"/>
@@ -1334,7 +1344,7 @@
       <c r="K25" s="6"/>
       <c r="L25" s="6"/>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A26" s="6"/>
       <c r="B26" s="6"/>
       <c r="C26" s="6"/>
@@ -1348,7 +1358,7 @@
       <c r="K26" s="6"/>
       <c r="L26" s="6"/>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A27" s="6"/>
       <c r="B27" s="6"/>
       <c r="C27" s="6"/>
@@ -1362,7 +1372,7 @@
       <c r="K27" s="6"/>
       <c r="L27" s="6"/>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A28" s="6"/>
       <c r="B28" s="6"/>
       <c r="C28" s="6"/>
@@ -1376,7 +1386,7 @@
       <c r="K28" s="6"/>
       <c r="L28" s="6"/>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A29" s="6"/>
       <c r="B29" s="6"/>
       <c r="C29" s="6"/>
@@ -1390,7 +1400,7 @@
       <c r="K29" s="6"/>
       <c r="L29" s="6"/>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A30" s="6"/>
       <c r="B30" s="6"/>
       <c r="C30" s="6"/>
@@ -1404,7 +1414,7 @@
       <c r="K30" s="6"/>
       <c r="L30" s="6"/>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A31" s="6"/>
       <c r="B31" s="6"/>
       <c r="C31" s="6"/>
@@ -1418,7 +1428,7 @@
       <c r="K31" s="6"/>
       <c r="L31" s="6"/>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A32" s="6"/>
       <c r="B32" s="6"/>
       <c r="C32" s="6"/>
@@ -1432,7 +1442,7 @@
       <c r="K32" s="6"/>
       <c r="L32" s="6"/>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A33" s="6"/>
       <c r="B33" s="6"/>
       <c r="C33" s="6"/>
@@ -1446,7 +1456,7 @@
       <c r="K33" s="6"/>
       <c r="L33" s="6"/>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A34" s="6"/>
       <c r="B34" s="6"/>
       <c r="C34" s="6"/>
@@ -1460,7 +1470,7 @@
       <c r="K34" s="6"/>
       <c r="L34" s="6"/>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A35" s="6"/>
       <c r="B35" s="6"/>
       <c r="C35" s="6"/>
@@ -1474,7 +1484,7 @@
       <c r="K35" s="6"/>
       <c r="L35" s="6"/>
     </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A36" s="6"/>
       <c r="B36" s="6"/>
       <c r="C36" s="6"/>
@@ -1488,7 +1498,7 @@
       <c r="K36" s="6"/>
       <c r="L36" s="6"/>
     </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A37" s="7"/>
       <c r="B37" s="7"/>
       <c r="C37" s="7"/>
@@ -1502,7 +1512,7 @@
       <c r="K37" s="7"/>
       <c r="L37" s="7"/>
     </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A38" s="7"/>
       <c r="B38" s="7"/>
       <c r="C38" s="7"/>
@@ -1516,7 +1526,7 @@
       <c r="K38" s="7"/>
       <c r="L38" s="7"/>
     </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A39" s="7"/>
       <c r="B39" s="7"/>
       <c r="C39" s="7"/>
@@ -1530,7 +1540,7 @@
       <c r="K39" s="7"/>
       <c r="L39" s="7"/>
     </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A40" s="7"/>
       <c r="B40" s="7"/>
       <c r="C40" s="7"/>
@@ -1544,7 +1554,7 @@
       <c r="K40" s="7"/>
       <c r="L40" s="7"/>
     </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A41" s="7"/>
       <c r="B41" s="7"/>
       <c r="C41" s="7"/>
@@ -1558,7 +1568,7 @@
       <c r="K41" s="7"/>
       <c r="L41" s="7"/>
     </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A42" s="6"/>
       <c r="B42" s="6"/>
       <c r="C42" s="6"/>
@@ -1572,7 +1582,7 @@
       <c r="K42" s="6"/>
       <c r="L42" s="6"/>
     </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A43" s="6"/>
       <c r="B43" s="6"/>
       <c r="C43" s="6"/>
@@ -1586,7 +1596,7 @@
       <c r="K43" s="6"/>
       <c r="L43" s="6"/>
     </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A44" s="6"/>
       <c r="B44" s="6"/>
       <c r="C44" s="6"/>
@@ -1600,7 +1610,7 @@
       <c r="K44" s="6"/>
       <c r="L44" s="6"/>
     </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A45" s="6"/>
       <c r="B45" s="6"/>
       <c r="C45" s="6"/>
@@ -1614,7 +1624,7 @@
       <c r="K45" s="6"/>
       <c r="L45" s="6"/>
     </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A46" s="6"/>
       <c r="B46" s="6"/>
       <c r="C46" s="6"/>
@@ -1628,7 +1638,7 @@
       <c r="K46" s="6"/>
       <c r="L46" s="6"/>
     </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A47" s="6"/>
       <c r="B47" s="6"/>
       <c r="C47" s="6"/>
@@ -1642,7 +1652,7 @@
       <c r="K47" s="6"/>
       <c r="L47" s="6"/>
     </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A48" s="6"/>
       <c r="B48" s="6"/>
       <c r="C48" s="6"/>
@@ -1656,7 +1666,7 @@
       <c r="K48" s="6"/>
       <c r="L48" s="6"/>
     </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A49" s="7"/>
       <c r="B49" s="7"/>
       <c r="C49" s="7"/>
@@ -1670,7 +1680,7 @@
       <c r="K49" s="7"/>
       <c r="L49" s="7"/>
     </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A50" s="7"/>
       <c r="B50" s="7"/>
       <c r="C50" s="7"/>
@@ -1684,7 +1694,7 @@
       <c r="K50" s="7"/>
       <c r="L50" s="7"/>
     </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A51" s="7"/>
       <c r="B51" s="7"/>
       <c r="C51" s="7"/>
@@ -1698,7 +1708,7 @@
       <c r="K51" s="7"/>
       <c r="L51" s="7"/>
     </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A52" s="7"/>
       <c r="B52" s="7"/>
       <c r="C52" s="7"/>
@@ -1712,7 +1722,7 @@
       <c r="K52" s="7"/>
       <c r="L52" s="7"/>
     </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A53" s="7"/>
       <c r="B53" s="7"/>
       <c r="C53" s="7"/>
@@ -1726,7 +1736,7 @@
       <c r="K53" s="7"/>
       <c r="L53" s="7"/>
     </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A54" s="6"/>
       <c r="B54" s="6"/>
       <c r="C54" s="6"/>
@@ -1740,7 +1750,7 @@
       <c r="K54" s="6"/>
       <c r="L54" s="6"/>
     </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A55" s="7"/>
       <c r="B55" s="7"/>
       <c r="C55" s="7"/>
@@ -1754,7 +1764,7 @@
       <c r="K55" s="7"/>
       <c r="L55" s="7"/>
     </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A56" s="7"/>
       <c r="B56" s="7"/>
       <c r="C56" s="7"/>
@@ -1768,7 +1778,7 @@
       <c r="K56" s="7"/>
       <c r="L56" s="7"/>
     </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A57" s="6"/>
       <c r="B57" s="6"/>
       <c r="C57" s="6"/>
@@ -1782,7 +1792,7 @@
       <c r="K57" s="6"/>
       <c r="L57" s="6"/>
     </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A58" s="6"/>
       <c r="B58" s="6"/>
       <c r="C58" s="6"/>
@@ -1796,7 +1806,7 @@
       <c r="K58" s="6"/>
       <c r="L58" s="6"/>
     </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A59" s="6"/>
       <c r="B59" s="6"/>
       <c r="C59" s="6"/>
@@ -1810,7 +1820,7 @@
       <c r="K59" s="6"/>
       <c r="L59" s="6"/>
     </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A60" s="7"/>
       <c r="B60" s="7"/>
       <c r="C60" s="7"/>
@@ -1824,7 +1834,7 @@
       <c r="K60" s="7"/>
       <c r="L60" s="7"/>
     </row>
-    <row r="61" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A61" s="7"/>
       <c r="B61" s="7"/>
       <c r="C61" s="7"/>
@@ -1838,7 +1848,7 @@
       <c r="K61" s="7"/>
       <c r="L61" s="7"/>
     </row>
-    <row r="62" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A62" s="7"/>
       <c r="B62" s="7"/>
       <c r="C62" s="7"/>
@@ -1852,7 +1862,7 @@
       <c r="K62" s="7"/>
       <c r="L62" s="7"/>
     </row>
-    <row r="63" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A63" s="7"/>
       <c r="B63" s="7"/>
       <c r="C63" s="7"/>
@@ -1866,7 +1876,7 @@
       <c r="K63" s="7"/>
       <c r="L63" s="7"/>
     </row>
-    <row r="64" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A64" s="7"/>
       <c r="B64" s="7"/>
       <c r="C64" s="7"/>
@@ -1880,7 +1890,7 @@
       <c r="K64" s="7"/>
       <c r="L64" s="7"/>
     </row>
-    <row r="65" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A65" s="7"/>
       <c r="B65" s="7"/>
       <c r="C65" s="7"/>
@@ -1894,7 +1904,7 @@
       <c r="K65" s="7"/>
       <c r="L65" s="7"/>
     </row>
-    <row r="66" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A66" s="7"/>
       <c r="B66" s="7"/>
       <c r="C66" s="7"/>
@@ -1908,7 +1918,7 @@
       <c r="K66" s="7"/>
       <c r="L66" s="7"/>
     </row>
-    <row r="67" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A67" s="6"/>
       <c r="B67" s="6"/>
       <c r="C67" s="6"/>
@@ -1922,7 +1932,7 @@
       <c r="K67" s="6"/>
       <c r="L67" s="6"/>
     </row>
-    <row r="68" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A68" s="6"/>
       <c r="B68" s="6"/>
       <c r="C68" s="6"/>
@@ -1936,7 +1946,7 @@
       <c r="K68" s="6"/>
       <c r="L68" s="6"/>
     </row>
-    <row r="69" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A69" s="6"/>
       <c r="B69" s="6"/>
       <c r="C69" s="6"/>
@@ -1950,7 +1960,7 @@
       <c r="K69" s="6"/>
       <c r="L69" s="6"/>
     </row>
-    <row r="70" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A70" s="6"/>
       <c r="B70" s="6"/>
       <c r="C70" s="6"/>
@@ -1964,7 +1974,7 @@
       <c r="K70" s="6"/>
       <c r="L70" s="6"/>
     </row>
-    <row r="71" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A71" s="7"/>
       <c r="B71" s="7"/>
       <c r="C71" s="7"/>
@@ -1978,7 +1988,7 @@
       <c r="K71" s="7"/>
       <c r="L71" s="7"/>
     </row>
-    <row r="72" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A72" s="7"/>
       <c r="B72" s="7"/>
       <c r="C72" s="7"/>
@@ -1992,7 +2002,7 @@
       <c r="K72" s="7"/>
       <c r="L72" s="7"/>
     </row>
-    <row r="73" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A73" s="7"/>
       <c r="B73" s="7"/>
       <c r="C73" s="7"/>
@@ -2006,7 +2016,7 @@
       <c r="K73" s="7"/>
       <c r="L73" s="7"/>
     </row>
-    <row r="74" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A74" s="7"/>
       <c r="B74" s="7"/>
       <c r="C74" s="7"/>
@@ -2020,7 +2030,7 @@
       <c r="K74" s="7"/>
       <c r="L74" s="7"/>
     </row>
-    <row r="75" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A75" s="7"/>
       <c r="B75" s="7"/>
       <c r="C75" s="7"/>
@@ -2034,7 +2044,7 @@
       <c r="K75" s="7"/>
       <c r="L75" s="7"/>
     </row>
-    <row r="76" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A76" s="7"/>
       <c r="B76" s="7"/>
       <c r="C76" s="7"/>
@@ -2048,7 +2058,7 @@
       <c r="K76" s="7"/>
       <c r="L76" s="7"/>
     </row>
-    <row r="77" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A77" s="7"/>
       <c r="B77" s="7"/>
       <c r="C77" s="7"/>
@@ -2062,7 +2072,7 @@
       <c r="K77" s="7"/>
       <c r="L77" s="7"/>
     </row>
-    <row r="78" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A78" s="7"/>
       <c r="B78" s="7"/>
       <c r="C78" s="7"/>
@@ -2076,7 +2086,7 @@
       <c r="K78" s="7"/>
       <c r="L78" s="7"/>
     </row>
-    <row r="79" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A79" s="7"/>
       <c r="B79" s="7"/>
       <c r="C79" s="7"/>
@@ -2090,7 +2100,7 @@
       <c r="K79" s="7"/>
       <c r="L79" s="7"/>
     </row>
-    <row r="80" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A80" s="7"/>
       <c r="B80" s="7"/>
       <c r="C80" s="7"/>
@@ -2104,7 +2114,7 @@
       <c r="K80" s="7"/>
       <c r="L80" s="7"/>
     </row>
-    <row r="81" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A81" s="7"/>
       <c r="B81" s="7"/>
       <c r="C81" s="7"/>
@@ -2118,7 +2128,7 @@
       <c r="K81" s="7"/>
       <c r="L81" s="7"/>
     </row>
-    <row r="82" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A82" s="6"/>
       <c r="B82" s="6"/>
       <c r="C82" s="6"/>
@@ -2132,7 +2142,7 @@
       <c r="K82" s="6"/>
       <c r="L82" s="6"/>
     </row>
-    <row r="83" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A83" s="6"/>
       <c r="B83" s="6"/>
       <c r="C83" s="6"/>
@@ -2146,7 +2156,7 @@
       <c r="K83" s="6"/>
       <c r="L83" s="6"/>
     </row>
-    <row r="84" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A84" s="6"/>
       <c r="B84" s="6"/>
       <c r="C84" s="6"/>
@@ -2160,7 +2170,7 @@
       <c r="K84" s="6"/>
       <c r="L84" s="6"/>
     </row>
-    <row r="85" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A85" s="7"/>
       <c r="B85" s="7"/>
       <c r="C85" s="7"/>
@@ -2174,7 +2184,7 @@
       <c r="K85" s="7"/>
       <c r="L85" s="7"/>
     </row>
-    <row r="86" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A86" s="7"/>
       <c r="B86" s="7"/>
       <c r="C86" s="7"/>
@@ -2188,7 +2198,7 @@
       <c r="K86" s="7"/>
       <c r="L86" s="7"/>
     </row>
-    <row r="87" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A87" s="6"/>
       <c r="B87" s="6"/>
       <c r="C87" s="6"/>
@@ -2202,7 +2212,7 @@
       <c r="K87" s="6"/>
       <c r="L87" s="6"/>
     </row>
-    <row r="88" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A88" s="6"/>
       <c r="B88" s="6"/>
       <c r="C88" s="6"/>
@@ -2216,7 +2226,7 @@
       <c r="K88" s="6"/>
       <c r="L88" s="6"/>
     </row>
-    <row r="89" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A89" s="6"/>
       <c r="B89" s="6"/>
       <c r="C89" s="6"/>
@@ -2230,7 +2240,7 @@
       <c r="K89" s="6"/>
       <c r="L89" s="6"/>
     </row>
-    <row r="90" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A90" s="7"/>
       <c r="B90" s="7"/>
       <c r="C90" s="7"/>
@@ -2244,7 +2254,7 @@
       <c r="K90" s="7"/>
       <c r="L90" s="7"/>
     </row>
-    <row r="91" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A91" s="7"/>
       <c r="B91" s="7"/>
       <c r="C91" s="7"/>
@@ -2258,7 +2268,7 @@
       <c r="K91" s="7"/>
       <c r="L91" s="7"/>
     </row>
-    <row r="92" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A92" s="7"/>
       <c r="B92" s="7"/>
       <c r="C92" s="7"/>
@@ -2272,7 +2282,7 @@
       <c r="K92" s="7"/>
       <c r="L92" s="7"/>
     </row>
-    <row r="93" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A93" s="7"/>
       <c r="B93" s="7"/>
       <c r="C93" s="7"/>
@@ -2286,7 +2296,7 @@
       <c r="K93" s="7"/>
       <c r="L93" s="7"/>
     </row>
-    <row r="94" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A94" s="7"/>
       <c r="B94" s="7"/>
       <c r="C94" s="7"/>
@@ -2300,7 +2310,7 @@
       <c r="K94" s="7"/>
       <c r="L94" s="7"/>
     </row>
-    <row r="95" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A95" s="6"/>
       <c r="B95" s="6"/>
       <c r="C95" s="6"/>
@@ -2314,7 +2324,7 @@
       <c r="K95" s="6"/>
       <c r="L95" s="6"/>
     </row>
-    <row r="96" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A96" s="6"/>
       <c r="B96" s="6"/>
       <c r="C96" s="6"/>
@@ -2328,7 +2338,7 @@
       <c r="K96" s="6"/>
       <c r="L96" s="6"/>
     </row>
-    <row r="97" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A97" s="6"/>
       <c r="B97" s="6"/>
       <c r="C97" s="6"/>
@@ -2342,7 +2352,7 @@
       <c r="K97" s="6"/>
       <c r="L97" s="6"/>
     </row>
-    <row r="98" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A98" s="6"/>
       <c r="B98" s="6"/>
       <c r="C98" s="6"/>
@@ -2356,7 +2366,7 @@
       <c r="K98" s="6"/>
       <c r="L98" s="6"/>
     </row>
-    <row r="99" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A99" s="6"/>
       <c r="B99" s="6"/>
       <c r="C99" s="6"/>
@@ -2370,7 +2380,7 @@
       <c r="K99" s="6"/>
       <c r="L99" s="6"/>
     </row>
-    <row r="100" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A100" s="6"/>
       <c r="B100" s="6"/>
       <c r="C100" s="6"/>
@@ -2384,7 +2394,7 @@
       <c r="K100" s="6"/>
       <c r="L100" s="6"/>
     </row>
-    <row r="101" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A101" s="7"/>
       <c r="B101" s="7"/>
       <c r="C101" s="7"/>
@@ -2398,7 +2408,7 @@
       <c r="K101" s="7"/>
       <c r="L101" s="7"/>
     </row>
-    <row r="102" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A102" s="7"/>
       <c r="B102" s="7"/>
       <c r="C102" s="7"/>
@@ -2412,7 +2422,7 @@
       <c r="K102" s="7"/>
       <c r="L102" s="7"/>
     </row>
-    <row r="103" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A103" s="7"/>
       <c r="B103" s="7"/>
       <c r="C103" s="7"/>
@@ -2426,7 +2436,7 @@
       <c r="K103" s="7"/>
       <c r="L103" s="7"/>
     </row>
-    <row r="104" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A104" s="7"/>
       <c r="B104" s="7"/>
       <c r="C104" s="7"/>
@@ -2440,7 +2450,7 @@
       <c r="K104" s="7"/>
       <c r="L104" s="7"/>
     </row>
-    <row r="105" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A105" s="7"/>
       <c r="B105" s="7"/>
       <c r="C105" s="7"/>
@@ -2454,7 +2464,7 @@
       <c r="K105" s="7"/>
       <c r="L105" s="7"/>
     </row>
-    <row r="106" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A106" s="7"/>
       <c r="B106" s="7"/>
       <c r="C106" s="7"/>
@@ -2468,7 +2478,7 @@
       <c r="K106" s="7"/>
       <c r="L106" s="7"/>
     </row>
-    <row r="107" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A107" s="7"/>
       <c r="B107" s="7"/>
       <c r="C107" s="7"/>
@@ -2482,7 +2492,7 @@
       <c r="K107" s="7"/>
       <c r="L107" s="7"/>
     </row>
-    <row r="108" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A108" s="6"/>
       <c r="B108" s="6"/>
       <c r="C108" s="6"/>
@@ -2496,7 +2506,7 @@
       <c r="K108" s="6"/>
       <c r="L108" s="6"/>
     </row>
-    <row r="109" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A109" s="6"/>
       <c r="B109" s="6"/>
       <c r="C109" s="6"/>
@@ -2510,7 +2520,7 @@
       <c r="K109" s="6"/>
       <c r="L109" s="6"/>
     </row>
-    <row r="110" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A110" s="6"/>
       <c r="B110" s="6"/>
       <c r="C110" s="6"/>
@@ -2524,7 +2534,7 @@
       <c r="K110" s="6"/>
       <c r="L110" s="6"/>
     </row>
-    <row r="111" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A111" s="6"/>
       <c r="B111" s="6"/>
       <c r="C111" s="6"/>
@@ -2538,7 +2548,7 @@
       <c r="K111" s="6"/>
       <c r="L111" s="6"/>
     </row>
-    <row r="112" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A112" s="6"/>
       <c r="B112" s="6"/>
       <c r="C112" s="6"/>
@@ -2552,7 +2562,7 @@
       <c r="K112" s="6"/>
       <c r="L112" s="6"/>
     </row>
-    <row r="113" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A113" s="6"/>
       <c r="B113" s="6"/>
       <c r="C113" s="6"/>
@@ -2566,7 +2576,7 @@
       <c r="K113" s="6"/>
       <c r="L113" s="6"/>
     </row>
-    <row r="114" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A114" s="6"/>
       <c r="B114" s="6"/>
       <c r="C114" s="6"/>
@@ -2580,7 +2590,7 @@
       <c r="K114" s="6"/>
       <c r="L114" s="6"/>
     </row>
-    <row r="115" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A115" s="6"/>
       <c r="B115" s="6"/>
       <c r="C115" s="6"/>
@@ -2594,7 +2604,7 @@
       <c r="K115" s="6"/>
       <c r="L115" s="6"/>
     </row>
-    <row r="116" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A116" s="6"/>
       <c r="B116" s="6"/>
       <c r="C116" s="6"/>
@@ -2608,7 +2618,7 @@
       <c r="K116" s="6"/>
       <c r="L116" s="6"/>
     </row>
-    <row r="117" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A117" s="6"/>
       <c r="B117" s="6"/>
       <c r="C117" s="6"/>
@@ -2622,7 +2632,7 @@
       <c r="K117" s="6"/>
       <c r="L117" s="6"/>
     </row>
-    <row r="118" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A118" s="6"/>
       <c r="B118" s="6"/>
       <c r="C118" s="6"/>
@@ -2636,7 +2646,7 @@
       <c r="K118" s="6"/>
       <c r="L118" s="6"/>
     </row>
-    <row r="119" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A119" s="6"/>
       <c r="B119" s="6"/>
       <c r="C119" s="6"/>
@@ -2650,7 +2660,7 @@
       <c r="K119" s="6"/>
       <c r="L119" s="6"/>
     </row>
-    <row r="120" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A120" s="6"/>
       <c r="B120" s="6"/>
       <c r="C120" s="6"/>
@@ -2664,7 +2674,7 @@
       <c r="K120" s="6"/>
       <c r="L120" s="6"/>
     </row>
-    <row r="121" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A121" s="6"/>
       <c r="B121" s="6"/>
       <c r="C121" s="6"/>
@@ -2678,7 +2688,7 @@
       <c r="K121" s="6"/>
       <c r="L121" s="6"/>
     </row>
-    <row r="122" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A122" s="6"/>
       <c r="B122" s="6"/>
       <c r="C122" s="6"/>
@@ -2692,7 +2702,7 @@
       <c r="K122" s="6"/>
       <c r="L122" s="6"/>
     </row>
-    <row r="123" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A123" s="6"/>
       <c r="B123" s="6"/>
       <c r="C123" s="6"/>
@@ -2706,7 +2716,7 @@
       <c r="K123" s="6"/>
       <c r="L123" s="6"/>
     </row>
-    <row r="124" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A124" s="6"/>
       <c r="B124" s="6"/>
       <c r="C124" s="6"/>
@@ -2720,7 +2730,7 @@
       <c r="K124" s="6"/>
       <c r="L124" s="6"/>
     </row>
-    <row r="125" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A125" s="6"/>
       <c r="B125" s="6"/>
       <c r="C125" s="6"/>
@@ -2734,7 +2744,7 @@
       <c r="K125" s="6"/>
       <c r="L125" s="6"/>
     </row>
-    <row r="126" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A126" s="6"/>
       <c r="B126" s="6"/>
       <c r="C126" s="6"/>
@@ -2748,7 +2758,7 @@
       <c r="K126" s="6"/>
       <c r="L126" s="6"/>
     </row>
-    <row r="127" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A127" s="6"/>
       <c r="B127" s="6"/>
       <c r="C127" s="6"/>
@@ -2762,7 +2772,7 @@
       <c r="K127" s="6"/>
       <c r="L127" s="6"/>
     </row>
-    <row r="128" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A128" s="6"/>
       <c r="B128" s="6"/>
       <c r="C128" s="6"/>
@@ -2776,7 +2786,7 @@
       <c r="K128" s="6"/>
       <c r="L128" s="6"/>
     </row>
-    <row r="129" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A129" s="6"/>
       <c r="B129" s="6"/>
       <c r="C129" s="6"/>
@@ -2790,7 +2800,7 @@
       <c r="K129" s="6"/>
       <c r="L129" s="6"/>
     </row>
-    <row r="130" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A130" s="7"/>
       <c r="B130" s="7"/>
       <c r="C130" s="7"/>
@@ -2804,7 +2814,7 @@
       <c r="K130" s="7"/>
       <c r="L130" s="7"/>
     </row>
-    <row r="131" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A131" s="7"/>
       <c r="B131" s="7"/>
       <c r="C131" s="7"/>
@@ -2818,7 +2828,7 @@
       <c r="K131" s="7"/>
       <c r="L131" s="7"/>
     </row>
-    <row r="132" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A132" s="6"/>
       <c r="B132" s="6"/>
       <c r="C132" s="6"/>
@@ -2832,7 +2842,7 @@
       <c r="K132" s="6"/>
       <c r="L132" s="6"/>
     </row>
-    <row r="133" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A133" s="6"/>
       <c r="B133" s="6"/>
       <c r="C133" s="6"/>
@@ -2846,7 +2856,7 @@
       <c r="K133" s="6"/>
       <c r="L133" s="6"/>
     </row>
-    <row r="134" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A134" s="7"/>
       <c r="B134" s="7"/>
       <c r="C134" s="7"/>
@@ -2860,7 +2870,7 @@
       <c r="K134" s="7"/>
       <c r="L134" s="7"/>
     </row>
-    <row r="135" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A135" s="7"/>
       <c r="B135" s="7"/>
       <c r="C135" s="7"/>
@@ -2874,7 +2884,7 @@
       <c r="K135" s="7"/>
       <c r="L135" s="7"/>
     </row>
-    <row r="136" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A136" s="7"/>
       <c r="B136" s="7"/>
       <c r="C136" s="7"/>
@@ -2888,7 +2898,7 @@
       <c r="K136" s="7"/>
       <c r="L136" s="7"/>
     </row>
-    <row r="137" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A137" s="7"/>
       <c r="B137" s="7"/>
       <c r="C137" s="7"/>
@@ -2902,7 +2912,7 @@
       <c r="K137" s="7"/>
       <c r="L137" s="7"/>
     </row>
-    <row r="138" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A138" s="7"/>
       <c r="B138" s="7"/>
       <c r="C138" s="7"/>
@@ -2916,7 +2926,7 @@
       <c r="K138" s="7"/>
       <c r="L138" s="7"/>
     </row>
-    <row r="139" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A139" s="7"/>
       <c r="B139" s="7"/>
       <c r="C139" s="7"/>
@@ -2930,7 +2940,7 @@
       <c r="K139" s="7"/>
       <c r="L139" s="7"/>
     </row>
-    <row r="140" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A140" s="7"/>
       <c r="B140" s="7"/>
       <c r="C140" s="7"/>
@@ -2944,7 +2954,7 @@
       <c r="K140" s="7"/>
       <c r="L140" s="7"/>
     </row>
-    <row r="141" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A141" s="7"/>
       <c r="B141" s="7"/>
       <c r="C141" s="7"/>
@@ -2958,7 +2968,7 @@
       <c r="K141" s="7"/>
       <c r="L141" s="7"/>
     </row>
-    <row r="142" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A142" s="7"/>
       <c r="B142" s="7"/>
       <c r="C142" s="7"/>
@@ -2972,7 +2982,7 @@
       <c r="K142" s="7"/>
       <c r="L142" s="7"/>
     </row>
-    <row r="143" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A143" s="7"/>
       <c r="B143" s="7"/>
       <c r="C143" s="7"/>
@@ -2986,7 +2996,7 @@
       <c r="K143" s="7"/>
       <c r="L143" s="7"/>
     </row>
-    <row r="144" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A144" s="7"/>
       <c r="B144" s="7"/>
       <c r="C144" s="7"/>
@@ -3000,7 +3010,7 @@
       <c r="K144" s="7"/>
       <c r="L144" s="7"/>
     </row>
-    <row r="145" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A145" s="7"/>
       <c r="B145" s="7"/>
       <c r="C145" s="7"/>
@@ -3014,7 +3024,7 @@
       <c r="K145" s="7"/>
       <c r="L145" s="7"/>
     </row>
-    <row r="146" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A146" s="7"/>
       <c r="B146" s="7"/>
       <c r="C146" s="7"/>
@@ -3028,7 +3038,7 @@
       <c r="K146" s="7"/>
       <c r="L146" s="7"/>
     </row>
-    <row r="147" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A147" s="7"/>
       <c r="B147" s="7"/>
       <c r="C147" s="7"/>
@@ -3042,7 +3052,7 @@
       <c r="K147" s="7"/>
       <c r="L147" s="7"/>
     </row>
-    <row r="148" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A148" s="6"/>
       <c r="B148" s="6"/>
       <c r="C148" s="6"/>
@@ -3056,7 +3066,7 @@
       <c r="K148" s="6"/>
       <c r="L148" s="6"/>
     </row>
-    <row r="149" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A149" s="7"/>
       <c r="B149" s="7"/>
       <c r="C149" s="7"/>
@@ -3070,7 +3080,7 @@
       <c r="K149" s="7"/>
       <c r="L149" s="7"/>
     </row>
-    <row r="150" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A150" s="7"/>
       <c r="B150" s="7"/>
       <c r="C150" s="7"/>
@@ -3084,7 +3094,7 @@
       <c r="K150" s="7"/>
       <c r="L150" s="7"/>
     </row>
-    <row r="151" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A151" s="7"/>
       <c r="B151" s="7"/>
       <c r="C151" s="7"/>
@@ -3098,7 +3108,7 @@
       <c r="K151" s="7"/>
       <c r="L151" s="7"/>
     </row>
-    <row r="152" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A152" s="7"/>
       <c r="B152" s="7"/>
       <c r="C152" s="7"/>
@@ -3112,7 +3122,7 @@
       <c r="K152" s="7"/>
       <c r="L152" s="7"/>
     </row>
-    <row r="153" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A153" s="7"/>
       <c r="B153" s="7"/>
       <c r="C153" s="7"/>
@@ -3126,7 +3136,7 @@
       <c r="K153" s="7"/>
       <c r="L153" s="7"/>
     </row>
-    <row r="154" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A154" s="7"/>
       <c r="B154" s="7"/>
       <c r="C154" s="7"/>
@@ -3140,7 +3150,7 @@
       <c r="K154" s="7"/>
       <c r="L154" s="7"/>
     </row>
-    <row r="155" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A155" s="7"/>
       <c r="B155" s="7"/>
       <c r="C155" s="7"/>
@@ -3154,7 +3164,7 @@
       <c r="K155" s="7"/>
       <c r="L155" s="7"/>
     </row>
-    <row r="156" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A156" s="7"/>
       <c r="B156" s="7"/>
       <c r="C156" s="7"/>
@@ -3168,7 +3178,7 @@
       <c r="K156" s="7"/>
       <c r="L156" s="7"/>
     </row>
-    <row r="157" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A157" s="7"/>
       <c r="B157" s="7"/>
       <c r="C157" s="7"/>
@@ -3182,7 +3192,7 @@
       <c r="K157" s="7"/>
       <c r="L157" s="7"/>
     </row>
-    <row r="158" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A158" s="6"/>
       <c r="B158" s="6"/>
       <c r="C158" s="6"/>
@@ -3196,7 +3206,7 @@
       <c r="K158" s="6"/>
       <c r="L158" s="6"/>
     </row>
-    <row r="159" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A159" s="6"/>
       <c r="B159" s="6"/>
       <c r="C159" s="6"/>
@@ -3210,7 +3220,7 @@
       <c r="K159" s="6"/>
       <c r="L159" s="6"/>
     </row>
-    <row r="160" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A160" s="7"/>
       <c r="B160" s="7"/>
       <c r="C160" s="7"/>
@@ -3224,7 +3234,7 @@
       <c r="K160" s="7"/>
       <c r="L160" s="7"/>
     </row>
-    <row r="161" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A161" s="7"/>
       <c r="B161" s="7"/>
       <c r="C161" s="7"/>
@@ -3238,7 +3248,7 @@
       <c r="K161" s="7"/>
       <c r="L161" s="7"/>
     </row>
-    <row r="162" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A162" s="7"/>
       <c r="B162" s="7"/>
       <c r="C162" s="7"/>
@@ -3252,7 +3262,7 @@
       <c r="K162" s="7"/>
       <c r="L162" s="7"/>
     </row>
-    <row r="163" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A163" s="7"/>
       <c r="B163" s="7"/>
       <c r="C163" s="7"/>
@@ -3266,7 +3276,7 @@
       <c r="K163" s="7"/>
       <c r="L163" s="7"/>
     </row>
-    <row r="164" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A164" s="7"/>
       <c r="B164" s="7"/>
       <c r="C164" s="7"/>
@@ -3280,7 +3290,7 @@
       <c r="K164" s="7"/>
       <c r="L164" s="7"/>
     </row>
-    <row r="165" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A165" s="7"/>
       <c r="B165" s="7"/>
       <c r="C165" s="7"/>
@@ -3294,7 +3304,7 @@
       <c r="K165" s="7"/>
       <c r="L165" s="7"/>
     </row>
-    <row r="166" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A166" s="7"/>
       <c r="B166" s="7"/>
       <c r="C166" s="7"/>
@@ -3308,7 +3318,7 @@
       <c r="K166" s="7"/>
       <c r="L166" s="7"/>
     </row>
-    <row r="167" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A167" s="7"/>
       <c r="B167" s="7"/>
       <c r="C167" s="7"/>
@@ -3322,7 +3332,7 @@
       <c r="K167" s="7"/>
       <c r="L167" s="7"/>
     </row>
-    <row r="168" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A168" s="7"/>
       <c r="B168" s="7"/>
       <c r="C168" s="7"/>
@@ -3336,7 +3346,7 @@
       <c r="K168" s="7"/>
       <c r="L168" s="7"/>
     </row>
-    <row r="169" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A169" s="7"/>
       <c r="B169" s="7"/>
       <c r="C169" s="7"/>
@@ -3350,7 +3360,7 @@
       <c r="K169" s="7"/>
       <c r="L169" s="7"/>
     </row>
-    <row r="170" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A170" s="6"/>
       <c r="B170" s="6"/>
       <c r="C170" s="6"/>
@@ -3364,7 +3374,7 @@
       <c r="K170" s="6"/>
       <c r="L170" s="6"/>
     </row>
-    <row r="171" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A171" s="6"/>
       <c r="B171" s="6"/>
       <c r="C171" s="6"/>
@@ -3378,7 +3388,7 @@
       <c r="K171" s="6"/>
       <c r="L171" s="6"/>
     </row>
-    <row r="172" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A172" s="6"/>
       <c r="B172" s="6"/>
       <c r="C172" s="6"/>
@@ -3392,7 +3402,7 @@
       <c r="K172" s="6"/>
       <c r="L172" s="6"/>
     </row>
-    <row r="173" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A173" s="7"/>
       <c r="B173" s="7"/>
       <c r="C173" s="7"/>
@@ -3406,7 +3416,7 @@
       <c r="K173" s="7"/>
       <c r="L173" s="7"/>
     </row>
-    <row r="174" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="174" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A174" s="6"/>
       <c r="B174" s="6"/>
       <c r="C174" s="6"/>
@@ -3420,7 +3430,7 @@
       <c r="K174" s="6"/>
       <c r="L174" s="6"/>
     </row>
-    <row r="175" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="175" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A175" s="6"/>
       <c r="B175" s="6"/>
       <c r="C175" s="6"/>
@@ -3434,7 +3444,7 @@
       <c r="K175" s="6"/>
       <c r="L175" s="6"/>
     </row>
-    <row r="176" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="176" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A176" s="6"/>
       <c r="B176" s="6"/>
       <c r="C176" s="6"/>
@@ -3448,7 +3458,7 @@
       <c r="K176" s="6"/>
       <c r="L176" s="6"/>
     </row>
-    <row r="177" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="177" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A177" s="7"/>
       <c r="B177" s="7"/>
       <c r="C177" s="7"/>
@@ -3462,7 +3472,7 @@
       <c r="K177" s="7"/>
       <c r="L177" s="7"/>
     </row>
-    <row r="178" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="178" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A178" s="7"/>
       <c r="B178" s="7"/>
       <c r="C178" s="7"/>
@@ -3476,7 +3486,7 @@
       <c r="K178" s="7"/>
       <c r="L178" s="7"/>
     </row>
-    <row r="179" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="179" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A179" s="7"/>
       <c r="B179" s="7"/>
       <c r="C179" s="7"/>
@@ -3490,7 +3500,7 @@
       <c r="K179" s="7"/>
       <c r="L179" s="7"/>
     </row>
-    <row r="180" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="180" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A180" s="7"/>
       <c r="B180" s="7"/>
       <c r="C180" s="7"/>
@@ -3504,7 +3514,7 @@
       <c r="K180" s="7"/>
       <c r="L180" s="7"/>
     </row>
-    <row r="181" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="181" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A181" s="7"/>
       <c r="B181" s="7"/>
       <c r="C181" s="7"/>
@@ -3518,7 +3528,7 @@
       <c r="K181" s="7"/>
       <c r="L181" s="7"/>
     </row>
-    <row r="182" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="182" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A182" s="7"/>
       <c r="B182" s="7"/>
       <c r="C182" s="7"/>
@@ -3532,7 +3542,7 @@
       <c r="K182" s="7"/>
       <c r="L182" s="7"/>
     </row>
-    <row r="183" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="183" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A183" s="6"/>
       <c r="B183" s="6"/>
       <c r="C183" s="6"/>
@@ -3546,7 +3556,7 @@
       <c r="K183" s="6"/>
       <c r="L183" s="6"/>
     </row>
-    <row r="184" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="184" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A184" s="6"/>
       <c r="B184" s="6"/>
       <c r="C184" s="6"/>
@@ -3560,7 +3570,7 @@
       <c r="K184" s="6"/>
       <c r="L184" s="6"/>
     </row>
-    <row r="185" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="185" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A185" s="6"/>
       <c r="B185" s="6"/>
       <c r="C185" s="6"/>
@@ -3574,7 +3584,7 @@
       <c r="K185" s="6"/>
       <c r="L185" s="6"/>
     </row>
-    <row r="186" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="186" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A186" s="6"/>
       <c r="B186" s="6"/>
       <c r="C186" s="6"/>
@@ -3588,7 +3598,7 @@
       <c r="K186" s="6"/>
       <c r="L186" s="6"/>
     </row>
-    <row r="187" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="187" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A187" s="7"/>
       <c r="B187" s="7"/>
       <c r="C187" s="7"/>
@@ -3602,7 +3612,7 @@
       <c r="K187" s="7"/>
       <c r="L187" s="7"/>
     </row>
-    <row r="188" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="188" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A188" s="7"/>
       <c r="B188" s="7"/>
       <c r="C188" s="7"/>
@@ -3616,7 +3626,7 @@
       <c r="K188" s="7"/>
       <c r="L188" s="7"/>
     </row>
-    <row r="189" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="189" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A189" s="7"/>
       <c r="B189" s="7"/>
       <c r="C189" s="7"/>
@@ -3630,7 +3640,7 @@
       <c r="K189" s="7"/>
       <c r="L189" s="7"/>
     </row>
-    <row r="190" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="190" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A190" s="7"/>
       <c r="B190" s="7"/>
       <c r="C190" s="7"/>
@@ -3644,7 +3654,7 @@
       <c r="K190" s="7"/>
       <c r="L190" s="7"/>
     </row>
-    <row r="191" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="191" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A191" s="7"/>
       <c r="B191" s="7"/>
       <c r="C191" s="7"/>
@@ -3658,7 +3668,7 @@
       <c r="K191" s="7"/>
       <c r="L191" s="7"/>
     </row>
-    <row r="192" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="192" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A192" s="7"/>
       <c r="B192" s="7"/>
       <c r="C192" s="7"/>
@@ -3672,7 +3682,7 @@
       <c r="K192" s="7"/>
       <c r="L192" s="7"/>
     </row>
-    <row r="193" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="193" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A193" s="7"/>
       <c r="B193" s="7"/>
       <c r="C193" s="7"/>
@@ -3686,7 +3696,7 @@
       <c r="K193" s="7"/>
       <c r="L193" s="7"/>
     </row>
-    <row r="194" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="194" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A194" s="7"/>
       <c r="B194" s="7"/>
       <c r="C194" s="7"/>
@@ -3700,7 +3710,7 @@
       <c r="K194" s="7"/>
       <c r="L194" s="7"/>
     </row>
-    <row r="195" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="195" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A195" s="7"/>
       <c r="B195" s="7"/>
       <c r="C195" s="7"/>
@@ -3714,7 +3724,7 @@
       <c r="K195" s="7"/>
       <c r="L195" s="7"/>
     </row>
-    <row r="196" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="196" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A196" s="7"/>
       <c r="B196" s="7"/>
       <c r="C196" s="7"/>
@@ -3728,7 +3738,7 @@
       <c r="K196" s="7"/>
       <c r="L196" s="7"/>
     </row>
-    <row r="197" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="197" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A197" s="7"/>
       <c r="B197" s="7"/>
       <c r="C197" s="7"/>
@@ -3742,7 +3752,7 @@
       <c r="K197" s="7"/>
       <c r="L197" s="7"/>
     </row>
-    <row r="198" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="198" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A198" s="7"/>
       <c r="B198" s="7"/>
       <c r="C198" s="7"/>
@@ -3756,7 +3766,7 @@
       <c r="K198" s="7"/>
       <c r="L198" s="7"/>
     </row>
-    <row r="199" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="199" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A199" s="7"/>
       <c r="B199" s="7"/>
       <c r="C199" s="7"/>
@@ -3770,7 +3780,7 @@
       <c r="K199" s="7"/>
       <c r="L199" s="7"/>
     </row>
-    <row r="200" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="200" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A200" s="6"/>
       <c r="B200" s="6"/>
       <c r="C200" s="6"/>
@@ -3784,7 +3794,7 @@
       <c r="K200" s="6"/>
       <c r="L200" s="6"/>
     </row>
-    <row r="201" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="201" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A201" s="6"/>
       <c r="B201" s="6"/>
       <c r="C201" s="6"/>
@@ -3798,7 +3808,7 @@
       <c r="K201" s="6"/>
       <c r="L201" s="6"/>
     </row>
-    <row r="202" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="202" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A202" s="6"/>
       <c r="B202" s="6"/>
       <c r="C202" s="6"/>
@@ -3812,7 +3822,7 @@
       <c r="K202" s="6"/>
       <c r="L202" s="6"/>
     </row>
-    <row r="203" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="203" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A203" s="6"/>
       <c r="B203" s="6"/>
       <c r="C203" s="6"/>
@@ -3826,7 +3836,7 @@
       <c r="K203" s="6"/>
       <c r="L203" s="6"/>
     </row>
-    <row r="204" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="204" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A204" s="6"/>
       <c r="B204" s="6"/>
       <c r="C204" s="6"/>
@@ -3840,7 +3850,7 @@
       <c r="K204" s="6"/>
       <c r="L204" s="6"/>
     </row>
-    <row r="205" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="205" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A205" s="6"/>
       <c r="B205" s="6"/>
       <c r="C205" s="6"/>
@@ -3854,7 +3864,7 @@
       <c r="K205" s="6"/>
       <c r="L205" s="6"/>
     </row>
-    <row r="206" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="206" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A206" s="6"/>
       <c r="B206" s="6"/>
       <c r="C206" s="6"/>
@@ -3868,7 +3878,7 @@
       <c r="K206" s="6"/>
       <c r="L206" s="6"/>
     </row>
-    <row r="207" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="207" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A207" s="6"/>
       <c r="B207" s="6"/>
       <c r="C207" s="6"/>
@@ -3882,7 +3892,7 @@
       <c r="K207" s="6"/>
       <c r="L207" s="6"/>
     </row>
-    <row r="208" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="208" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A208" s="6"/>
       <c r="B208" s="6"/>
       <c r="C208" s="6"/>
@@ -3896,7 +3906,7 @@
       <c r="K208" s="6"/>
       <c r="L208" s="6"/>
     </row>
-    <row r="209" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="209" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A209" s="6"/>
       <c r="B209" s="6"/>
       <c r="C209" s="6"/>
@@ -3910,7 +3920,7 @@
       <c r="K209" s="6"/>
       <c r="L209" s="6"/>
     </row>
-    <row r="210" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="210" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A210" s="6"/>
       <c r="B210" s="6"/>
       <c r="C210" s="6"/>
@@ -3924,7 +3934,7 @@
       <c r="K210" s="6"/>
       <c r="L210" s="6"/>
     </row>
-    <row r="211" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="211" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A211" s="6"/>
       <c r="B211" s="6"/>
       <c r="C211" s="6"/>
@@ -3938,7 +3948,7 @@
       <c r="K211" s="6"/>
       <c r="L211" s="6"/>
     </row>
-    <row r="212" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="212" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A212" s="6"/>
       <c r="B212" s="6"/>
       <c r="C212" s="6"/>
@@ -3952,7 +3962,7 @@
       <c r="K212" s="6"/>
       <c r="L212" s="6"/>
     </row>
-    <row r="213" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="213" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A213" s="6"/>
       <c r="B213" s="6"/>
       <c r="C213" s="6"/>
@@ -3966,7 +3976,7 @@
       <c r="K213" s="6"/>
       <c r="L213" s="6"/>
     </row>
-    <row r="214" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="214" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A214" s="6"/>
       <c r="B214" s="6"/>
       <c r="C214" s="6"/>
@@ -3980,7 +3990,7 @@
       <c r="K214" s="6"/>
       <c r="L214" s="6"/>
     </row>
-    <row r="215" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="215" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A215" s="6"/>
       <c r="B215" s="6"/>
       <c r="C215" s="6"/>
@@ -3994,7 +4004,7 @@
       <c r="K215" s="6"/>
       <c r="L215" s="6"/>
     </row>
-    <row r="216" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="216" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A216" s="6"/>
       <c r="B216" s="6"/>
       <c r="C216" s="6"/>
@@ -4008,7 +4018,7 @@
       <c r="K216" s="6"/>
       <c r="L216" s="6"/>
     </row>
-    <row r="217" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="217" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A217" s="6"/>
       <c r="B217" s="6"/>
       <c r="C217" s="6"/>
@@ -4022,7 +4032,7 @@
       <c r="K217" s="6"/>
       <c r="L217" s="6"/>
     </row>
-    <row r="218" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="218" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A218" s="7"/>
       <c r="B218" s="7"/>
       <c r="C218" s="7"/>
@@ -4036,7 +4046,7 @@
       <c r="K218" s="7"/>
       <c r="L218" s="7"/>
     </row>
-    <row r="219" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="219" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A219" s="7"/>
       <c r="B219" s="7"/>
       <c r="C219" s="7"/>
@@ -4050,7 +4060,7 @@
       <c r="K219" s="7"/>
       <c r="L219" s="7"/>
     </row>
-    <row r="220" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="220" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A220" s="7"/>
       <c r="B220" s="7"/>
       <c r="C220" s="7"/>
@@ -4064,7 +4074,7 @@
       <c r="K220" s="7"/>
       <c r="L220" s="7"/>
     </row>
-    <row r="221" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="221" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A221" s="7"/>
       <c r="B221" s="7"/>
       <c r="C221" s="7"/>
@@ -4078,7 +4088,7 @@
       <c r="K221" s="7"/>
       <c r="L221" s="7"/>
     </row>
-    <row r="222" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="222" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A222" s="7"/>
       <c r="B222" s="7"/>
       <c r="C222" s="7"/>
@@ -4092,7 +4102,7 @@
       <c r="K222" s="7"/>
       <c r="L222" s="7"/>
     </row>
-    <row r="223" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="223" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A223" s="7"/>
       <c r="B223" s="7"/>
       <c r="C223" s="7"/>
@@ -4106,7 +4116,7 @@
       <c r="K223" s="7"/>
       <c r="L223" s="7"/>
     </row>
-    <row r="224" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="224" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A224" s="7"/>
       <c r="B224" s="7"/>
       <c r="C224" s="7"/>
@@ -4120,7 +4130,7 @@
       <c r="K224" s="7"/>
       <c r="L224" s="7"/>
     </row>
-    <row r="225" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="225" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A225" s="7"/>
       <c r="B225" s="7"/>
       <c r="C225" s="7"/>
@@ -4134,7 +4144,7 @@
       <c r="K225" s="7"/>
       <c r="L225" s="7"/>
     </row>
-    <row r="226" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="226" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A226" s="7"/>
       <c r="B226" s="7"/>
       <c r="C226" s="7"/>
@@ -4148,7 +4158,7 @@
       <c r="K226" s="7"/>
       <c r="L226" s="7"/>
     </row>
-    <row r="227" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="227" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A227" s="7"/>
       <c r="B227" s="7"/>
       <c r="C227" s="7"/>
@@ -4162,7 +4172,7 @@
       <c r="K227" s="7"/>
       <c r="L227" s="7"/>
     </row>
-    <row r="228" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="228" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A228" s="7"/>
       <c r="B228" s="7"/>
       <c r="C228" s="7"/>
@@ -4176,7 +4186,7 @@
       <c r="K228" s="7"/>
       <c r="L228" s="7"/>
     </row>
-    <row r="229" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="229" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A229" s="7"/>
       <c r="B229" s="7"/>
       <c r="C229" s="7"/>
@@ -4190,7 +4200,7 @@
       <c r="K229" s="7"/>
       <c r="L229" s="7"/>
     </row>
-    <row r="230" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="230" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A230" s="6"/>
       <c r="B230" s="6"/>
       <c r="C230" s="6"/>
@@ -4204,7 +4214,7 @@
       <c r="K230" s="6"/>
       <c r="L230" s="6"/>
     </row>
-    <row r="231" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="231" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A231" s="6"/>
       <c r="B231" s="6"/>
       <c r="C231" s="6"/>
@@ -4218,7 +4228,7 @@
       <c r="K231" s="6"/>
       <c r="L231" s="6"/>
     </row>
-    <row r="232" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="232" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A232" s="6"/>
       <c r="B232" s="6"/>
       <c r="C232" s="6"/>
@@ -4232,7 +4242,7 @@
       <c r="K232" s="6"/>
       <c r="L232" s="6"/>
     </row>
-    <row r="233" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="233" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A233" s="6"/>
       <c r="B233" s="6"/>
       <c r="C233" s="6"/>
@@ -4246,7 +4256,7 @@
       <c r="K233" s="6"/>
       <c r="L233" s="6"/>
     </row>
-    <row r="234" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="234" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A234" s="7"/>
       <c r="B234" s="7"/>
       <c r="C234" s="7"/>
@@ -4260,7 +4270,7 @@
       <c r="K234" s="7"/>
       <c r="L234" s="7"/>
     </row>
-    <row r="235" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="235" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A235" s="7"/>
       <c r="B235" s="7"/>
       <c r="C235" s="7"/>
@@ -4274,7 +4284,7 @@
       <c r="K235" s="7"/>
       <c r="L235" s="7"/>
     </row>
-    <row r="236" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="236" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A236" s="6"/>
       <c r="B236" s="6"/>
       <c r="C236" s="6"/>
@@ -4288,7 +4298,7 @@
       <c r="K236" s="6"/>
       <c r="L236" s="6"/>
     </row>
-    <row r="237" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="237" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A237" s="6"/>
       <c r="B237" s="6"/>
       <c r="C237" s="6"/>
@@ -4302,7 +4312,7 @@
       <c r="K237" s="6"/>
       <c r="L237" s="6"/>
     </row>
-    <row r="238" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="238" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A238" s="7"/>
       <c r="B238" s="7"/>
       <c r="C238" s="7"/>
@@ -4316,7 +4326,7 @@
       <c r="K238" s="7"/>
       <c r="L238" s="7"/>
     </row>
-    <row r="239" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="239" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A239" s="7"/>
       <c r="B239" s="7"/>
       <c r="C239" s="7"/>
@@ -4330,7 +4340,7 @@
       <c r="K239" s="7"/>
       <c r="L239" s="7"/>
     </row>
-    <row r="240" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="240" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A240" s="7"/>
       <c r="B240" s="7"/>
       <c r="C240" s="7"/>
@@ -4344,7 +4354,7 @@
       <c r="K240" s="7"/>
       <c r="L240" s="7"/>
     </row>
-    <row r="241" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="241" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A241" s="6"/>
       <c r="B241" s="6"/>
       <c r="C241" s="6"/>
@@ -4358,7 +4368,7 @@
       <c r="K241" s="6"/>
       <c r="L241" s="6"/>
     </row>
-    <row r="242" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="242" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A242" s="6"/>
       <c r="B242" s="6"/>
       <c r="C242" s="6"/>
@@ -4372,7 +4382,7 @@
       <c r="K242" s="6"/>
       <c r="L242" s="6"/>
     </row>
-    <row r="243" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="243" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A243" s="6"/>
       <c r="B243" s="6"/>
       <c r="C243" s="6"/>
@@ -4386,7 +4396,7 @@
       <c r="K243" s="6"/>
       <c r="L243" s="6"/>
     </row>
-    <row r="244" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="244" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A244" s="6"/>
       <c r="B244" s="6"/>
       <c r="C244" s="6"/>
@@ -4400,7 +4410,7 @@
       <c r="K244" s="6"/>
       <c r="L244" s="6"/>
     </row>
-    <row r="245" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="245" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A245" s="6"/>
       <c r="B245" s="6"/>
       <c r="C245" s="6"/>
@@ -4414,7 +4424,7 @@
       <c r="K245" s="6"/>
       <c r="L245" s="6"/>
     </row>
-    <row r="246" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="246" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A246" s="6"/>
       <c r="B246" s="6"/>
       <c r="C246" s="6"/>
@@ -4428,7 +4438,7 @@
       <c r="K246" s="6"/>
       <c r="L246" s="6"/>
     </row>
-    <row r="247" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="247" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A247" s="6"/>
       <c r="B247" s="6"/>
       <c r="C247" s="6"/>
@@ -4442,7 +4452,7 @@
       <c r="K247" s="6"/>
       <c r="L247" s="6"/>
     </row>
-    <row r="248" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="248" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A248" s="6"/>
       <c r="B248" s="6"/>
       <c r="C248" s="6"/>
@@ -4456,7 +4466,7 @@
       <c r="K248" s="6"/>
       <c r="L248" s="6"/>
     </row>
-    <row r="249" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="249" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A249" s="6"/>
       <c r="B249" s="6"/>
       <c r="C249" s="6"/>
@@ -4470,7 +4480,7 @@
       <c r="K249" s="6"/>
       <c r="L249" s="6"/>
     </row>
-    <row r="250" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="250" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A250" s="6"/>
       <c r="B250" s="6"/>
       <c r="C250" s="6"/>
@@ -4484,7 +4494,7 @@
       <c r="K250" s="6"/>
       <c r="L250" s="6"/>
     </row>
-    <row r="251" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="251" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A251" s="6"/>
       <c r="B251" s="6"/>
       <c r="C251" s="6"/>
@@ -4498,7 +4508,7 @@
       <c r="K251" s="6"/>
       <c r="L251" s="6"/>
     </row>
-    <row r="252" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="252" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A252" s="6"/>
       <c r="B252" s="6"/>
       <c r="C252" s="6"/>
@@ -4512,7 +4522,7 @@
       <c r="K252" s="6"/>
       <c r="L252" s="6"/>
     </row>
-    <row r="253" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="253" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A253" s="6"/>
       <c r="B253" s="6"/>
       <c r="C253" s="6"/>
@@ -4526,7 +4536,7 @@
       <c r="K253" s="6"/>
       <c r="L253" s="6"/>
     </row>
-    <row r="254" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="254" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A254" s="6"/>
       <c r="B254" s="6"/>
       <c r="C254" s="6"/>
@@ -4540,7 +4550,7 @@
       <c r="K254" s="6"/>
       <c r="L254" s="6"/>
     </row>
-    <row r="255" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="255" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A255" s="6"/>
       <c r="B255" s="6"/>
       <c r="C255" s="6"/>
@@ -4554,7 +4564,7 @@
       <c r="K255" s="6"/>
       <c r="L255" s="6"/>
     </row>
-    <row r="256" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="256" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A256" s="6"/>
       <c r="B256" s="6"/>
       <c r="C256" s="6"/>
@@ -4568,7 +4578,7 @@
       <c r="K256" s="6"/>
       <c r="L256" s="6"/>
     </row>
-    <row r="257" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="257" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A257" s="7"/>
       <c r="B257" s="7"/>
       <c r="C257" s="7"/>
@@ -4582,7 +4592,7 @@
       <c r="K257" s="7"/>
       <c r="L257" s="7"/>
     </row>
-    <row r="258" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="258" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A258" s="7"/>
       <c r="B258" s="7"/>
       <c r="C258" s="7"/>
@@ -4596,7 +4606,7 @@
       <c r="K258" s="7"/>
       <c r="L258" s="7"/>
     </row>
-    <row r="259" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="259" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A259" s="7"/>
       <c r="B259" s="7"/>
       <c r="C259" s="7"/>
@@ -4610,7 +4620,7 @@
       <c r="K259" s="7"/>
       <c r="L259" s="7"/>
     </row>
-    <row r="260" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="260" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A260" s="7"/>
       <c r="B260" s="7"/>
       <c r="C260" s="7"/>
@@ -4624,7 +4634,7 @@
       <c r="K260" s="7"/>
       <c r="L260" s="7"/>
     </row>
-    <row r="261" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="261" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A261" s="6"/>
       <c r="B261" s="6"/>
       <c r="C261" s="6"/>
@@ -4638,7 +4648,7 @@
       <c r="K261" s="6"/>
       <c r="L261" s="6"/>
     </row>
-    <row r="262" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="262" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A262" s="6"/>
       <c r="B262" s="6"/>
       <c r="C262" s="6"/>
@@ -4652,7 +4662,7 @@
       <c r="K262" s="6"/>
       <c r="L262" s="6"/>
     </row>
-    <row r="263" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="263" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A263" s="6"/>
       <c r="B263" s="6"/>
       <c r="C263" s="6"/>
@@ -4666,7 +4676,7 @@
       <c r="K263" s="6"/>
       <c r="L263" s="6"/>
     </row>
-    <row r="264" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="264" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A264" s="6"/>
       <c r="B264" s="6"/>
       <c r="C264" s="6"/>
@@ -4680,7 +4690,7 @@
       <c r="K264" s="6"/>
       <c r="L264" s="6"/>
     </row>
-    <row r="265" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="265" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A265" s="6"/>
       <c r="B265" s="6"/>
       <c r="C265" s="6"/>
@@ -4694,7 +4704,7 @@
       <c r="K265" s="6"/>
       <c r="L265" s="6"/>
     </row>
-    <row r="266" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="266" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A266" s="6"/>
       <c r="B266" s="6"/>
       <c r="C266" s="6"/>
@@ -4708,7 +4718,7 @@
       <c r="K266" s="6"/>
       <c r="L266" s="6"/>
     </row>
-    <row r="267" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="267" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A267" s="7"/>
       <c r="B267" s="7"/>
       <c r="C267" s="7"/>
@@ -4722,7 +4732,7 @@
       <c r="K267" s="7"/>
       <c r="L267" s="7"/>
     </row>
-    <row r="268" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="268" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A268" s="7"/>
       <c r="B268" s="7"/>
       <c r="C268" s="7"/>
@@ -4736,7 +4746,7 @@
       <c r="K268" s="7"/>
       <c r="L268" s="7"/>
     </row>
-    <row r="269" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="269" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A269" s="7"/>
       <c r="B269" s="7"/>
       <c r="C269" s="7"/>
@@ -4750,7 +4760,7 @@
       <c r="K269" s="7"/>
       <c r="L269" s="7"/>
     </row>
-    <row r="270" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="270" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A270" s="6"/>
       <c r="B270" s="6"/>
       <c r="C270" s="6"/>
@@ -4764,7 +4774,7 @@
       <c r="K270" s="6"/>
       <c r="L270" s="6"/>
     </row>
-    <row r="271" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="271" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A271" s="6"/>
       <c r="B271" s="6"/>
       <c r="C271" s="6"/>
@@ -4778,7 +4788,7 @@
       <c r="K271" s="6"/>
       <c r="L271" s="6"/>
     </row>
-    <row r="272" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="272" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A272" s="6"/>
       <c r="B272" s="6"/>
       <c r="C272" s="6"/>
@@ -4792,7 +4802,7 @@
       <c r="K272" s="6"/>
       <c r="L272" s="6"/>
     </row>
-    <row r="273" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="273" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A273" s="6"/>
       <c r="B273" s="6"/>
       <c r="C273" s="6"/>
@@ -4806,7 +4816,7 @@
       <c r="K273" s="6"/>
       <c r="L273" s="6"/>
     </row>
-    <row r="274" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="274" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A274" s="6"/>
       <c r="B274" s="6"/>
       <c r="C274" s="6"/>
@@ -4820,7 +4830,7 @@
       <c r="K274" s="6"/>
       <c r="L274" s="6"/>
     </row>
-    <row r="275" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="275" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A275" s="7"/>
       <c r="B275" s="7"/>
       <c r="C275" s="7"/>
@@ -4834,7 +4844,7 @@
       <c r="K275" s="7"/>
       <c r="L275" s="7"/>
     </row>
-    <row r="276" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="276" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A276" s="7"/>
       <c r="B276" s="7"/>
       <c r="C276" s="7"/>
@@ -4848,7 +4858,7 @@
       <c r="K276" s="7"/>
       <c r="L276" s="7"/>
     </row>
-    <row r="277" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="277" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A277" s="7"/>
       <c r="B277" s="7"/>
       <c r="C277" s="7"/>
@@ -4862,7 +4872,7 @@
       <c r="K277" s="7"/>
       <c r="L277" s="7"/>
     </row>
-    <row r="278" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="278" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A278" s="6"/>
       <c r="B278" s="6"/>
       <c r="C278" s="6"/>
@@ -4876,7 +4886,7 @@
       <c r="K278" s="6"/>
       <c r="L278" s="6"/>
     </row>
-    <row r="279" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="279" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A279" s="6"/>
       <c r="B279" s="6"/>
       <c r="C279" s="6"/>
@@ -4890,7 +4900,7 @@
       <c r="K279" s="6"/>
       <c r="L279" s="6"/>
     </row>
-    <row r="280" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="280" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A280" s="6"/>
       <c r="B280" s="6"/>
       <c r="C280" s="6"/>
@@ -4904,7 +4914,7 @@
       <c r="K280" s="6"/>
       <c r="L280" s="6"/>
     </row>
-    <row r="281" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="281" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A281" s="6"/>
       <c r="B281" s="6"/>
       <c r="C281" s="6"/>
@@ -4918,7 +4928,7 @@
       <c r="K281" s="6"/>
       <c r="L281" s="6"/>
     </row>
-    <row r="282" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="282" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A282" s="6"/>
       <c r="B282" s="6"/>
       <c r="C282" s="6"/>
@@ -4932,7 +4942,7 @@
       <c r="K282" s="6"/>
       <c r="L282" s="6"/>
     </row>
-    <row r="283" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="283" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A283" s="6"/>
       <c r="B283" s="6"/>
       <c r="C283" s="6"/>
@@ -4946,7 +4956,7 @@
       <c r="K283" s="6"/>
       <c r="L283" s="6"/>
     </row>
-    <row r="284" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="284" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A284" s="6"/>
       <c r="B284" s="6"/>
       <c r="C284" s="6"/>
@@ -4960,7 +4970,7 @@
       <c r="K284" s="6"/>
       <c r="L284" s="6"/>
     </row>
-    <row r="285" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="285" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A285" s="6"/>
       <c r="B285" s="6"/>
       <c r="C285" s="6"/>
@@ -4974,7 +4984,7 @@
       <c r="K285" s="6"/>
       <c r="L285" s="6"/>
     </row>
-    <row r="286" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="286" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A286" s="7"/>
       <c r="B286" s="7"/>
       <c r="C286" s="7"/>
@@ -4988,7 +4998,7 @@
       <c r="K286" s="7"/>
       <c r="L286" s="7"/>
     </row>
-    <row r="287" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="287" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A287" s="7"/>
       <c r="B287" s="7"/>
       <c r="C287" s="7"/>
@@ -5002,7 +5012,7 @@
       <c r="K287" s="7"/>
       <c r="L287" s="7"/>
     </row>
-    <row r="288" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="288" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A288" s="7"/>
       <c r="B288" s="7"/>
       <c r="C288" s="7"/>
@@ -5016,7 +5026,7 @@
       <c r="K288" s="7"/>
       <c r="L288" s="7"/>
     </row>
-    <row r="289" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="289" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A289" s="7"/>
       <c r="B289" s="7"/>
       <c r="C289" s="7"/>
@@ -5030,7 +5040,7 @@
       <c r="K289" s="7"/>
       <c r="L289" s="7"/>
     </row>
-    <row r="290" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="290" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A290" s="6"/>
       <c r="B290" s="6"/>
       <c r="C290" s="6"/>
@@ -5044,7 +5054,7 @@
       <c r="K290" s="6"/>
       <c r="L290" s="6"/>
     </row>
-    <row r="291" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="291" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A291" s="6"/>
       <c r="B291" s="6"/>
       <c r="C291" s="6"/>
@@ -5058,7 +5068,7 @@
       <c r="K291" s="6"/>
       <c r="L291" s="6"/>
     </row>
-    <row r="292" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="292" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A292" s="6"/>
       <c r="B292" s="6"/>
       <c r="C292" s="6"/>
@@ -5072,7 +5082,7 @@
       <c r="K292" s="6"/>
       <c r="L292" s="6"/>
     </row>
-    <row r="293" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="293" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A293" s="6"/>
       <c r="B293" s="6"/>
       <c r="C293" s="6"/>
@@ -5086,7 +5096,7 @@
       <c r="K293" s="6"/>
       <c r="L293" s="6"/>
     </row>
-    <row r="294" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="294" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A294" s="6"/>
       <c r="B294" s="6"/>
       <c r="C294" s="6"/>
@@ -5100,7 +5110,7 @@
       <c r="K294" s="6"/>
       <c r="L294" s="6"/>
     </row>
-    <row r="295" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="295" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A295" s="6"/>
       <c r="B295" s="6"/>
       <c r="C295" s="6"/>
@@ -5114,7 +5124,7 @@
       <c r="K295" s="6"/>
       <c r="L295" s="6"/>
     </row>
-    <row r="296" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="296" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A296" s="6"/>
       <c r="B296" s="6"/>
       <c r="C296" s="6"/>
@@ -5128,7 +5138,7 @@
       <c r="K296" s="6"/>
       <c r="L296" s="6"/>
     </row>
-    <row r="297" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="297" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A297" s="7"/>
       <c r="B297" s="7"/>
       <c r="C297" s="7"/>
@@ -5142,7 +5152,7 @@
       <c r="K297" s="7"/>
       <c r="L297" s="7"/>
     </row>
-    <row r="298" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="298" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A298" s="7"/>
       <c r="B298" s="7"/>
       <c r="C298" s="7"/>
@@ -5156,7 +5166,7 @@
       <c r="K298" s="7"/>
       <c r="L298" s="7"/>
     </row>
-    <row r="299" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="299" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A299" s="7"/>
       <c r="B299" s="7"/>
       <c r="C299" s="7"/>
@@ -5170,7 +5180,7 @@
       <c r="K299" s="7"/>
       <c r="L299" s="7"/>
     </row>
-    <row r="300" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="300" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A300" s="7"/>
       <c r="B300" s="7"/>
       <c r="C300" s="7"/>
@@ -5184,7 +5194,7 @@
       <c r="K300" s="7"/>
       <c r="L300" s="7"/>
     </row>
-    <row r="301" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="301" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A301" s="7"/>
       <c r="B301" s="7"/>
       <c r="C301" s="7"/>
@@ -5198,7 +5208,7 @@
       <c r="K301" s="7"/>
       <c r="L301" s="7"/>
     </row>
-    <row r="302" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="302" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A302" s="7"/>
       <c r="B302" s="7"/>
       <c r="C302" s="7"/>
@@ -5212,7 +5222,7 @@
       <c r="K302" s="7"/>
       <c r="L302" s="7"/>
     </row>
-    <row r="303" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="303" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A303" s="7"/>
       <c r="B303" s="7"/>
       <c r="C303" s="7"/>
@@ -5226,7 +5236,7 @@
       <c r="K303" s="7"/>
       <c r="L303" s="7"/>
     </row>
-    <row r="304" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="304" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A304" s="7"/>
       <c r="B304" s="7"/>
       <c r="C304" s="7"/>
@@ -5240,7 +5250,7 @@
       <c r="K304" s="7"/>
       <c r="L304" s="7"/>
     </row>
-    <row r="305" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="305" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A305" s="6"/>
       <c r="B305" s="6"/>
       <c r="C305" s="6"/>
@@ -5254,7 +5264,7 @@
       <c r="K305" s="6"/>
       <c r="L305" s="6"/>
     </row>
-    <row r="306" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="306" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A306" s="6"/>
       <c r="B306" s="6"/>
       <c r="C306" s="6"/>
@@ -5268,7 +5278,7 @@
       <c r="K306" s="6"/>
       <c r="L306" s="6"/>
     </row>
-    <row r="307" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="307" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A307" s="7"/>
       <c r="B307" s="7"/>
       <c r="C307" s="7"/>
@@ -5282,7 +5292,7 @@
       <c r="K307" s="7"/>
       <c r="L307" s="7"/>
     </row>
-    <row r="308" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="308" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A308" s="7"/>
       <c r="B308" s="7"/>
       <c r="C308" s="7"/>
@@ -5296,7 +5306,7 @@
       <c r="K308" s="7"/>
       <c r="L308" s="7"/>
     </row>
-    <row r="309" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="309" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A309" s="7"/>
       <c r="B309" s="7"/>
       <c r="C309" s="7"/>
@@ -5310,7 +5320,7 @@
       <c r="K309" s="7"/>
       <c r="L309" s="7"/>
     </row>
-    <row r="310" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="310" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A310" s="7"/>
       <c r="B310" s="7"/>
       <c r="C310" s="7"/>
@@ -5324,7 +5334,7 @@
       <c r="K310" s="7"/>
       <c r="L310" s="7"/>
     </row>
-    <row r="311" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="311" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A311" s="7"/>
       <c r="B311" s="7"/>
       <c r="C311" s="7"/>
@@ -5338,7 +5348,7 @@
       <c r="K311" s="7"/>
       <c r="L311" s="7"/>
     </row>
-    <row r="312" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="312" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A312" s="6"/>
       <c r="B312" s="6"/>
       <c r="C312" s="6"/>
@@ -5352,7 +5362,7 @@
       <c r="K312" s="6"/>
       <c r="L312" s="6"/>
     </row>
-    <row r="313" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="313" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A313" s="6"/>
       <c r="B313" s="6"/>
       <c r="C313" s="6"/>
@@ -5366,7 +5376,7 @@
       <c r="K313" s="6"/>
       <c r="L313" s="6"/>
     </row>
-    <row r="314" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="314" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A314" s="6"/>
       <c r="B314" s="6"/>
       <c r="C314" s="6"/>
@@ -5380,7 +5390,7 @@
       <c r="K314" s="6"/>
       <c r="L314" s="6"/>
     </row>
-    <row r="315" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="315" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A315" s="6"/>
       <c r="B315" s="6"/>
       <c r="C315" s="6"/>
@@ -5394,7 +5404,7 @@
       <c r="K315" s="6"/>
       <c r="L315" s="6"/>
     </row>
-    <row r="316" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="316" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A316" s="7"/>
       <c r="B316" s="7"/>
       <c r="C316" s="7"/>
@@ -5408,7 +5418,7 @@
       <c r="K316" s="7"/>
       <c r="L316" s="7"/>
     </row>
-    <row r="317" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="317" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A317" s="7"/>
       <c r="B317" s="7"/>
       <c r="C317" s="7"/>
@@ -5422,7 +5432,7 @@
       <c r="K317" s="7"/>
       <c r="L317" s="7"/>
     </row>
-    <row r="318" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="318" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A318" s="7"/>
       <c r="B318" s="7"/>
       <c r="C318" s="7"/>
@@ -5436,7 +5446,7 @@
       <c r="K318" s="7"/>
       <c r="L318" s="7"/>
     </row>
-    <row r="319" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="319" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A319" s="6"/>
       <c r="B319" s="6"/>
       <c r="C319" s="6"/>
@@ -5450,7 +5460,7 @@
       <c r="K319" s="6"/>
       <c r="L319" s="6"/>
     </row>
-    <row r="320" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="320" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A320" s="6"/>
       <c r="B320" s="6"/>
       <c r="C320" s="6"/>
@@ -5464,7 +5474,7 @@
       <c r="K320" s="6"/>
       <c r="L320" s="6"/>
     </row>
-    <row r="321" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="321" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A321" s="6"/>
       <c r="B321" s="6"/>
       <c r="C321" s="6"/>
@@ -5478,7 +5488,7 @@
       <c r="K321" s="6"/>
       <c r="L321" s="6"/>
     </row>
-    <row r="322" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="322" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A322" s="6"/>
       <c r="B322" s="6"/>
       <c r="C322" s="6"/>
@@ -5492,7 +5502,7 @@
       <c r="K322" s="6"/>
       <c r="L322" s="6"/>
     </row>
-    <row r="323" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="323" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A323" s="6"/>
       <c r="B323" s="6"/>
       <c r="C323" s="6"/>
@@ -5506,7 +5516,7 @@
       <c r="K323" s="6"/>
       <c r="L323" s="6"/>
     </row>
-    <row r="324" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="324" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A324" s="6"/>
       <c r="B324" s="6"/>
       <c r="C324" s="6"/>
@@ -5520,7 +5530,7 @@
       <c r="K324" s="6"/>
       <c r="L324" s="6"/>
     </row>
-    <row r="325" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="325" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A325" s="7"/>
       <c r="B325" s="7"/>
       <c r="C325" s="7"/>
@@ -5534,7 +5544,7 @@
       <c r="K325" s="7"/>
       <c r="L325" s="7"/>
     </row>
-    <row r="326" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="326" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A326" s="7"/>
       <c r="B326" s="7"/>
       <c r="C326" s="7"/>
@@ -5548,7 +5558,7 @@
       <c r="K326" s="7"/>
       <c r="L326" s="7"/>
     </row>
-    <row r="327" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="327" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A327" s="7"/>
       <c r="B327" s="7"/>
       <c r="C327" s="7"/>
@@ -5562,7 +5572,7 @@
       <c r="K327" s="7"/>
       <c r="L327" s="7"/>
     </row>
-    <row r="328" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="328" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A328" s="7"/>
       <c r="B328" s="7"/>
       <c r="C328" s="7"/>
@@ -5576,7 +5586,7 @@
       <c r="K328" s="7"/>
       <c r="L328" s="7"/>
     </row>
-    <row r="329" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="329" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A329" s="7"/>
       <c r="B329" s="7"/>
       <c r="C329" s="7"/>
@@ -5590,7 +5600,7 @@
       <c r="K329" s="7"/>
       <c r="L329" s="7"/>
     </row>
-    <row r="330" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="330" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A330" s="7"/>
       <c r="B330" s="7"/>
       <c r="C330" s="7"/>
@@ -5604,7 +5614,7 @@
       <c r="K330" s="7"/>
       <c r="L330" s="7"/>
     </row>
-    <row r="331" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="331" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A331" s="7"/>
       <c r="B331" s="7"/>
       <c r="C331" s="7"/>
@@ -5618,7 +5628,7 @@
       <c r="K331" s="7"/>
       <c r="L331" s="7"/>
     </row>
-    <row r="332" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="332" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A332" s="6"/>
       <c r="B332" s="6"/>
       <c r="C332" s="6"/>
@@ -5632,7 +5642,7 @@
       <c r="K332" s="6"/>
       <c r="L332" s="6"/>
     </row>
-    <row r="333" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="333" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A333" s="6"/>
       <c r="B333" s="6"/>
       <c r="C333" s="6"/>
@@ -5646,7 +5656,7 @@
       <c r="K333" s="6"/>
       <c r="L333" s="6"/>
     </row>
-    <row r="334" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="334" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A334" s="6"/>
       <c r="B334" s="6"/>
       <c r="C334" s="6"/>
@@ -5669,22 +5679,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:H61"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C13" sqref="C13"/>
+      <selection pane="bottomLeft" activeCell="H3" sqref="H3:H61"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="26.44140625" customWidth="1"/>
+    <col min="1" max="1" width="26.5" customWidth="1"/>
     <col min="2" max="3" width="13" customWidth="1"/>
-    <col min="4" max="4" width="29.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="29.5" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="70" customWidth="1"/>
-    <col min="6" max="7" width="13" hidden="1" customWidth="1"/>
-    <col min="8" max="8" width="70" hidden="1" customWidth="1"/>
+    <col min="6" max="7" width="13" customWidth="1"/>
+    <col min="8" max="8" width="70" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="25.8" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:8" ht="26" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>25</v>
       </c>
@@ -5696,7 +5706,7 @@
       <c r="G1" s="4"/>
       <c r="H1" s="4"/>
     </row>
-    <row r="2" spans="1:8" ht="18" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" ht="19" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>15</v>
       </c>
@@ -5722,315 +5732,316 @@
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>76</v>
+      </c>
+      <c r="D3" t="s">
+        <v>77</v>
+      </c>
+      <c r="H3" s="8" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>78</v>
+      </c>
+      <c r="D4" t="s">
+        <v>76</v>
+      </c>
+      <c r="H4" s="8" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="H5" s="8" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="H6" s="8" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="H7" s="8" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="H8" s="8" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="H9" s="8" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="H10" s="8" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="H11" s="8" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="H12" s="8" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="H13" s="8" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="H14" s="8" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="H15" s="8" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="H16" s="8" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="17" spans="8:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="H17" s="8" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="18" spans="8:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="H18" s="8" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="19" spans="8:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="H19" s="8" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="20" spans="8:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="H20" s="8" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="21" spans="8:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="H21" s="8" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="22" spans="8:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="H22" s="8" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="23" spans="8:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="H23" s="8" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="24" spans="8:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="H24" s="8" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="25" spans="8:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="H25" s="8" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="26" spans="8:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="H26" s="8" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="27" spans="8:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="H27" s="8" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="28" spans="8:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="H28" s="8" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="29" spans="8:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="H29" s="8" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="30" spans="8:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="H30" s="8" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="31" spans="8:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="H31" s="8" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="32" spans="8:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="H32" s="8" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="33" spans="8:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="H33" s="8" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="34" spans="8:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="H34" s="8" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="35" spans="8:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="H35" s="8" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="36" spans="8:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="H36" s="8" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="37" spans="8:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="H37" s="8" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="38" spans="8:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="H38" s="8" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="39" spans="8:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="H39" s="8" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="40" spans="8:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="H40" s="8" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="41" spans="8:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="H41" s="8" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="42" spans="8:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="H42" s="8" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="43" spans="8:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="H43" s="8" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="44" spans="8:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="H44" s="8" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="45" spans="8:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="H45" s="8" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="46" spans="8:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="H46" s="8" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="47" spans="8:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="H47" s="8" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="48" spans="8:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="H48" s="8" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="49" spans="8:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="H49" s="8" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="50" spans="8:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="H50" s="8" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="51" spans="8:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="H51" s="8" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="52" spans="8:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="H52" s="8" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="53" spans="8:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="H53" s="8" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="54" spans="8:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="H54" s="8" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="55" spans="8:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="H55" s="8" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="56" spans="8:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="H56" s="8" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="57" spans="8:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="H57" s="8" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="58" spans="8:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="H58" s="8" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="59" spans="8:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="H59" s="8" t="s">
         <v>135</v>
       </c>
-      <c r="D3" t="s">
+    </row>
+    <row r="60" spans="8:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="H60" s="8" t="s">
         <v>136</v>
       </c>
-      <c r="H3" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+    </row>
+    <row r="61" spans="8:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="H61" s="8" t="s">
         <v>137</v>
-      </c>
-      <c r="D4" t="s">
-        <v>135</v>
-      </c>
-      <c r="H4" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="H5" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="H6" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="H7" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="H8" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="H9" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="H10" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="H11" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="H12" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="H13" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="H14" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="H15" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="H16" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="17" spans="8:8" x14ac:dyDescent="0.3">
-      <c r="H17" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="18" spans="8:8" x14ac:dyDescent="0.3">
-      <c r="H18" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="19" spans="8:8" x14ac:dyDescent="0.3">
-      <c r="H19" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="20" spans="8:8" x14ac:dyDescent="0.3">
-      <c r="H20" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="21" spans="8:8" x14ac:dyDescent="0.3">
-      <c r="H21" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="22" spans="8:8" x14ac:dyDescent="0.3">
-      <c r="H22" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="23" spans="8:8" x14ac:dyDescent="0.3">
-      <c r="H23" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="24" spans="8:8" x14ac:dyDescent="0.3">
-      <c r="H24" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="25" spans="8:8" x14ac:dyDescent="0.3">
-      <c r="H25" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="26" spans="8:8" x14ac:dyDescent="0.3">
-      <c r="H26" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="27" spans="8:8" x14ac:dyDescent="0.3">
-      <c r="H27" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="28" spans="8:8" x14ac:dyDescent="0.3">
-      <c r="H28" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="29" spans="8:8" x14ac:dyDescent="0.3">
-      <c r="H29" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="30" spans="8:8" x14ac:dyDescent="0.3">
-      <c r="H30" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="31" spans="8:8" x14ac:dyDescent="0.3">
-      <c r="H31" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="32" spans="8:8" x14ac:dyDescent="0.3">
-      <c r="H32" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="33" spans="8:8" x14ac:dyDescent="0.3">
-      <c r="H33" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="34" spans="8:8" x14ac:dyDescent="0.3">
-      <c r="H34" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="35" spans="8:8" x14ac:dyDescent="0.3">
-      <c r="H35" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="36" spans="8:8" x14ac:dyDescent="0.3">
-      <c r="H36" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="37" spans="8:8" x14ac:dyDescent="0.3">
-      <c r="H37" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="38" spans="8:8" x14ac:dyDescent="0.3">
-      <c r="H38" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="39" spans="8:8" x14ac:dyDescent="0.3">
-      <c r="H39" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="40" spans="8:8" x14ac:dyDescent="0.3">
-      <c r="H40" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="41" spans="8:8" x14ac:dyDescent="0.3">
-      <c r="H41" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="42" spans="8:8" x14ac:dyDescent="0.3">
-      <c r="H42" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="43" spans="8:8" x14ac:dyDescent="0.3">
-      <c r="H43" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="44" spans="8:8" x14ac:dyDescent="0.3">
-      <c r="H44" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="45" spans="8:8" x14ac:dyDescent="0.3">
-      <c r="H45" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="46" spans="8:8" x14ac:dyDescent="0.3">
-      <c r="H46" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="47" spans="8:8" x14ac:dyDescent="0.3">
-      <c r="H47" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="48" spans="8:8" x14ac:dyDescent="0.3">
-      <c r="H48" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="49" spans="8:8" x14ac:dyDescent="0.3">
-      <c r="H49" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="50" spans="8:8" x14ac:dyDescent="0.3">
-      <c r="H50" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="51" spans="8:8" x14ac:dyDescent="0.3">
-      <c r="H51" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="52" spans="8:8" x14ac:dyDescent="0.3">
-      <c r="H52" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="53" spans="8:8" x14ac:dyDescent="0.3">
-      <c r="H53" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="54" spans="8:8" x14ac:dyDescent="0.3">
-      <c r="H54" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="55" spans="8:8" x14ac:dyDescent="0.3">
-      <c r="H55" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="56" spans="8:8" x14ac:dyDescent="0.3">
-      <c r="H56" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="57" spans="8:8" x14ac:dyDescent="0.3">
-      <c r="H57" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="58" spans="8:8" x14ac:dyDescent="0.3">
-      <c r="H58" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="59" spans="8:8" x14ac:dyDescent="0.3">
-      <c r="H59" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="60" spans="8:8" x14ac:dyDescent="0.3">
-      <c r="H60" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="61" spans="8:8" x14ac:dyDescent="0.3">
-      <c r="H61" t="s">
-        <v>85</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
@@ -6040,186 +6051,186 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="13" customWidth="1"/>
-    <col min="2" max="2" width="48.44140625" customWidth="1"/>
+    <col min="2" max="2" width="48.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>86</v>
+        <v>27</v>
       </c>
       <c r="B1" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>88</v>
+        <v>29</v>
       </c>
       <c r="B2" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>90</v>
+        <v>31</v>
       </c>
       <c r="B3" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>92</v>
+        <v>33</v>
       </c>
       <c r="B4" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>94</v>
+        <v>35</v>
       </c>
       <c r="B5" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>96</v>
+        <v>37</v>
       </c>
       <c r="B6" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>98</v>
+        <v>39</v>
       </c>
       <c r="B7" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>100</v>
+        <v>41</v>
       </c>
       <c r="B8" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>102</v>
+        <v>43</v>
       </c>
       <c r="B9" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>104</v>
+        <v>45</v>
       </c>
       <c r="B10" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>106</v>
+        <v>47</v>
       </c>
       <c r="B11" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>108</v>
+        <v>49</v>
       </c>
       <c r="B12" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
-        <v>110</v>
+        <v>51</v>
       </c>
       <c r="B13" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
-        <v>112</v>
+        <v>53</v>
       </c>
       <c r="B14" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
-        <v>114</v>
+        <v>55</v>
       </c>
       <c r="B15" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
-        <v>116</v>
+        <v>57</v>
       </c>
       <c r="B16" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
-        <v>118</v>
+        <v>59</v>
       </c>
       <c r="B17" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
-        <v>120</v>
+        <v>61</v>
       </c>
       <c r="B18" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
-        <v>122</v>
+        <v>63</v>
       </c>
       <c r="B19" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
-        <v>124</v>
+        <v>65</v>
       </c>
       <c r="B20" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
-        <v>126</v>
+        <v>67</v>
       </c>
       <c r="B21" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
-        <v>128</v>
+        <v>69</v>
       </c>
       <c r="B22" t="s">
-        <v>129</v>
+        <v>70</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Neat 968 rename info rules to conceptual dm (#1182)
</commit_message>
<xml_diff>
--- a/tests/data/_schema/conceptual/only_concepts.xlsx
+++ b/tests/data/_schema/conceptual/only_concepts.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10512"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AndersAlbert\Projects\internal\neat\tests\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nikola/Repos/neat/tests/data/_schema/conceptual/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B24E51D4-BDA2-4CB4-85AA-7439C45A42FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6686FB3-51CC-9A4D-B93E-56A519791CEC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="48520" windowHeight="27500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Metadata" sheetId="1" r:id="rId1"/>
@@ -106,183 +106,6 @@
     <t>Implements</t>
   </si>
   <si>
-    <t>http://purl.org/cognite/neat/data-model/verified/logical/neat_space/NeatInferredDataModel/v1/CircuitShare</t>
-  </si>
-  <si>
-    <t>http://purl.org/cognite/neat/data-model/verified/logical/neat_space/NeatInferredDataModel/v1/EnergyCongestionZone</t>
-  </si>
-  <si>
-    <t>http://purl.org/cognite/neat/data-model/verified/logical/neat_space/NeatInferredDataModel/v1/EnergySchedulingArea</t>
-  </si>
-  <si>
-    <t>http://purl.org/cognite/neat/data-model/verified/logical/neat_space/NeatInferredDataModel/v1/LineCircuit</t>
-  </si>
-  <si>
-    <t>http://purl.org/cognite/neat/data-model/verified/logical/neat_space/NeatInferredDataModel/v1/PowerTransferCorridor</t>
-  </si>
-  <si>
-    <t>http://purl.org/cognite/neat/data-model/verified/logical/neat_space/NeatInferredDataModel/v1/RateTemperature</t>
-  </si>
-  <si>
-    <t>http://purl.org/cognite/neat/data-model/verified/logical/neat_space/NeatInferredDataModel/v1/ACLineSegment</t>
-  </si>
-  <si>
-    <t>http://purl.org/cognite/neat/data-model/verified/logical/neat_space/NeatInferredDataModel/v1/ActivePowerLimit</t>
-  </si>
-  <si>
-    <t>http://purl.org/cognite/neat/data-model/verified/logical/neat_space/NeatInferredDataModel/v1/Analog</t>
-  </si>
-  <si>
-    <t>http://purl.org/cognite/neat/data-model/verified/logical/neat_space/NeatInferredDataModel/v1/AnalogValue</t>
-  </si>
-  <si>
-    <t>http://purl.org/cognite/neat/data-model/verified/logical/neat_space/NeatInferredDataModel/v1/BasePower</t>
-  </si>
-  <si>
-    <t>http://purl.org/cognite/neat/data-model/verified/logical/neat_space/NeatInferredDataModel/v1/BaseVoltage</t>
-  </si>
-  <si>
-    <t>http://purl.org/cognite/neat/data-model/verified/logical/neat_space/NeatInferredDataModel/v1/Bay</t>
-  </si>
-  <si>
-    <t>http://purl.org/cognite/neat/data-model/verified/logical/neat_space/NeatInferredDataModel/v1/Breaker</t>
-  </si>
-  <si>
-    <t>http://purl.org/cognite/neat/data-model/verified/logical/neat_space/NeatInferredDataModel/v1/BusbarSection</t>
-  </si>
-  <si>
-    <t>http://purl.org/cognite/neat/data-model/verified/logical/neat_space/NeatInferredDataModel/v1/ConformLoad</t>
-  </si>
-  <si>
-    <t>http://purl.org/cognite/neat/data-model/verified/logical/neat_space/NeatInferredDataModel/v1/ConformLoadGroup</t>
-  </si>
-  <si>
-    <t>http://purl.org/cognite/neat/data-model/verified/logical/neat_space/NeatInferredDataModel/v1/ConnectivityNode</t>
-  </si>
-  <si>
-    <t>http://purl.org/cognite/neat/data-model/verified/logical/neat_space/NeatInferredDataModel/v1/ControlArea</t>
-  </si>
-  <si>
-    <t>http://purl.org/cognite/neat/data-model/verified/logical/neat_space/NeatInferredDataModel/v1/ControlAreaGeneratingUnit</t>
-  </si>
-  <si>
-    <t>http://purl.org/cognite/neat/data-model/verified/logical/neat_space/NeatInferredDataModel/v1/CurrentLimit</t>
-  </si>
-  <si>
-    <t>http://purl.org/cognite/neat/data-model/verified/logical/neat_space/NeatInferredDataModel/v1/Disconnector</t>
-  </si>
-  <si>
-    <t>http://purl.org/cognite/neat/data-model/verified/logical/neat_space/NeatInferredDataModel/v1/GeneratingUnit</t>
-  </si>
-  <si>
-    <t>http://purl.org/cognite/neat/data-model/verified/logical/neat_space/NeatInferredDataModel/v1/GeographicalRegion</t>
-  </si>
-  <si>
-    <t>http://purl.org/cognite/neat/data-model/verified/logical/neat_space/NeatInferredDataModel/v1/Line</t>
-  </si>
-  <si>
-    <t>http://purl.org/cognite/neat/data-model/verified/logical/neat_space/NeatInferredDataModel/v1/LinearShuntCompensator</t>
-  </si>
-  <si>
-    <t>http://purl.org/cognite/neat/data-model/verified/logical/neat_space/NeatInferredDataModel/v1/LoadArea</t>
-  </si>
-  <si>
-    <t>http://purl.org/cognite/neat/data-model/verified/logical/neat_space/NeatInferredDataModel/v1/LoadResponseCharacteristic</t>
-  </si>
-  <si>
-    <t>http://purl.org/cognite/neat/data-model/verified/logical/neat_space/NeatInferredDataModel/v1/MeasurementValueSource</t>
-  </si>
-  <si>
-    <t>http://purl.org/cognite/neat/data-model/verified/logical/neat_space/NeatInferredDataModel/v1/NonConformLoad</t>
-  </si>
-  <si>
-    <t>http://purl.org/cognite/neat/data-model/verified/logical/neat_space/NeatInferredDataModel/v1/NonConformLoadGroup</t>
-  </si>
-  <si>
-    <t>http://purl.org/cognite/neat/data-model/verified/logical/neat_space/NeatInferredDataModel/v1/OperatingParticipant</t>
-  </si>
-  <si>
-    <t>http://purl.org/cognite/neat/data-model/verified/logical/neat_space/NeatInferredDataModel/v1/OperatingShare</t>
-  </si>
-  <si>
-    <t>http://purl.org/cognite/neat/data-model/verified/logical/neat_space/NeatInferredDataModel/v1/OperationalLimitSet</t>
-  </si>
-  <si>
-    <t>http://purl.org/cognite/neat/data-model/verified/logical/neat_space/NeatInferredDataModel/v1/OperationalLimitType</t>
-  </si>
-  <si>
-    <t>http://purl.org/cognite/neat/data-model/verified/logical/neat_space/NeatInferredDataModel/v1/PowerTransformer</t>
-  </si>
-  <si>
-    <t>http://purl.org/cognite/neat/data-model/verified/logical/neat_space/NeatInferredDataModel/v1/PowerTransformerEnd</t>
-  </si>
-  <si>
-    <t>http://purl.org/cognite/neat/data-model/verified/logical/neat_space/NeatInferredDataModel/v1/RatioTapChanger</t>
-  </si>
-  <si>
-    <t>http://purl.org/cognite/neat/data-model/verified/logical/neat_space/NeatInferredDataModel/v1/RegulatingControl</t>
-  </si>
-  <si>
-    <t>http://purl.org/cognite/neat/data-model/verified/logical/neat_space/NeatInferredDataModel/v1/SubGeographicalRegion</t>
-  </si>
-  <si>
-    <t>http://purl.org/cognite/neat/data-model/verified/logical/neat_space/NeatInferredDataModel/v1/SubLoadArea</t>
-  </si>
-  <si>
-    <t>http://purl.org/cognite/neat/data-model/verified/logical/neat_space/NeatInferredDataModel/v1/Substation</t>
-  </si>
-  <si>
-    <t>http://purl.org/cognite/neat/data-model/verified/logical/neat_space/NeatInferredDataModel/v1/SynchronousMachine</t>
-  </si>
-  <si>
-    <t>http://purl.org/cognite/neat/data-model/verified/logical/neat_space/NeatInferredDataModel/v1/TapChangerControl</t>
-  </si>
-  <si>
-    <t>http://purl.org/cognite/neat/data-model/verified/logical/neat_space/NeatInferredDataModel/v1/Terminal</t>
-  </si>
-  <si>
-    <t>http://purl.org/cognite/neat/data-model/verified/logical/neat_space/NeatInferredDataModel/v1/VoltageLevel</t>
-  </si>
-  <si>
-    <t>http://purl.org/cognite/neat/data-model/verified/logical/neat_space/NeatInferredDataModel/v1/VoltageLimit</t>
-  </si>
-  <si>
-    <t>http://purl.org/cognite/neat/data-model/verified/logical/neat_space/NeatInferredDataModel/v1/Gate</t>
-  </si>
-  <si>
-    <t>http://purl.org/cognite/neat/data-model/verified/logical/neat_space/NeatInferredDataModel/v1/PinEquipment</t>
-  </si>
-  <si>
-    <t>http://purl.org/cognite/neat/data-model/verified/logical/neat_space/NeatInferredDataModel/v1/PinGate</t>
-  </si>
-  <si>
-    <t>http://purl.org/cognite/neat/data-model/verified/logical/neat_space/NeatInferredDataModel/v1/PinTerminal</t>
-  </si>
-  <si>
-    <t>http://purl.org/cognite/neat/data-model/verified/logical/neat_space/NeatInferredDataModel/v1/ProtectiveActionAdjustment</t>
-  </si>
-  <si>
-    <t>http://purl.org/cognite/neat/data-model/verified/logical/neat_space/NeatInferredDataModel/v1/ProtectiveActionCollection</t>
-  </si>
-  <si>
-    <t>http://purl.org/cognite/neat/data-model/verified/logical/neat_space/NeatInferredDataModel/v1/ProtectiveActionEquipment</t>
-  </si>
-  <si>
-    <t>http://purl.org/cognite/neat/data-model/verified/logical/neat_space/NeatInferredDataModel/v1/RemedialActionScheme</t>
-  </si>
-  <si>
-    <t>http://purl.org/cognite/neat/data-model/verified/logical/neat_space/NeatInferredDataModel/v1/Stage</t>
-  </si>
-  <si>
-    <t>http://purl.org/cognite/neat/data-model/verified/logical/neat_space/NeatInferredDataModel/v1/StageTrigger</t>
-  </si>
-  <si>
-    <t>http://purl.org/cognite/neat/data-model/verified/logical/neat_space/NeatInferredDataModel/v1/FullModel</t>
-  </si>
-  <si>
-    <t>http://purl.org/cognite/neat/data-model/verified/logical/neat_space/NeatInferredDataModel/v1/ScheduleResourceGeneration</t>
-  </si>
-  <si>
     <t>Prefix</t>
   </si>
   <si>
@@ -437,6 +260,183 @@
   </si>
   <si>
     <t>WindTurbine</t>
+  </si>
+  <si>
+    <t>http://purl.org/cognite/neat/data-model/verified/conceptual/neat_space/NeatInferredDataModel/v1/CircuitShare</t>
+  </si>
+  <si>
+    <t>http://purl.org/cognite/neat/data-model/verified/conceptual/neat_space/NeatInferredDataModel/v1/EnergyCongestionZone</t>
+  </si>
+  <si>
+    <t>http://purl.org/cognite/neat/data-model/verified/conceptual/neat_space/NeatInferredDataModel/v1/EnergySchedulingArea</t>
+  </si>
+  <si>
+    <t>http://purl.org/cognite/neat/data-model/verified/conceptual/neat_space/NeatInferredDataModel/v1/LineCircuit</t>
+  </si>
+  <si>
+    <t>http://purl.org/cognite/neat/data-model/verified/conceptual/neat_space/NeatInferredDataModel/v1/PowerTransferCorridor</t>
+  </si>
+  <si>
+    <t>http://purl.org/cognite/neat/data-model/verified/conceptual/neat_space/NeatInferredDataModel/v1/RateTemperature</t>
+  </si>
+  <si>
+    <t>http://purl.org/cognite/neat/data-model/verified/conceptual/neat_space/NeatInferredDataModel/v1/ACLineSegment</t>
+  </si>
+  <si>
+    <t>http://purl.org/cognite/neat/data-model/verified/conceptual/neat_space/NeatInferredDataModel/v1/ActivePowerLimit</t>
+  </si>
+  <si>
+    <t>http://purl.org/cognite/neat/data-model/verified/conceptual/neat_space/NeatInferredDataModel/v1/Analog</t>
+  </si>
+  <si>
+    <t>http://purl.org/cognite/neat/data-model/verified/conceptual/neat_space/NeatInferredDataModel/v1/AnalogValue</t>
+  </si>
+  <si>
+    <t>http://purl.org/cognite/neat/data-model/verified/conceptual/neat_space/NeatInferredDataModel/v1/BasePower</t>
+  </si>
+  <si>
+    <t>http://purl.org/cognite/neat/data-model/verified/conceptual/neat_space/NeatInferredDataModel/v1/BaseVoltage</t>
+  </si>
+  <si>
+    <t>http://purl.org/cognite/neat/data-model/verified/conceptual/neat_space/NeatInferredDataModel/v1/Bay</t>
+  </si>
+  <si>
+    <t>http://purl.org/cognite/neat/data-model/verified/conceptual/neat_space/NeatInferredDataModel/v1/Breaker</t>
+  </si>
+  <si>
+    <t>http://purl.org/cognite/neat/data-model/verified/conceptual/neat_space/NeatInferredDataModel/v1/BusbarSection</t>
+  </si>
+  <si>
+    <t>http://purl.org/cognite/neat/data-model/verified/conceptual/neat_space/NeatInferredDataModel/v1/ConformLoad</t>
+  </si>
+  <si>
+    <t>http://purl.org/cognite/neat/data-model/verified/conceptual/neat_space/NeatInferredDataModel/v1/ConformLoadGroup</t>
+  </si>
+  <si>
+    <t>http://purl.org/cognite/neat/data-model/verified/conceptual/neat_space/NeatInferredDataModel/v1/ConnectivityNode</t>
+  </si>
+  <si>
+    <t>http://purl.org/cognite/neat/data-model/verified/conceptual/neat_space/NeatInferredDataModel/v1/ControlArea</t>
+  </si>
+  <si>
+    <t>http://purl.org/cognite/neat/data-model/verified/conceptual/neat_space/NeatInferredDataModel/v1/ControlAreaGeneratingUnit</t>
+  </si>
+  <si>
+    <t>http://purl.org/cognite/neat/data-model/verified/conceptual/neat_space/NeatInferredDataModel/v1/CurrentLimit</t>
+  </si>
+  <si>
+    <t>http://purl.org/cognite/neat/data-model/verified/conceptual/neat_space/NeatInferredDataModel/v1/Disconnector</t>
+  </si>
+  <si>
+    <t>http://purl.org/cognite/neat/data-model/verified/conceptual/neat_space/NeatInferredDataModel/v1/GeneratingUnit</t>
+  </si>
+  <si>
+    <t>http://purl.org/cognite/neat/data-model/verified/conceptual/neat_space/NeatInferredDataModel/v1/GeographicalRegion</t>
+  </si>
+  <si>
+    <t>http://purl.org/cognite/neat/data-model/verified/conceptual/neat_space/NeatInferredDataModel/v1/Line</t>
+  </si>
+  <si>
+    <t>http://purl.org/cognite/neat/data-model/verified/conceptual/neat_space/NeatInferredDataModel/v1/LinearShuntCompensator</t>
+  </si>
+  <si>
+    <t>http://purl.org/cognite/neat/data-model/verified/conceptual/neat_space/NeatInferredDataModel/v1/LoadArea</t>
+  </si>
+  <si>
+    <t>http://purl.org/cognite/neat/data-model/verified/conceptual/neat_space/NeatInferredDataModel/v1/LoadResponseCharacteristic</t>
+  </si>
+  <si>
+    <t>http://purl.org/cognite/neat/data-model/verified/conceptual/neat_space/NeatInferredDataModel/v1/MeasurementValueSource</t>
+  </si>
+  <si>
+    <t>http://purl.org/cognite/neat/data-model/verified/conceptual/neat_space/NeatInferredDataModel/v1/NonConformLoad</t>
+  </si>
+  <si>
+    <t>http://purl.org/cognite/neat/data-model/verified/conceptual/neat_space/NeatInferredDataModel/v1/NonConformLoadGroup</t>
+  </si>
+  <si>
+    <t>http://purl.org/cognite/neat/data-model/verified/conceptual/neat_space/NeatInferredDataModel/v1/OperatingParticipant</t>
+  </si>
+  <si>
+    <t>http://purl.org/cognite/neat/data-model/verified/conceptual/neat_space/NeatInferredDataModel/v1/OperatingShare</t>
+  </si>
+  <si>
+    <t>http://purl.org/cognite/neat/data-model/verified/conceptual/neat_space/NeatInferredDataModel/v1/OperationalLimitSet</t>
+  </si>
+  <si>
+    <t>http://purl.org/cognite/neat/data-model/verified/conceptual/neat_space/NeatInferredDataModel/v1/OperationalLimitType</t>
+  </si>
+  <si>
+    <t>http://purl.org/cognite/neat/data-model/verified/conceptual/neat_space/NeatInferredDataModel/v1/PowerTransformer</t>
+  </si>
+  <si>
+    <t>http://purl.org/cognite/neat/data-model/verified/conceptual/neat_space/NeatInferredDataModel/v1/PowerTransformerEnd</t>
+  </si>
+  <si>
+    <t>http://purl.org/cognite/neat/data-model/verified/conceptual/neat_space/NeatInferredDataModel/v1/RatioTapChanger</t>
+  </si>
+  <si>
+    <t>http://purl.org/cognite/neat/data-model/verified/conceptual/neat_space/NeatInferredDataModel/v1/RegulatingControl</t>
+  </si>
+  <si>
+    <t>http://purl.org/cognite/neat/data-model/verified/conceptual/neat_space/NeatInferredDataModel/v1/SubGeographicalRegion</t>
+  </si>
+  <si>
+    <t>http://purl.org/cognite/neat/data-model/verified/conceptual/neat_space/NeatInferredDataModel/v1/SubLoadArea</t>
+  </si>
+  <si>
+    <t>http://purl.org/cognite/neat/data-model/verified/conceptual/neat_space/NeatInferredDataModel/v1/Substation</t>
+  </si>
+  <si>
+    <t>http://purl.org/cognite/neat/data-model/verified/conceptual/neat_space/NeatInferredDataModel/v1/SynchronousMachine</t>
+  </si>
+  <si>
+    <t>http://purl.org/cognite/neat/data-model/verified/conceptual/neat_space/NeatInferredDataModel/v1/TapChangerControl</t>
+  </si>
+  <si>
+    <t>http://purl.org/cognite/neat/data-model/verified/conceptual/neat_space/NeatInferredDataModel/v1/Terminal</t>
+  </si>
+  <si>
+    <t>http://purl.org/cognite/neat/data-model/verified/conceptual/neat_space/NeatInferredDataModel/v1/VoltageLevel</t>
+  </si>
+  <si>
+    <t>http://purl.org/cognite/neat/data-model/verified/conceptual/neat_space/NeatInferredDataModel/v1/VoltageLimit</t>
+  </si>
+  <si>
+    <t>http://purl.org/cognite/neat/data-model/verified/conceptual/neat_space/NeatInferredDataModel/v1/Gate</t>
+  </si>
+  <si>
+    <t>http://purl.org/cognite/neat/data-model/verified/conceptual/neat_space/NeatInferredDataModel/v1/PinEquipment</t>
+  </si>
+  <si>
+    <t>http://purl.org/cognite/neat/data-model/verified/conceptual/neat_space/NeatInferredDataModel/v1/PinGate</t>
+  </si>
+  <si>
+    <t>http://purl.org/cognite/neat/data-model/verified/conceptual/neat_space/NeatInferredDataModel/v1/PinTerminal</t>
+  </si>
+  <si>
+    <t>http://purl.org/cognite/neat/data-model/verified/conceptual/neat_space/NeatInferredDataModel/v1/ProtectiveActionAdjustment</t>
+  </si>
+  <si>
+    <t>http://purl.org/cognite/neat/data-model/verified/conceptual/neat_space/NeatInferredDataModel/v1/ProtectiveActionCollection</t>
+  </si>
+  <si>
+    <t>http://purl.org/cognite/neat/data-model/verified/conceptual/neat_space/NeatInferredDataModel/v1/ProtectiveActionEquipment</t>
+  </si>
+  <si>
+    <t>http://purl.org/cognite/neat/data-model/verified/conceptual/neat_space/NeatInferredDataModel/v1/RemedialActionScheme</t>
+  </si>
+  <si>
+    <t>http://purl.org/cognite/neat/data-model/verified/conceptual/neat_space/NeatInferredDataModel/v1/Stage</t>
+  </si>
+  <si>
+    <t>http://purl.org/cognite/neat/data-model/verified/conceptual/neat_space/NeatInferredDataModel/v1/StageTrigger</t>
+  </si>
+  <si>
+    <t>http://purl.org/cognite/neat/data-model/verified/conceptual/neat_space/NeatInferredDataModel/v1/FullModel</t>
+  </si>
+  <si>
+    <t>http://purl.org/cognite/neat/data-model/verified/conceptual/neat_space/NeatInferredDataModel/v1/ScheduleResourceGeneration</t>
   </si>
 </sst>
 </file>
@@ -446,7 +446,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd\ h:mm:ss"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -458,16 +458,25 @@
       <b/>
       <sz val="12"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="20"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="14"/>
       <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF839496"/>
+      <name val="Menlo"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="5">
@@ -520,7 +529,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -531,6 +540,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -839,13 +849,13 @@
       <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="13" customWidth="1"/>
     <col min="2" max="2" width="70" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -853,23 +863,23 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
@@ -877,31 +887,31 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B5" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B6" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B7" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>9</v>
       </c>
@@ -909,7 +919,7 @@
         <v>45728.612507300008</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>10</v>
       </c>
@@ -917,17 +927,17 @@
         <v>45728.612507300008</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="12" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>13</v>
       </c>
@@ -941,15 +951,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:L334"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="26.44140625" customWidth="1"/>
-    <col min="2" max="2" width="45.44140625" customWidth="1"/>
+    <col min="1" max="1" width="26.5" customWidth="1"/>
+    <col min="2" max="2" width="45.5" customWidth="1"/>
     <col min="3" max="4" width="13" customWidth="1"/>
     <col min="5" max="5" width="70" customWidth="1"/>
     <col min="6" max="8" width="13" customWidth="1"/>
@@ -958,7 +968,7 @@
     <col min="12" max="12" width="70" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="25.8" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:12" ht="26" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>14</v>
       </c>
@@ -974,7 +984,7 @@
       <c r="K1" s="4"/>
       <c r="L1" s="4"/>
     </row>
-    <row r="2" spans="1:12" ht="18" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:12" ht="19" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>15</v>
       </c>
@@ -1012,7 +1022,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3" s="6"/>
       <c r="B3" s="6"/>
       <c r="C3" s="6"/>
@@ -1026,7 +1036,7 @@
       <c r="K3" s="6"/>
       <c r="L3" s="6"/>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4" s="6"/>
       <c r="B4" s="6"/>
       <c r="C4" s="6"/>
@@ -1040,7 +1050,7 @@
       <c r="K4" s="6"/>
       <c r="L4" s="6"/>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5" s="6"/>
       <c r="B5" s="6"/>
       <c r="C5" s="6"/>
@@ -1054,7 +1064,7 @@
       <c r="K5" s="6"/>
       <c r="L5" s="6"/>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A6" s="6"/>
       <c r="B6" s="6"/>
       <c r="C6" s="6"/>
@@ -1068,7 +1078,7 @@
       <c r="K6" s="6"/>
       <c r="L6" s="6"/>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A7" s="7"/>
       <c r="B7" s="7"/>
       <c r="C7" s="7"/>
@@ -1082,7 +1092,7 @@
       <c r="K7" s="7"/>
       <c r="L7" s="7"/>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A8" s="7"/>
       <c r="B8" s="7"/>
       <c r="C8" s="7"/>
@@ -1096,7 +1106,7 @@
       <c r="K8" s="7"/>
       <c r="L8" s="7"/>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A9" s="7"/>
       <c r="B9" s="7"/>
       <c r="C9" s="7"/>
@@ -1110,7 +1120,7 @@
       <c r="K9" s="7"/>
       <c r="L9" s="7"/>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A10" s="7"/>
       <c r="B10" s="7"/>
       <c r="C10" s="7"/>
@@ -1124,7 +1134,7 @@
       <c r="K10" s="7"/>
       <c r="L10" s="7"/>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A11" s="6"/>
       <c r="B11" s="6"/>
       <c r="C11" s="6"/>
@@ -1138,7 +1148,7 @@
       <c r="K11" s="6"/>
       <c r="L11" s="6"/>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
@@ -1152,7 +1162,7 @@
       <c r="K12" s="6"/>
       <c r="L12" s="6"/>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A13" s="6"/>
       <c r="B13" s="6"/>
       <c r="C13" s="6"/>
@@ -1166,7 +1176,7 @@
       <c r="K13" s="6"/>
       <c r="L13" s="6"/>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A14" s="6"/>
       <c r="B14" s="6"/>
       <c r="C14" s="6"/>
@@ -1180,7 +1190,7 @@
       <c r="K14" s="6"/>
       <c r="L14" s="6"/>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A15" s="6"/>
       <c r="B15" s="6"/>
       <c r="C15" s="6"/>
@@ -1194,7 +1204,7 @@
       <c r="K15" s="6"/>
       <c r="L15" s="6"/>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A16" s="7"/>
       <c r="B16" s="7"/>
       <c r="C16" s="7"/>
@@ -1208,7 +1218,7 @@
       <c r="K16" s="7"/>
       <c r="L16" s="7"/>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A17" s="7"/>
       <c r="B17" s="7"/>
       <c r="C17" s="7"/>
@@ -1222,7 +1232,7 @@
       <c r="K17" s="7"/>
       <c r="L17" s="7"/>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A18" s="7"/>
       <c r="B18" s="7"/>
       <c r="C18" s="7"/>
@@ -1236,7 +1246,7 @@
       <c r="K18" s="7"/>
       <c r="L18" s="7"/>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A19" s="7"/>
       <c r="B19" s="7"/>
       <c r="C19" s="7"/>
@@ -1250,7 +1260,7 @@
       <c r="K19" s="7"/>
       <c r="L19" s="7"/>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A20" s="6"/>
       <c r="B20" s="6"/>
       <c r="C20" s="6"/>
@@ -1264,7 +1274,7 @@
       <c r="K20" s="6"/>
       <c r="L20" s="6"/>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A21" s="6"/>
       <c r="B21" s="6"/>
       <c r="C21" s="6"/>
@@ -1278,7 +1288,7 @@
       <c r="K21" s="6"/>
       <c r="L21" s="6"/>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A22" s="7"/>
       <c r="B22" s="7"/>
       <c r="C22" s="7"/>
@@ -1292,7 +1302,7 @@
       <c r="K22" s="7"/>
       <c r="L22" s="7"/>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A23" s="7"/>
       <c r="B23" s="7"/>
       <c r="C23" s="7"/>
@@ -1306,7 +1316,7 @@
       <c r="K23" s="7"/>
       <c r="L23" s="7"/>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A24" s="7"/>
       <c r="B24" s="7"/>
       <c r="C24" s="7"/>
@@ -1320,7 +1330,7 @@
       <c r="K24" s="7"/>
       <c r="L24" s="7"/>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A25" s="6"/>
       <c r="B25" s="6"/>
       <c r="C25" s="6"/>
@@ -1334,7 +1344,7 @@
       <c r="K25" s="6"/>
       <c r="L25" s="6"/>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A26" s="6"/>
       <c r="B26" s="6"/>
       <c r="C26" s="6"/>
@@ -1348,7 +1358,7 @@
       <c r="K26" s="6"/>
       <c r="L26" s="6"/>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A27" s="6"/>
       <c r="B27" s="6"/>
       <c r="C27" s="6"/>
@@ -1362,7 +1372,7 @@
       <c r="K27" s="6"/>
       <c r="L27" s="6"/>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A28" s="6"/>
       <c r="B28" s="6"/>
       <c r="C28" s="6"/>
@@ -1376,7 +1386,7 @@
       <c r="K28" s="6"/>
       <c r="L28" s="6"/>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A29" s="6"/>
       <c r="B29" s="6"/>
       <c r="C29" s="6"/>
@@ -1390,7 +1400,7 @@
       <c r="K29" s="6"/>
       <c r="L29" s="6"/>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A30" s="6"/>
       <c r="B30" s="6"/>
       <c r="C30" s="6"/>
@@ -1404,7 +1414,7 @@
       <c r="K30" s="6"/>
       <c r="L30" s="6"/>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A31" s="6"/>
       <c r="B31" s="6"/>
       <c r="C31" s="6"/>
@@ -1418,7 +1428,7 @@
       <c r="K31" s="6"/>
       <c r="L31" s="6"/>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A32" s="6"/>
       <c r="B32" s="6"/>
       <c r="C32" s="6"/>
@@ -1432,7 +1442,7 @@
       <c r="K32" s="6"/>
       <c r="L32" s="6"/>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A33" s="6"/>
       <c r="B33" s="6"/>
       <c r="C33" s="6"/>
@@ -1446,7 +1456,7 @@
       <c r="K33" s="6"/>
       <c r="L33" s="6"/>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A34" s="6"/>
       <c r="B34" s="6"/>
       <c r="C34" s="6"/>
@@ -1460,7 +1470,7 @@
       <c r="K34" s="6"/>
       <c r="L34" s="6"/>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A35" s="6"/>
       <c r="B35" s="6"/>
       <c r="C35" s="6"/>
@@ -1474,7 +1484,7 @@
       <c r="K35" s="6"/>
       <c r="L35" s="6"/>
     </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A36" s="6"/>
       <c r="B36" s="6"/>
       <c r="C36" s="6"/>
@@ -1488,7 +1498,7 @@
       <c r="K36" s="6"/>
       <c r="L36" s="6"/>
     </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A37" s="7"/>
       <c r="B37" s="7"/>
       <c r="C37" s="7"/>
@@ -1502,7 +1512,7 @@
       <c r="K37" s="7"/>
       <c r="L37" s="7"/>
     </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A38" s="7"/>
       <c r="B38" s="7"/>
       <c r="C38" s="7"/>
@@ -1516,7 +1526,7 @@
       <c r="K38" s="7"/>
       <c r="L38" s="7"/>
     </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A39" s="7"/>
       <c r="B39" s="7"/>
       <c r="C39" s="7"/>
@@ -1530,7 +1540,7 @@
       <c r="K39" s="7"/>
       <c r="L39" s="7"/>
     </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A40" s="7"/>
       <c r="B40" s="7"/>
       <c r="C40" s="7"/>
@@ -1544,7 +1554,7 @@
       <c r="K40" s="7"/>
       <c r="L40" s="7"/>
     </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A41" s="7"/>
       <c r="B41" s="7"/>
       <c r="C41" s="7"/>
@@ -1558,7 +1568,7 @@
       <c r="K41" s="7"/>
       <c r="L41" s="7"/>
     </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A42" s="6"/>
       <c r="B42" s="6"/>
       <c r="C42" s="6"/>
@@ -1572,7 +1582,7 @@
       <c r="K42" s="6"/>
       <c r="L42" s="6"/>
     </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A43" s="6"/>
       <c r="B43" s="6"/>
       <c r="C43" s="6"/>
@@ -1586,7 +1596,7 @@
       <c r="K43" s="6"/>
       <c r="L43" s="6"/>
     </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A44" s="6"/>
       <c r="B44" s="6"/>
       <c r="C44" s="6"/>
@@ -1600,7 +1610,7 @@
       <c r="K44" s="6"/>
       <c r="L44" s="6"/>
     </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A45" s="6"/>
       <c r="B45" s="6"/>
       <c r="C45" s="6"/>
@@ -1614,7 +1624,7 @@
       <c r="K45" s="6"/>
       <c r="L45" s="6"/>
     </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A46" s="6"/>
       <c r="B46" s="6"/>
       <c r="C46" s="6"/>
@@ -1628,7 +1638,7 @@
       <c r="K46" s="6"/>
       <c r="L46" s="6"/>
     </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A47" s="6"/>
       <c r="B47" s="6"/>
       <c r="C47" s="6"/>
@@ -1642,7 +1652,7 @@
       <c r="K47" s="6"/>
       <c r="L47" s="6"/>
     </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A48" s="6"/>
       <c r="B48" s="6"/>
       <c r="C48" s="6"/>
@@ -1656,7 +1666,7 @@
       <c r="K48" s="6"/>
       <c r="L48" s="6"/>
     </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A49" s="7"/>
       <c r="B49" s="7"/>
       <c r="C49" s="7"/>
@@ -1670,7 +1680,7 @@
       <c r="K49" s="7"/>
       <c r="L49" s="7"/>
     </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A50" s="7"/>
       <c r="B50" s="7"/>
       <c r="C50" s="7"/>
@@ -1684,7 +1694,7 @@
       <c r="K50" s="7"/>
       <c r="L50" s="7"/>
     </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A51" s="7"/>
       <c r="B51" s="7"/>
       <c r="C51" s="7"/>
@@ -1698,7 +1708,7 @@
       <c r="K51" s="7"/>
       <c r="L51" s="7"/>
     </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A52" s="7"/>
       <c r="B52" s="7"/>
       <c r="C52" s="7"/>
@@ -1712,7 +1722,7 @@
       <c r="K52" s="7"/>
       <c r="L52" s="7"/>
     </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A53" s="7"/>
       <c r="B53" s="7"/>
       <c r="C53" s="7"/>
@@ -1726,7 +1736,7 @@
       <c r="K53" s="7"/>
       <c r="L53" s="7"/>
     </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A54" s="6"/>
       <c r="B54" s="6"/>
       <c r="C54" s="6"/>
@@ -1740,7 +1750,7 @@
       <c r="K54" s="6"/>
       <c r="L54" s="6"/>
     </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A55" s="7"/>
       <c r="B55" s="7"/>
       <c r="C55" s="7"/>
@@ -1754,7 +1764,7 @@
       <c r="K55" s="7"/>
       <c r="L55" s="7"/>
     </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A56" s="7"/>
       <c r="B56" s="7"/>
       <c r="C56" s="7"/>
@@ -1768,7 +1778,7 @@
       <c r="K56" s="7"/>
       <c r="L56" s="7"/>
     </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A57" s="6"/>
       <c r="B57" s="6"/>
       <c r="C57" s="6"/>
@@ -1782,7 +1792,7 @@
       <c r="K57" s="6"/>
       <c r="L57" s="6"/>
     </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A58" s="6"/>
       <c r="B58" s="6"/>
       <c r="C58" s="6"/>
@@ -1796,7 +1806,7 @@
       <c r="K58" s="6"/>
       <c r="L58" s="6"/>
     </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A59" s="6"/>
       <c r="B59" s="6"/>
       <c r="C59" s="6"/>
@@ -1810,7 +1820,7 @@
       <c r="K59" s="6"/>
       <c r="L59" s="6"/>
     </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A60" s="7"/>
       <c r="B60" s="7"/>
       <c r="C60" s="7"/>
@@ -1824,7 +1834,7 @@
       <c r="K60" s="7"/>
       <c r="L60" s="7"/>
     </row>
-    <row r="61" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A61" s="7"/>
       <c r="B61" s="7"/>
       <c r="C61" s="7"/>
@@ -1838,7 +1848,7 @@
       <c r="K61" s="7"/>
       <c r="L61" s="7"/>
     </row>
-    <row r="62" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A62" s="7"/>
       <c r="B62" s="7"/>
       <c r="C62" s="7"/>
@@ -1852,7 +1862,7 @@
       <c r="K62" s="7"/>
       <c r="L62" s="7"/>
     </row>
-    <row r="63" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A63" s="7"/>
       <c r="B63" s="7"/>
       <c r="C63" s="7"/>
@@ -1866,7 +1876,7 @@
       <c r="K63" s="7"/>
       <c r="L63" s="7"/>
     </row>
-    <row r="64" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A64" s="7"/>
       <c r="B64" s="7"/>
       <c r="C64" s="7"/>
@@ -1880,7 +1890,7 @@
       <c r="K64" s="7"/>
       <c r="L64" s="7"/>
     </row>
-    <row r="65" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A65" s="7"/>
       <c r="B65" s="7"/>
       <c r="C65" s="7"/>
@@ -1894,7 +1904,7 @@
       <c r="K65" s="7"/>
       <c r="L65" s="7"/>
     </row>
-    <row r="66" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A66" s="7"/>
       <c r="B66" s="7"/>
       <c r="C66" s="7"/>
@@ -1908,7 +1918,7 @@
       <c r="K66" s="7"/>
       <c r="L66" s="7"/>
     </row>
-    <row r="67" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A67" s="6"/>
       <c r="B67" s="6"/>
       <c r="C67" s="6"/>
@@ -1922,7 +1932,7 @@
       <c r="K67" s="6"/>
       <c r="L67" s="6"/>
     </row>
-    <row r="68" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A68" s="6"/>
       <c r="B68" s="6"/>
       <c r="C68" s="6"/>
@@ -1936,7 +1946,7 @@
       <c r="K68" s="6"/>
       <c r="L68" s="6"/>
     </row>
-    <row r="69" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A69" s="6"/>
       <c r="B69" s="6"/>
       <c r="C69" s="6"/>
@@ -1950,7 +1960,7 @@
       <c r="K69" s="6"/>
       <c r="L69" s="6"/>
     </row>
-    <row r="70" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A70" s="6"/>
       <c r="B70" s="6"/>
       <c r="C70" s="6"/>
@@ -1964,7 +1974,7 @@
       <c r="K70" s="6"/>
       <c r="L70" s="6"/>
     </row>
-    <row r="71" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A71" s="7"/>
       <c r="B71" s="7"/>
       <c r="C71" s="7"/>
@@ -1978,7 +1988,7 @@
       <c r="K71" s="7"/>
       <c r="L71" s="7"/>
     </row>
-    <row r="72" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A72" s="7"/>
       <c r="B72" s="7"/>
       <c r="C72" s="7"/>
@@ -1992,7 +2002,7 @@
       <c r="K72" s="7"/>
       <c r="L72" s="7"/>
     </row>
-    <row r="73" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A73" s="7"/>
       <c r="B73" s="7"/>
       <c r="C73" s="7"/>
@@ -2006,7 +2016,7 @@
       <c r="K73" s="7"/>
       <c r="L73" s="7"/>
     </row>
-    <row r="74" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A74" s="7"/>
       <c r="B74" s="7"/>
       <c r="C74" s="7"/>
@@ -2020,7 +2030,7 @@
       <c r="K74" s="7"/>
       <c r="L74" s="7"/>
     </row>
-    <row r="75" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A75" s="7"/>
       <c r="B75" s="7"/>
       <c r="C75" s="7"/>
@@ -2034,7 +2044,7 @@
       <c r="K75" s="7"/>
       <c r="L75" s="7"/>
     </row>
-    <row r="76" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A76" s="7"/>
       <c r="B76" s="7"/>
       <c r="C76" s="7"/>
@@ -2048,7 +2058,7 @@
       <c r="K76" s="7"/>
       <c r="L76" s="7"/>
     </row>
-    <row r="77" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A77" s="7"/>
       <c r="B77" s="7"/>
       <c r="C77" s="7"/>
@@ -2062,7 +2072,7 @@
       <c r="K77" s="7"/>
       <c r="L77" s="7"/>
     </row>
-    <row r="78" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A78" s="7"/>
       <c r="B78" s="7"/>
       <c r="C78" s="7"/>
@@ -2076,7 +2086,7 @@
       <c r="K78" s="7"/>
       <c r="L78" s="7"/>
     </row>
-    <row r="79" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A79" s="7"/>
       <c r="B79" s="7"/>
       <c r="C79" s="7"/>
@@ -2090,7 +2100,7 @@
       <c r="K79" s="7"/>
       <c r="L79" s="7"/>
     </row>
-    <row r="80" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A80" s="7"/>
       <c r="B80" s="7"/>
       <c r="C80" s="7"/>
@@ -2104,7 +2114,7 @@
       <c r="K80" s="7"/>
       <c r="L80" s="7"/>
     </row>
-    <row r="81" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A81" s="7"/>
       <c r="B81" s="7"/>
       <c r="C81" s="7"/>
@@ -2118,7 +2128,7 @@
       <c r="K81" s="7"/>
       <c r="L81" s="7"/>
     </row>
-    <row r="82" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A82" s="6"/>
       <c r="B82" s="6"/>
       <c r="C82" s="6"/>
@@ -2132,7 +2142,7 @@
       <c r="K82" s="6"/>
       <c r="L82" s="6"/>
     </row>
-    <row r="83" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A83" s="6"/>
       <c r="B83" s="6"/>
       <c r="C83" s="6"/>
@@ -2146,7 +2156,7 @@
       <c r="K83" s="6"/>
       <c r="L83" s="6"/>
     </row>
-    <row r="84" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A84" s="6"/>
       <c r="B84" s="6"/>
       <c r="C84" s="6"/>
@@ -2160,7 +2170,7 @@
       <c r="K84" s="6"/>
       <c r="L84" s="6"/>
     </row>
-    <row r="85" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A85" s="7"/>
       <c r="B85" s="7"/>
       <c r="C85" s="7"/>
@@ -2174,7 +2184,7 @@
       <c r="K85" s="7"/>
       <c r="L85" s="7"/>
     </row>
-    <row r="86" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A86" s="7"/>
       <c r="B86" s="7"/>
       <c r="C86" s="7"/>
@@ -2188,7 +2198,7 @@
       <c r="K86" s="7"/>
       <c r="L86" s="7"/>
     </row>
-    <row r="87" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A87" s="6"/>
       <c r="B87" s="6"/>
       <c r="C87" s="6"/>
@@ -2202,7 +2212,7 @@
       <c r="K87" s="6"/>
       <c r="L87" s="6"/>
     </row>
-    <row r="88" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A88" s="6"/>
       <c r="B88" s="6"/>
       <c r="C88" s="6"/>
@@ -2216,7 +2226,7 @@
       <c r="K88" s="6"/>
       <c r="L88" s="6"/>
     </row>
-    <row r="89" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A89" s="6"/>
       <c r="B89" s="6"/>
       <c r="C89" s="6"/>
@@ -2230,7 +2240,7 @@
       <c r="K89" s="6"/>
       <c r="L89" s="6"/>
     </row>
-    <row r="90" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A90" s="7"/>
       <c r="B90" s="7"/>
       <c r="C90" s="7"/>
@@ -2244,7 +2254,7 @@
       <c r="K90" s="7"/>
       <c r="L90" s="7"/>
     </row>
-    <row r="91" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A91" s="7"/>
       <c r="B91" s="7"/>
       <c r="C91" s="7"/>
@@ -2258,7 +2268,7 @@
       <c r="K91" s="7"/>
       <c r="L91" s="7"/>
     </row>
-    <row r="92" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A92" s="7"/>
       <c r="B92" s="7"/>
       <c r="C92" s="7"/>
@@ -2272,7 +2282,7 @@
       <c r="K92" s="7"/>
       <c r="L92" s="7"/>
     </row>
-    <row r="93" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A93" s="7"/>
       <c r="B93" s="7"/>
       <c r="C93" s="7"/>
@@ -2286,7 +2296,7 @@
       <c r="K93" s="7"/>
       <c r="L93" s="7"/>
     </row>
-    <row r="94" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A94" s="7"/>
       <c r="B94" s="7"/>
       <c r="C94" s="7"/>
@@ -2300,7 +2310,7 @@
       <c r="K94" s="7"/>
       <c r="L94" s="7"/>
     </row>
-    <row r="95" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A95" s="6"/>
       <c r="B95" s="6"/>
       <c r="C95" s="6"/>
@@ -2314,7 +2324,7 @@
       <c r="K95" s="6"/>
       <c r="L95" s="6"/>
     </row>
-    <row r="96" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A96" s="6"/>
       <c r="B96" s="6"/>
       <c r="C96" s="6"/>
@@ -2328,7 +2338,7 @@
       <c r="K96" s="6"/>
       <c r="L96" s="6"/>
     </row>
-    <row r="97" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A97" s="6"/>
       <c r="B97" s="6"/>
       <c r="C97" s="6"/>
@@ -2342,7 +2352,7 @@
       <c r="K97" s="6"/>
       <c r="L97" s="6"/>
     </row>
-    <row r="98" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A98" s="6"/>
       <c r="B98" s="6"/>
       <c r="C98" s="6"/>
@@ -2356,7 +2366,7 @@
       <c r="K98" s="6"/>
       <c r="L98" s="6"/>
     </row>
-    <row r="99" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A99" s="6"/>
       <c r="B99" s="6"/>
       <c r="C99" s="6"/>
@@ -2370,7 +2380,7 @@
       <c r="K99" s="6"/>
       <c r="L99" s="6"/>
     </row>
-    <row r="100" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A100" s="6"/>
       <c r="B100" s="6"/>
       <c r="C100" s="6"/>
@@ -2384,7 +2394,7 @@
       <c r="K100" s="6"/>
       <c r="L100" s="6"/>
     </row>
-    <row r="101" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A101" s="7"/>
       <c r="B101" s="7"/>
       <c r="C101" s="7"/>
@@ -2398,7 +2408,7 @@
       <c r="K101" s="7"/>
       <c r="L101" s="7"/>
     </row>
-    <row r="102" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A102" s="7"/>
       <c r="B102" s="7"/>
       <c r="C102" s="7"/>
@@ -2412,7 +2422,7 @@
       <c r="K102" s="7"/>
       <c r="L102" s="7"/>
     </row>
-    <row r="103" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A103" s="7"/>
       <c r="B103" s="7"/>
       <c r="C103" s="7"/>
@@ -2426,7 +2436,7 @@
       <c r="K103" s="7"/>
       <c r="L103" s="7"/>
     </row>
-    <row r="104" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A104" s="7"/>
       <c r="B104" s="7"/>
       <c r="C104" s="7"/>
@@ -2440,7 +2450,7 @@
       <c r="K104" s="7"/>
       <c r="L104" s="7"/>
     </row>
-    <row r="105" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A105" s="7"/>
       <c r="B105" s="7"/>
       <c r="C105" s="7"/>
@@ -2454,7 +2464,7 @@
       <c r="K105" s="7"/>
       <c r="L105" s="7"/>
     </row>
-    <row r="106" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A106" s="7"/>
       <c r="B106" s="7"/>
       <c r="C106" s="7"/>
@@ -2468,7 +2478,7 @@
       <c r="K106" s="7"/>
       <c r="L106" s="7"/>
     </row>
-    <row r="107" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A107" s="7"/>
       <c r="B107" s="7"/>
       <c r="C107" s="7"/>
@@ -2482,7 +2492,7 @@
       <c r="K107" s="7"/>
       <c r="L107" s="7"/>
     </row>
-    <row r="108" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A108" s="6"/>
       <c r="B108" s="6"/>
       <c r="C108" s="6"/>
@@ -2496,7 +2506,7 @@
       <c r="K108" s="6"/>
       <c r="L108" s="6"/>
     </row>
-    <row r="109" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A109" s="6"/>
       <c r="B109" s="6"/>
       <c r="C109" s="6"/>
@@ -2510,7 +2520,7 @@
       <c r="K109" s="6"/>
       <c r="L109" s="6"/>
     </row>
-    <row r="110" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A110" s="6"/>
       <c r="B110" s="6"/>
       <c r="C110" s="6"/>
@@ -2524,7 +2534,7 @@
       <c r="K110" s="6"/>
       <c r="L110" s="6"/>
     </row>
-    <row r="111" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A111" s="6"/>
       <c r="B111" s="6"/>
       <c r="C111" s="6"/>
@@ -2538,7 +2548,7 @@
       <c r="K111" s="6"/>
       <c r="L111" s="6"/>
     </row>
-    <row r="112" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A112" s="6"/>
       <c r="B112" s="6"/>
       <c r="C112" s="6"/>
@@ -2552,7 +2562,7 @@
       <c r="K112" s="6"/>
       <c r="L112" s="6"/>
     </row>
-    <row r="113" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A113" s="6"/>
       <c r="B113" s="6"/>
       <c r="C113" s="6"/>
@@ -2566,7 +2576,7 @@
       <c r="K113" s="6"/>
       <c r="L113" s="6"/>
     </row>
-    <row r="114" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A114" s="6"/>
       <c r="B114" s="6"/>
       <c r="C114" s="6"/>
@@ -2580,7 +2590,7 @@
       <c r="K114" s="6"/>
       <c r="L114" s="6"/>
     </row>
-    <row r="115" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A115" s="6"/>
       <c r="B115" s="6"/>
       <c r="C115" s="6"/>
@@ -2594,7 +2604,7 @@
       <c r="K115" s="6"/>
       <c r="L115" s="6"/>
     </row>
-    <row r="116" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A116" s="6"/>
       <c r="B116" s="6"/>
       <c r="C116" s="6"/>
@@ -2608,7 +2618,7 @@
       <c r="K116" s="6"/>
       <c r="L116" s="6"/>
     </row>
-    <row r="117" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A117" s="6"/>
       <c r="B117" s="6"/>
       <c r="C117" s="6"/>
@@ -2622,7 +2632,7 @@
       <c r="K117" s="6"/>
       <c r="L117" s="6"/>
     </row>
-    <row r="118" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A118" s="6"/>
       <c r="B118" s="6"/>
       <c r="C118" s="6"/>
@@ -2636,7 +2646,7 @@
       <c r="K118" s="6"/>
       <c r="L118" s="6"/>
     </row>
-    <row r="119" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A119" s="6"/>
       <c r="B119" s="6"/>
       <c r="C119" s="6"/>
@@ -2650,7 +2660,7 @@
       <c r="K119" s="6"/>
       <c r="L119" s="6"/>
     </row>
-    <row r="120" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A120" s="6"/>
       <c r="B120" s="6"/>
       <c r="C120" s="6"/>
@@ -2664,7 +2674,7 @@
       <c r="K120" s="6"/>
       <c r="L120" s="6"/>
     </row>
-    <row r="121" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A121" s="6"/>
       <c r="B121" s="6"/>
       <c r="C121" s="6"/>
@@ -2678,7 +2688,7 @@
       <c r="K121" s="6"/>
       <c r="L121" s="6"/>
     </row>
-    <row r="122" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A122" s="6"/>
       <c r="B122" s="6"/>
       <c r="C122" s="6"/>
@@ -2692,7 +2702,7 @@
       <c r="K122" s="6"/>
       <c r="L122" s="6"/>
     </row>
-    <row r="123" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A123" s="6"/>
       <c r="B123" s="6"/>
       <c r="C123" s="6"/>
@@ -2706,7 +2716,7 @@
       <c r="K123" s="6"/>
       <c r="L123" s="6"/>
     </row>
-    <row r="124" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A124" s="6"/>
       <c r="B124" s="6"/>
       <c r="C124" s="6"/>
@@ -2720,7 +2730,7 @@
       <c r="K124" s="6"/>
       <c r="L124" s="6"/>
     </row>
-    <row r="125" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A125" s="6"/>
       <c r="B125" s="6"/>
       <c r="C125" s="6"/>
@@ -2734,7 +2744,7 @@
       <c r="K125" s="6"/>
       <c r="L125" s="6"/>
     </row>
-    <row r="126" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A126" s="6"/>
       <c r="B126" s="6"/>
       <c r="C126" s="6"/>
@@ -2748,7 +2758,7 @@
       <c r="K126" s="6"/>
       <c r="L126" s="6"/>
     </row>
-    <row r="127" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A127" s="6"/>
       <c r="B127" s="6"/>
       <c r="C127" s="6"/>
@@ -2762,7 +2772,7 @@
       <c r="K127" s="6"/>
       <c r="L127" s="6"/>
     </row>
-    <row r="128" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A128" s="6"/>
       <c r="B128" s="6"/>
       <c r="C128" s="6"/>
@@ -2776,7 +2786,7 @@
       <c r="K128" s="6"/>
       <c r="L128" s="6"/>
     </row>
-    <row r="129" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A129" s="6"/>
       <c r="B129" s="6"/>
       <c r="C129" s="6"/>
@@ -2790,7 +2800,7 @@
       <c r="K129" s="6"/>
       <c r="L129" s="6"/>
     </row>
-    <row r="130" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A130" s="7"/>
       <c r="B130" s="7"/>
       <c r="C130" s="7"/>
@@ -2804,7 +2814,7 @@
       <c r="K130" s="7"/>
       <c r="L130" s="7"/>
     </row>
-    <row r="131" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A131" s="7"/>
       <c r="B131" s="7"/>
       <c r="C131" s="7"/>
@@ -2818,7 +2828,7 @@
       <c r="K131" s="7"/>
       <c r="L131" s="7"/>
     </row>
-    <row r="132" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A132" s="6"/>
       <c r="B132" s="6"/>
       <c r="C132" s="6"/>
@@ -2832,7 +2842,7 @@
       <c r="K132" s="6"/>
       <c r="L132" s="6"/>
     </row>
-    <row r="133" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A133" s="6"/>
       <c r="B133" s="6"/>
       <c r="C133" s="6"/>
@@ -2846,7 +2856,7 @@
       <c r="K133" s="6"/>
       <c r="L133" s="6"/>
     </row>
-    <row r="134" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A134" s="7"/>
       <c r="B134" s="7"/>
       <c r="C134" s="7"/>
@@ -2860,7 +2870,7 @@
       <c r="K134" s="7"/>
       <c r="L134" s="7"/>
     </row>
-    <row r="135" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A135" s="7"/>
       <c r="B135" s="7"/>
       <c r="C135" s="7"/>
@@ -2874,7 +2884,7 @@
       <c r="K135" s="7"/>
       <c r="L135" s="7"/>
     </row>
-    <row r="136" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A136" s="7"/>
       <c r="B136" s="7"/>
       <c r="C136" s="7"/>
@@ -2888,7 +2898,7 @@
       <c r="K136" s="7"/>
       <c r="L136" s="7"/>
     </row>
-    <row r="137" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A137" s="7"/>
       <c r="B137" s="7"/>
       <c r="C137" s="7"/>
@@ -2902,7 +2912,7 @@
       <c r="K137" s="7"/>
       <c r="L137" s="7"/>
     </row>
-    <row r="138" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A138" s="7"/>
       <c r="B138" s="7"/>
       <c r="C138" s="7"/>
@@ -2916,7 +2926,7 @@
       <c r="K138" s="7"/>
       <c r="L138" s="7"/>
     </row>
-    <row r="139" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A139" s="7"/>
       <c r="B139" s="7"/>
       <c r="C139" s="7"/>
@@ -2930,7 +2940,7 @@
       <c r="K139" s="7"/>
       <c r="L139" s="7"/>
     </row>
-    <row r="140" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A140" s="7"/>
       <c r="B140" s="7"/>
       <c r="C140" s="7"/>
@@ -2944,7 +2954,7 @@
       <c r="K140" s="7"/>
       <c r="L140" s="7"/>
     </row>
-    <row r="141" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A141" s="7"/>
       <c r="B141" s="7"/>
       <c r="C141" s="7"/>
@@ -2958,7 +2968,7 @@
       <c r="K141" s="7"/>
       <c r="L141" s="7"/>
     </row>
-    <row r="142" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A142" s="7"/>
       <c r="B142" s="7"/>
       <c r="C142" s="7"/>
@@ -2972,7 +2982,7 @@
       <c r="K142" s="7"/>
       <c r="L142" s="7"/>
     </row>
-    <row r="143" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A143" s="7"/>
       <c r="B143" s="7"/>
       <c r="C143" s="7"/>
@@ -2986,7 +2996,7 @@
       <c r="K143" s="7"/>
       <c r="L143" s="7"/>
     </row>
-    <row r="144" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A144" s="7"/>
       <c r="B144" s="7"/>
       <c r="C144" s="7"/>
@@ -3000,7 +3010,7 @@
       <c r="K144" s="7"/>
       <c r="L144" s="7"/>
     </row>
-    <row r="145" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A145" s="7"/>
       <c r="B145" s="7"/>
       <c r="C145" s="7"/>
@@ -3014,7 +3024,7 @@
       <c r="K145" s="7"/>
       <c r="L145" s="7"/>
     </row>
-    <row r="146" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A146" s="7"/>
       <c r="B146" s="7"/>
       <c r="C146" s="7"/>
@@ -3028,7 +3038,7 @@
       <c r="K146" s="7"/>
       <c r="L146" s="7"/>
     </row>
-    <row r="147" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A147" s="7"/>
       <c r="B147" s="7"/>
       <c r="C147" s="7"/>
@@ -3042,7 +3052,7 @@
       <c r="K147" s="7"/>
       <c r="L147" s="7"/>
     </row>
-    <row r="148" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A148" s="6"/>
       <c r="B148" s="6"/>
       <c r="C148" s="6"/>
@@ -3056,7 +3066,7 @@
       <c r="K148" s="6"/>
       <c r="L148" s="6"/>
     </row>
-    <row r="149" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A149" s="7"/>
       <c r="B149" s="7"/>
       <c r="C149" s="7"/>
@@ -3070,7 +3080,7 @@
       <c r="K149" s="7"/>
       <c r="L149" s="7"/>
     </row>
-    <row r="150" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A150" s="7"/>
       <c r="B150" s="7"/>
       <c r="C150" s="7"/>
@@ -3084,7 +3094,7 @@
       <c r="K150" s="7"/>
       <c r="L150" s="7"/>
     </row>
-    <row r="151" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A151" s="7"/>
       <c r="B151" s="7"/>
       <c r="C151" s="7"/>
@@ -3098,7 +3108,7 @@
       <c r="K151" s="7"/>
       <c r="L151" s="7"/>
     </row>
-    <row r="152" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A152" s="7"/>
       <c r="B152" s="7"/>
       <c r="C152" s="7"/>
@@ -3112,7 +3122,7 @@
       <c r="K152" s="7"/>
       <c r="L152" s="7"/>
     </row>
-    <row r="153" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A153" s="7"/>
       <c r="B153" s="7"/>
       <c r="C153" s="7"/>
@@ -3126,7 +3136,7 @@
       <c r="K153" s="7"/>
       <c r="L153" s="7"/>
     </row>
-    <row r="154" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A154" s="7"/>
       <c r="B154" s="7"/>
       <c r="C154" s="7"/>
@@ -3140,7 +3150,7 @@
       <c r="K154" s="7"/>
       <c r="L154" s="7"/>
     </row>
-    <row r="155" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A155" s="7"/>
       <c r="B155" s="7"/>
       <c r="C155" s="7"/>
@@ -3154,7 +3164,7 @@
       <c r="K155" s="7"/>
       <c r="L155" s="7"/>
     </row>
-    <row r="156" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A156" s="7"/>
       <c r="B156" s="7"/>
       <c r="C156" s="7"/>
@@ -3168,7 +3178,7 @@
       <c r="K156" s="7"/>
       <c r="L156" s="7"/>
     </row>
-    <row r="157" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A157" s="7"/>
       <c r="B157" s="7"/>
       <c r="C157" s="7"/>
@@ -3182,7 +3192,7 @@
       <c r="K157" s="7"/>
       <c r="L157" s="7"/>
     </row>
-    <row r="158" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A158" s="6"/>
       <c r="B158" s="6"/>
       <c r="C158" s="6"/>
@@ -3196,7 +3206,7 @@
       <c r="K158" s="6"/>
       <c r="L158" s="6"/>
     </row>
-    <row r="159" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A159" s="6"/>
       <c r="B159" s="6"/>
       <c r="C159" s="6"/>
@@ -3210,7 +3220,7 @@
       <c r="K159" s="6"/>
       <c r="L159" s="6"/>
     </row>
-    <row r="160" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A160" s="7"/>
       <c r="B160" s="7"/>
       <c r="C160" s="7"/>
@@ -3224,7 +3234,7 @@
       <c r="K160" s="7"/>
       <c r="L160" s="7"/>
     </row>
-    <row r="161" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A161" s="7"/>
       <c r="B161" s="7"/>
       <c r="C161" s="7"/>
@@ -3238,7 +3248,7 @@
       <c r="K161" s="7"/>
       <c r="L161" s="7"/>
     </row>
-    <row r="162" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A162" s="7"/>
       <c r="B162" s="7"/>
       <c r="C162" s="7"/>
@@ -3252,7 +3262,7 @@
       <c r="K162" s="7"/>
       <c r="L162" s="7"/>
     </row>
-    <row r="163" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A163" s="7"/>
       <c r="B163" s="7"/>
       <c r="C163" s="7"/>
@@ -3266,7 +3276,7 @@
       <c r="K163" s="7"/>
       <c r="L163" s="7"/>
     </row>
-    <row r="164" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A164" s="7"/>
       <c r="B164" s="7"/>
       <c r="C164" s="7"/>
@@ -3280,7 +3290,7 @@
       <c r="K164" s="7"/>
       <c r="L164" s="7"/>
     </row>
-    <row r="165" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A165" s="7"/>
       <c r="B165" s="7"/>
       <c r="C165" s="7"/>
@@ -3294,7 +3304,7 @@
       <c r="K165" s="7"/>
       <c r="L165" s="7"/>
     </row>
-    <row r="166" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A166" s="7"/>
       <c r="B166" s="7"/>
       <c r="C166" s="7"/>
@@ -3308,7 +3318,7 @@
       <c r="K166" s="7"/>
       <c r="L166" s="7"/>
     </row>
-    <row r="167" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A167" s="7"/>
       <c r="B167" s="7"/>
       <c r="C167" s="7"/>
@@ -3322,7 +3332,7 @@
       <c r="K167" s="7"/>
       <c r="L167" s="7"/>
     </row>
-    <row r="168" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A168" s="7"/>
       <c r="B168" s="7"/>
       <c r="C168" s="7"/>
@@ -3336,7 +3346,7 @@
       <c r="K168" s="7"/>
       <c r="L168" s="7"/>
     </row>
-    <row r="169" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A169" s="7"/>
       <c r="B169" s="7"/>
       <c r="C169" s="7"/>
@@ -3350,7 +3360,7 @@
       <c r="K169" s="7"/>
       <c r="L169" s="7"/>
     </row>
-    <row r="170" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A170" s="6"/>
       <c r="B170" s="6"/>
       <c r="C170" s="6"/>
@@ -3364,7 +3374,7 @@
       <c r="K170" s="6"/>
       <c r="L170" s="6"/>
     </row>
-    <row r="171" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A171" s="6"/>
       <c r="B171" s="6"/>
       <c r="C171" s="6"/>
@@ -3378,7 +3388,7 @@
       <c r="K171" s="6"/>
       <c r="L171" s="6"/>
     </row>
-    <row r="172" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A172" s="6"/>
       <c r="B172" s="6"/>
       <c r="C172" s="6"/>
@@ -3392,7 +3402,7 @@
       <c r="K172" s="6"/>
       <c r="L172" s="6"/>
     </row>
-    <row r="173" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A173" s="7"/>
       <c r="B173" s="7"/>
       <c r="C173" s="7"/>
@@ -3406,7 +3416,7 @@
       <c r="K173" s="7"/>
       <c r="L173" s="7"/>
     </row>
-    <row r="174" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="174" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A174" s="6"/>
       <c r="B174" s="6"/>
       <c r="C174" s="6"/>
@@ -3420,7 +3430,7 @@
       <c r="K174" s="6"/>
       <c r="L174" s="6"/>
     </row>
-    <row r="175" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="175" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A175" s="6"/>
       <c r="B175" s="6"/>
       <c r="C175" s="6"/>
@@ -3434,7 +3444,7 @@
       <c r="K175" s="6"/>
       <c r="L175" s="6"/>
     </row>
-    <row r="176" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="176" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A176" s="6"/>
       <c r="B176" s="6"/>
       <c r="C176" s="6"/>
@@ -3448,7 +3458,7 @@
       <c r="K176" s="6"/>
       <c r="L176" s="6"/>
     </row>
-    <row r="177" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="177" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A177" s="7"/>
       <c r="B177" s="7"/>
       <c r="C177" s="7"/>
@@ -3462,7 +3472,7 @@
       <c r="K177" s="7"/>
       <c r="L177" s="7"/>
     </row>
-    <row r="178" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="178" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A178" s="7"/>
       <c r="B178" s="7"/>
       <c r="C178" s="7"/>
@@ -3476,7 +3486,7 @@
       <c r="K178" s="7"/>
       <c r="L178" s="7"/>
     </row>
-    <row r="179" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="179" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A179" s="7"/>
       <c r="B179" s="7"/>
       <c r="C179" s="7"/>
@@ -3490,7 +3500,7 @@
       <c r="K179" s="7"/>
       <c r="L179" s="7"/>
     </row>
-    <row r="180" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="180" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A180" s="7"/>
       <c r="B180" s="7"/>
       <c r="C180" s="7"/>
@@ -3504,7 +3514,7 @@
       <c r="K180" s="7"/>
       <c r="L180" s="7"/>
     </row>
-    <row r="181" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="181" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A181" s="7"/>
       <c r="B181" s="7"/>
       <c r="C181" s="7"/>
@@ -3518,7 +3528,7 @@
       <c r="K181" s="7"/>
       <c r="L181" s="7"/>
     </row>
-    <row r="182" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="182" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A182" s="7"/>
       <c r="B182" s="7"/>
       <c r="C182" s="7"/>
@@ -3532,7 +3542,7 @@
       <c r="K182" s="7"/>
       <c r="L182" s="7"/>
     </row>
-    <row r="183" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="183" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A183" s="6"/>
       <c r="B183" s="6"/>
       <c r="C183" s="6"/>
@@ -3546,7 +3556,7 @@
       <c r="K183" s="6"/>
       <c r="L183" s="6"/>
     </row>
-    <row r="184" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="184" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A184" s="6"/>
       <c r="B184" s="6"/>
       <c r="C184" s="6"/>
@@ -3560,7 +3570,7 @@
       <c r="K184" s="6"/>
       <c r="L184" s="6"/>
     </row>
-    <row r="185" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="185" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A185" s="6"/>
       <c r="B185" s="6"/>
       <c r="C185" s="6"/>
@@ -3574,7 +3584,7 @@
       <c r="K185" s="6"/>
       <c r="L185" s="6"/>
     </row>
-    <row r="186" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="186" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A186" s="6"/>
       <c r="B186" s="6"/>
       <c r="C186" s="6"/>
@@ -3588,7 +3598,7 @@
       <c r="K186" s="6"/>
       <c r="L186" s="6"/>
     </row>
-    <row r="187" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="187" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A187" s="7"/>
       <c r="B187" s="7"/>
       <c r="C187" s="7"/>
@@ -3602,7 +3612,7 @@
       <c r="K187" s="7"/>
       <c r="L187" s="7"/>
     </row>
-    <row r="188" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="188" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A188" s="7"/>
       <c r="B188" s="7"/>
       <c r="C188" s="7"/>
@@ -3616,7 +3626,7 @@
       <c r="K188" s="7"/>
       <c r="L188" s="7"/>
     </row>
-    <row r="189" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="189" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A189" s="7"/>
       <c r="B189" s="7"/>
       <c r="C189" s="7"/>
@@ -3630,7 +3640,7 @@
       <c r="K189" s="7"/>
       <c r="L189" s="7"/>
     </row>
-    <row r="190" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="190" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A190" s="7"/>
       <c r="B190" s="7"/>
       <c r="C190" s="7"/>
@@ -3644,7 +3654,7 @@
       <c r="K190" s="7"/>
       <c r="L190" s="7"/>
     </row>
-    <row r="191" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="191" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A191" s="7"/>
       <c r="B191" s="7"/>
       <c r="C191" s="7"/>
@@ -3658,7 +3668,7 @@
       <c r="K191" s="7"/>
       <c r="L191" s="7"/>
     </row>
-    <row r="192" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="192" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A192" s="7"/>
       <c r="B192" s="7"/>
       <c r="C192" s="7"/>
@@ -3672,7 +3682,7 @@
       <c r="K192" s="7"/>
       <c r="L192" s="7"/>
     </row>
-    <row r="193" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="193" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A193" s="7"/>
       <c r="B193" s="7"/>
       <c r="C193" s="7"/>
@@ -3686,7 +3696,7 @@
       <c r="K193" s="7"/>
       <c r="L193" s="7"/>
     </row>
-    <row r="194" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="194" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A194" s="7"/>
       <c r="B194" s="7"/>
       <c r="C194" s="7"/>
@@ -3700,7 +3710,7 @@
       <c r="K194" s="7"/>
       <c r="L194" s="7"/>
     </row>
-    <row r="195" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="195" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A195" s="7"/>
       <c r="B195" s="7"/>
       <c r="C195" s="7"/>
@@ -3714,7 +3724,7 @@
       <c r="K195" s="7"/>
       <c r="L195" s="7"/>
     </row>
-    <row r="196" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="196" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A196" s="7"/>
       <c r="B196" s="7"/>
       <c r="C196" s="7"/>
@@ -3728,7 +3738,7 @@
       <c r="K196" s="7"/>
       <c r="L196" s="7"/>
     </row>
-    <row r="197" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="197" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A197" s="7"/>
       <c r="B197" s="7"/>
       <c r="C197" s="7"/>
@@ -3742,7 +3752,7 @@
       <c r="K197" s="7"/>
       <c r="L197" s="7"/>
     </row>
-    <row r="198" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="198" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A198" s="7"/>
       <c r="B198" s="7"/>
       <c r="C198" s="7"/>
@@ -3756,7 +3766,7 @@
       <c r="K198" s="7"/>
       <c r="L198" s="7"/>
     </row>
-    <row r="199" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="199" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A199" s="7"/>
       <c r="B199" s="7"/>
       <c r="C199" s="7"/>
@@ -3770,7 +3780,7 @@
       <c r="K199" s="7"/>
       <c r="L199" s="7"/>
     </row>
-    <row r="200" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="200" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A200" s="6"/>
       <c r="B200" s="6"/>
       <c r="C200" s="6"/>
@@ -3784,7 +3794,7 @@
       <c r="K200" s="6"/>
       <c r="L200" s="6"/>
     </row>
-    <row r="201" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="201" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A201" s="6"/>
       <c r="B201" s="6"/>
       <c r="C201" s="6"/>
@@ -3798,7 +3808,7 @@
       <c r="K201" s="6"/>
       <c r="L201" s="6"/>
     </row>
-    <row r="202" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="202" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A202" s="6"/>
       <c r="B202" s="6"/>
       <c r="C202" s="6"/>
@@ -3812,7 +3822,7 @@
       <c r="K202" s="6"/>
       <c r="L202" s="6"/>
     </row>
-    <row r="203" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="203" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A203" s="6"/>
       <c r="B203" s="6"/>
       <c r="C203" s="6"/>
@@ -3826,7 +3836,7 @@
       <c r="K203" s="6"/>
       <c r="L203" s="6"/>
     </row>
-    <row r="204" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="204" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A204" s="6"/>
       <c r="B204" s="6"/>
       <c r="C204" s="6"/>
@@ -3840,7 +3850,7 @@
       <c r="K204" s="6"/>
       <c r="L204" s="6"/>
     </row>
-    <row r="205" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="205" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A205" s="6"/>
       <c r="B205" s="6"/>
       <c r="C205" s="6"/>
@@ -3854,7 +3864,7 @@
       <c r="K205" s="6"/>
       <c r="L205" s="6"/>
     </row>
-    <row r="206" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="206" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A206" s="6"/>
       <c r="B206" s="6"/>
       <c r="C206" s="6"/>
@@ -3868,7 +3878,7 @@
       <c r="K206" s="6"/>
       <c r="L206" s="6"/>
     </row>
-    <row r="207" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="207" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A207" s="6"/>
       <c r="B207" s="6"/>
       <c r="C207" s="6"/>
@@ -3882,7 +3892,7 @@
       <c r="K207" s="6"/>
       <c r="L207" s="6"/>
     </row>
-    <row r="208" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="208" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A208" s="6"/>
       <c r="B208" s="6"/>
       <c r="C208" s="6"/>
@@ -3896,7 +3906,7 @@
       <c r="K208" s="6"/>
       <c r="L208" s="6"/>
     </row>
-    <row r="209" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="209" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A209" s="6"/>
       <c r="B209" s="6"/>
       <c r="C209" s="6"/>
@@ -3910,7 +3920,7 @@
       <c r="K209" s="6"/>
       <c r="L209" s="6"/>
     </row>
-    <row r="210" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="210" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A210" s="6"/>
       <c r="B210" s="6"/>
       <c r="C210" s="6"/>
@@ -3924,7 +3934,7 @@
       <c r="K210" s="6"/>
       <c r="L210" s="6"/>
     </row>
-    <row r="211" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="211" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A211" s="6"/>
       <c r="B211" s="6"/>
       <c r="C211" s="6"/>
@@ -3938,7 +3948,7 @@
       <c r="K211" s="6"/>
       <c r="L211" s="6"/>
     </row>
-    <row r="212" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="212" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A212" s="6"/>
       <c r="B212" s="6"/>
       <c r="C212" s="6"/>
@@ -3952,7 +3962,7 @@
       <c r="K212" s="6"/>
       <c r="L212" s="6"/>
     </row>
-    <row r="213" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="213" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A213" s="6"/>
       <c r="B213" s="6"/>
       <c r="C213" s="6"/>
@@ -3966,7 +3976,7 @@
       <c r="K213" s="6"/>
       <c r="L213" s="6"/>
     </row>
-    <row r="214" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="214" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A214" s="6"/>
       <c r="B214" s="6"/>
       <c r="C214" s="6"/>
@@ -3980,7 +3990,7 @@
       <c r="K214" s="6"/>
       <c r="L214" s="6"/>
     </row>
-    <row r="215" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="215" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A215" s="6"/>
       <c r="B215" s="6"/>
       <c r="C215" s="6"/>
@@ -3994,7 +4004,7 @@
       <c r="K215" s="6"/>
       <c r="L215" s="6"/>
     </row>
-    <row r="216" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="216" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A216" s="6"/>
       <c r="B216" s="6"/>
       <c r="C216" s="6"/>
@@ -4008,7 +4018,7 @@
       <c r="K216" s="6"/>
       <c r="L216" s="6"/>
     </row>
-    <row r="217" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="217" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A217" s="6"/>
       <c r="B217" s="6"/>
       <c r="C217" s="6"/>
@@ -4022,7 +4032,7 @@
       <c r="K217" s="6"/>
       <c r="L217" s="6"/>
     </row>
-    <row r="218" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="218" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A218" s="7"/>
       <c r="B218" s="7"/>
       <c r="C218" s="7"/>
@@ -4036,7 +4046,7 @@
       <c r="K218" s="7"/>
       <c r="L218" s="7"/>
     </row>
-    <row r="219" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="219" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A219" s="7"/>
       <c r="B219" s="7"/>
       <c r="C219" s="7"/>
@@ -4050,7 +4060,7 @@
       <c r="K219" s="7"/>
       <c r="L219" s="7"/>
     </row>
-    <row r="220" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="220" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A220" s="7"/>
       <c r="B220" s="7"/>
       <c r="C220" s="7"/>
@@ -4064,7 +4074,7 @@
       <c r="K220" s="7"/>
       <c r="L220" s="7"/>
     </row>
-    <row r="221" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="221" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A221" s="7"/>
       <c r="B221" s="7"/>
       <c r="C221" s="7"/>
@@ -4078,7 +4088,7 @@
       <c r="K221" s="7"/>
       <c r="L221" s="7"/>
     </row>
-    <row r="222" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="222" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A222" s="7"/>
       <c r="B222" s="7"/>
       <c r="C222" s="7"/>
@@ -4092,7 +4102,7 @@
       <c r="K222" s="7"/>
       <c r="L222" s="7"/>
     </row>
-    <row r="223" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="223" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A223" s="7"/>
       <c r="B223" s="7"/>
       <c r="C223" s="7"/>
@@ -4106,7 +4116,7 @@
       <c r="K223" s="7"/>
       <c r="L223" s="7"/>
     </row>
-    <row r="224" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="224" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A224" s="7"/>
       <c r="B224" s="7"/>
       <c r="C224" s="7"/>
@@ -4120,7 +4130,7 @@
       <c r="K224" s="7"/>
       <c r="L224" s="7"/>
     </row>
-    <row r="225" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="225" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A225" s="7"/>
       <c r="B225" s="7"/>
       <c r="C225" s="7"/>
@@ -4134,7 +4144,7 @@
       <c r="K225" s="7"/>
       <c r="L225" s="7"/>
     </row>
-    <row r="226" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="226" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A226" s="7"/>
       <c r="B226" s="7"/>
       <c r="C226" s="7"/>
@@ -4148,7 +4158,7 @@
       <c r="K226" s="7"/>
       <c r="L226" s="7"/>
     </row>
-    <row r="227" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="227" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A227" s="7"/>
       <c r="B227" s="7"/>
       <c r="C227" s="7"/>
@@ -4162,7 +4172,7 @@
       <c r="K227" s="7"/>
       <c r="L227" s="7"/>
     </row>
-    <row r="228" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="228" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A228" s="7"/>
       <c r="B228" s="7"/>
       <c r="C228" s="7"/>
@@ -4176,7 +4186,7 @@
       <c r="K228" s="7"/>
       <c r="L228" s="7"/>
     </row>
-    <row r="229" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="229" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A229" s="7"/>
       <c r="B229" s="7"/>
       <c r="C229" s="7"/>
@@ -4190,7 +4200,7 @@
       <c r="K229" s="7"/>
       <c r="L229" s="7"/>
     </row>
-    <row r="230" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="230" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A230" s="6"/>
       <c r="B230" s="6"/>
       <c r="C230" s="6"/>
@@ -4204,7 +4214,7 @@
       <c r="K230" s="6"/>
       <c r="L230" s="6"/>
     </row>
-    <row r="231" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="231" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A231" s="6"/>
       <c r="B231" s="6"/>
       <c r="C231" s="6"/>
@@ -4218,7 +4228,7 @@
       <c r="K231" s="6"/>
       <c r="L231" s="6"/>
     </row>
-    <row r="232" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="232" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A232" s="6"/>
       <c r="B232" s="6"/>
       <c r="C232" s="6"/>
@@ -4232,7 +4242,7 @@
       <c r="K232" s="6"/>
       <c r="L232" s="6"/>
     </row>
-    <row r="233" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="233" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A233" s="6"/>
       <c r="B233" s="6"/>
       <c r="C233" s="6"/>
@@ -4246,7 +4256,7 @@
       <c r="K233" s="6"/>
       <c r="L233" s="6"/>
     </row>
-    <row r="234" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="234" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A234" s="7"/>
       <c r="B234" s="7"/>
       <c r="C234" s="7"/>
@@ -4260,7 +4270,7 @@
       <c r="K234" s="7"/>
       <c r="L234" s="7"/>
     </row>
-    <row r="235" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="235" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A235" s="7"/>
       <c r="B235" s="7"/>
       <c r="C235" s="7"/>
@@ -4274,7 +4284,7 @@
       <c r="K235" s="7"/>
       <c r="L235" s="7"/>
     </row>
-    <row r="236" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="236" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A236" s="6"/>
       <c r="B236" s="6"/>
       <c r="C236" s="6"/>
@@ -4288,7 +4298,7 @@
       <c r="K236" s="6"/>
       <c r="L236" s="6"/>
     </row>
-    <row r="237" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="237" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A237" s="6"/>
       <c r="B237" s="6"/>
       <c r="C237" s="6"/>
@@ -4302,7 +4312,7 @@
       <c r="K237" s="6"/>
       <c r="L237" s="6"/>
     </row>
-    <row r="238" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="238" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A238" s="7"/>
       <c r="B238" s="7"/>
       <c r="C238" s="7"/>
@@ -4316,7 +4326,7 @@
       <c r="K238" s="7"/>
       <c r="L238" s="7"/>
     </row>
-    <row r="239" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="239" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A239" s="7"/>
       <c r="B239" s="7"/>
       <c r="C239" s="7"/>
@@ -4330,7 +4340,7 @@
       <c r="K239" s="7"/>
       <c r="L239" s="7"/>
     </row>
-    <row r="240" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="240" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A240" s="7"/>
       <c r="B240" s="7"/>
       <c r="C240" s="7"/>
@@ -4344,7 +4354,7 @@
       <c r="K240" s="7"/>
       <c r="L240" s="7"/>
     </row>
-    <row r="241" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="241" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A241" s="6"/>
       <c r="B241" s="6"/>
       <c r="C241" s="6"/>
@@ -4358,7 +4368,7 @@
       <c r="K241" s="6"/>
       <c r="L241" s="6"/>
     </row>
-    <row r="242" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="242" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A242" s="6"/>
       <c r="B242" s="6"/>
       <c r="C242" s="6"/>
@@ -4372,7 +4382,7 @@
       <c r="K242" s="6"/>
       <c r="L242" s="6"/>
     </row>
-    <row r="243" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="243" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A243" s="6"/>
       <c r="B243" s="6"/>
       <c r="C243" s="6"/>
@@ -4386,7 +4396,7 @@
       <c r="K243" s="6"/>
       <c r="L243" s="6"/>
     </row>
-    <row r="244" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="244" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A244" s="6"/>
       <c r="B244" s="6"/>
       <c r="C244" s="6"/>
@@ -4400,7 +4410,7 @@
       <c r="K244" s="6"/>
       <c r="L244" s="6"/>
     </row>
-    <row r="245" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="245" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A245" s="6"/>
       <c r="B245" s="6"/>
       <c r="C245" s="6"/>
@@ -4414,7 +4424,7 @@
       <c r="K245" s="6"/>
       <c r="L245" s="6"/>
     </row>
-    <row r="246" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="246" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A246" s="6"/>
       <c r="B246" s="6"/>
       <c r="C246" s="6"/>
@@ -4428,7 +4438,7 @@
       <c r="K246" s="6"/>
       <c r="L246" s="6"/>
     </row>
-    <row r="247" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="247" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A247" s="6"/>
       <c r="B247" s="6"/>
       <c r="C247" s="6"/>
@@ -4442,7 +4452,7 @@
       <c r="K247" s="6"/>
       <c r="L247" s="6"/>
     </row>
-    <row r="248" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="248" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A248" s="6"/>
       <c r="B248" s="6"/>
       <c r="C248" s="6"/>
@@ -4456,7 +4466,7 @@
       <c r="K248" s="6"/>
       <c r="L248" s="6"/>
     </row>
-    <row r="249" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="249" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A249" s="6"/>
       <c r="B249" s="6"/>
       <c r="C249" s="6"/>
@@ -4470,7 +4480,7 @@
       <c r="K249" s="6"/>
       <c r="L249" s="6"/>
     </row>
-    <row r="250" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="250" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A250" s="6"/>
       <c r="B250" s="6"/>
       <c r="C250" s="6"/>
@@ -4484,7 +4494,7 @@
       <c r="K250" s="6"/>
       <c r="L250" s="6"/>
     </row>
-    <row r="251" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="251" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A251" s="6"/>
       <c r="B251" s="6"/>
       <c r="C251" s="6"/>
@@ -4498,7 +4508,7 @@
       <c r="K251" s="6"/>
       <c r="L251" s="6"/>
     </row>
-    <row r="252" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="252" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A252" s="6"/>
       <c r="B252" s="6"/>
       <c r="C252" s="6"/>
@@ -4512,7 +4522,7 @@
       <c r="K252" s="6"/>
       <c r="L252" s="6"/>
     </row>
-    <row r="253" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="253" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A253" s="6"/>
       <c r="B253" s="6"/>
       <c r="C253" s="6"/>
@@ -4526,7 +4536,7 @@
       <c r="K253" s="6"/>
       <c r="L253" s="6"/>
     </row>
-    <row r="254" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="254" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A254" s="6"/>
       <c r="B254" s="6"/>
       <c r="C254" s="6"/>
@@ -4540,7 +4550,7 @@
       <c r="K254" s="6"/>
       <c r="L254" s="6"/>
     </row>
-    <row r="255" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="255" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A255" s="6"/>
       <c r="B255" s="6"/>
       <c r="C255" s="6"/>
@@ -4554,7 +4564,7 @@
       <c r="K255" s="6"/>
       <c r="L255" s="6"/>
     </row>
-    <row r="256" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="256" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A256" s="6"/>
       <c r="B256" s="6"/>
       <c r="C256" s="6"/>
@@ -4568,7 +4578,7 @@
       <c r="K256" s="6"/>
       <c r="L256" s="6"/>
     </row>
-    <row r="257" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="257" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A257" s="7"/>
       <c r="B257" s="7"/>
       <c r="C257" s="7"/>
@@ -4582,7 +4592,7 @@
       <c r="K257" s="7"/>
       <c r="L257" s="7"/>
     </row>
-    <row r="258" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="258" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A258" s="7"/>
       <c r="B258" s="7"/>
       <c r="C258" s="7"/>
@@ -4596,7 +4606,7 @@
       <c r="K258" s="7"/>
       <c r="L258" s="7"/>
     </row>
-    <row r="259" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="259" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A259" s="7"/>
       <c r="B259" s="7"/>
       <c r="C259" s="7"/>
@@ -4610,7 +4620,7 @@
       <c r="K259" s="7"/>
       <c r="L259" s="7"/>
     </row>
-    <row r="260" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="260" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A260" s="7"/>
       <c r="B260" s="7"/>
       <c r="C260" s="7"/>
@@ -4624,7 +4634,7 @@
       <c r="K260" s="7"/>
       <c r="L260" s="7"/>
     </row>
-    <row r="261" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="261" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A261" s="6"/>
       <c r="B261" s="6"/>
       <c r="C261" s="6"/>
@@ -4638,7 +4648,7 @@
       <c r="K261" s="6"/>
       <c r="L261" s="6"/>
     </row>
-    <row r="262" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="262" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A262" s="6"/>
       <c r="B262" s="6"/>
       <c r="C262" s="6"/>
@@ -4652,7 +4662,7 @@
       <c r="K262" s="6"/>
       <c r="L262" s="6"/>
     </row>
-    <row r="263" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="263" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A263" s="6"/>
       <c r="B263" s="6"/>
       <c r="C263" s="6"/>
@@ -4666,7 +4676,7 @@
       <c r="K263" s="6"/>
       <c r="L263" s="6"/>
     </row>
-    <row r="264" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="264" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A264" s="6"/>
       <c r="B264" s="6"/>
       <c r="C264" s="6"/>
@@ -4680,7 +4690,7 @@
       <c r="K264" s="6"/>
       <c r="L264" s="6"/>
     </row>
-    <row r="265" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="265" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A265" s="6"/>
       <c r="B265" s="6"/>
       <c r="C265" s="6"/>
@@ -4694,7 +4704,7 @@
       <c r="K265" s="6"/>
       <c r="L265" s="6"/>
     </row>
-    <row r="266" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="266" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A266" s="6"/>
       <c r="B266" s="6"/>
       <c r="C266" s="6"/>
@@ -4708,7 +4718,7 @@
       <c r="K266" s="6"/>
       <c r="L266" s="6"/>
     </row>
-    <row r="267" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="267" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A267" s="7"/>
       <c r="B267" s="7"/>
       <c r="C267" s="7"/>
@@ -4722,7 +4732,7 @@
       <c r="K267" s="7"/>
       <c r="L267" s="7"/>
     </row>
-    <row r="268" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="268" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A268" s="7"/>
       <c r="B268" s="7"/>
       <c r="C268" s="7"/>
@@ -4736,7 +4746,7 @@
       <c r="K268" s="7"/>
       <c r="L268" s="7"/>
     </row>
-    <row r="269" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="269" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A269" s="7"/>
       <c r="B269" s="7"/>
       <c r="C269" s="7"/>
@@ -4750,7 +4760,7 @@
       <c r="K269" s="7"/>
       <c r="L269" s="7"/>
     </row>
-    <row r="270" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="270" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A270" s="6"/>
       <c r="B270" s="6"/>
       <c r="C270" s="6"/>
@@ -4764,7 +4774,7 @@
       <c r="K270" s="6"/>
       <c r="L270" s="6"/>
     </row>
-    <row r="271" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="271" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A271" s="6"/>
       <c r="B271" s="6"/>
       <c r="C271" s="6"/>
@@ -4778,7 +4788,7 @@
       <c r="K271" s="6"/>
       <c r="L271" s="6"/>
     </row>
-    <row r="272" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="272" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A272" s="6"/>
       <c r="B272" s="6"/>
       <c r="C272" s="6"/>
@@ -4792,7 +4802,7 @@
       <c r="K272" s="6"/>
       <c r="L272" s="6"/>
     </row>
-    <row r="273" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="273" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A273" s="6"/>
       <c r="B273" s="6"/>
       <c r="C273" s="6"/>
@@ -4806,7 +4816,7 @@
       <c r="K273" s="6"/>
       <c r="L273" s="6"/>
     </row>
-    <row r="274" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="274" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A274" s="6"/>
       <c r="B274" s="6"/>
       <c r="C274" s="6"/>
@@ -4820,7 +4830,7 @@
       <c r="K274" s="6"/>
       <c r="L274" s="6"/>
     </row>
-    <row r="275" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="275" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A275" s="7"/>
       <c r="B275" s="7"/>
       <c r="C275" s="7"/>
@@ -4834,7 +4844,7 @@
       <c r="K275" s="7"/>
       <c r="L275" s="7"/>
     </row>
-    <row r="276" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="276" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A276" s="7"/>
       <c r="B276" s="7"/>
       <c r="C276" s="7"/>
@@ -4848,7 +4858,7 @@
       <c r="K276" s="7"/>
       <c r="L276" s="7"/>
     </row>
-    <row r="277" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="277" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A277" s="7"/>
       <c r="B277" s="7"/>
       <c r="C277" s="7"/>
@@ -4862,7 +4872,7 @@
       <c r="K277" s="7"/>
       <c r="L277" s="7"/>
     </row>
-    <row r="278" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="278" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A278" s="6"/>
       <c r="B278" s="6"/>
       <c r="C278" s="6"/>
@@ -4876,7 +4886,7 @@
       <c r="K278" s="6"/>
       <c r="L278" s="6"/>
     </row>
-    <row r="279" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="279" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A279" s="6"/>
       <c r="B279" s="6"/>
       <c r="C279" s="6"/>
@@ -4890,7 +4900,7 @@
       <c r="K279" s="6"/>
       <c r="L279" s="6"/>
     </row>
-    <row r="280" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="280" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A280" s="6"/>
       <c r="B280" s="6"/>
       <c r="C280" s="6"/>
@@ -4904,7 +4914,7 @@
       <c r="K280" s="6"/>
       <c r="L280" s="6"/>
     </row>
-    <row r="281" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="281" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A281" s="6"/>
       <c r="B281" s="6"/>
       <c r="C281" s="6"/>
@@ -4918,7 +4928,7 @@
       <c r="K281" s="6"/>
       <c r="L281" s="6"/>
     </row>
-    <row r="282" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="282" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A282" s="6"/>
       <c r="B282" s="6"/>
       <c r="C282" s="6"/>
@@ -4932,7 +4942,7 @@
       <c r="K282" s="6"/>
       <c r="L282" s="6"/>
     </row>
-    <row r="283" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="283" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A283" s="6"/>
       <c r="B283" s="6"/>
       <c r="C283" s="6"/>
@@ -4946,7 +4956,7 @@
       <c r="K283" s="6"/>
       <c r="L283" s="6"/>
     </row>
-    <row r="284" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="284" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A284" s="6"/>
       <c r="B284" s="6"/>
       <c r="C284" s="6"/>
@@ -4960,7 +4970,7 @@
       <c r="K284" s="6"/>
       <c r="L284" s="6"/>
     </row>
-    <row r="285" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="285" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A285" s="6"/>
       <c r="B285" s="6"/>
       <c r="C285" s="6"/>
@@ -4974,7 +4984,7 @@
       <c r="K285" s="6"/>
       <c r="L285" s="6"/>
     </row>
-    <row r="286" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="286" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A286" s="7"/>
       <c r="B286" s="7"/>
       <c r="C286" s="7"/>
@@ -4988,7 +4998,7 @@
       <c r="K286" s="7"/>
       <c r="L286" s="7"/>
     </row>
-    <row r="287" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="287" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A287" s="7"/>
       <c r="B287" s="7"/>
       <c r="C287" s="7"/>
@@ -5002,7 +5012,7 @@
       <c r="K287" s="7"/>
       <c r="L287" s="7"/>
     </row>
-    <row r="288" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="288" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A288" s="7"/>
       <c r="B288" s="7"/>
       <c r="C288" s="7"/>
@@ -5016,7 +5026,7 @@
       <c r="K288" s="7"/>
       <c r="L288" s="7"/>
     </row>
-    <row r="289" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="289" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A289" s="7"/>
       <c r="B289" s="7"/>
       <c r="C289" s="7"/>
@@ -5030,7 +5040,7 @@
       <c r="K289" s="7"/>
       <c r="L289" s="7"/>
     </row>
-    <row r="290" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="290" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A290" s="6"/>
       <c r="B290" s="6"/>
       <c r="C290" s="6"/>
@@ -5044,7 +5054,7 @@
       <c r="K290" s="6"/>
       <c r="L290" s="6"/>
     </row>
-    <row r="291" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="291" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A291" s="6"/>
       <c r="B291" s="6"/>
       <c r="C291" s="6"/>
@@ -5058,7 +5068,7 @@
       <c r="K291" s="6"/>
       <c r="L291" s="6"/>
     </row>
-    <row r="292" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="292" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A292" s="6"/>
       <c r="B292" s="6"/>
       <c r="C292" s="6"/>
@@ -5072,7 +5082,7 @@
       <c r="K292" s="6"/>
       <c r="L292" s="6"/>
     </row>
-    <row r="293" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="293" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A293" s="6"/>
       <c r="B293" s="6"/>
       <c r="C293" s="6"/>
@@ -5086,7 +5096,7 @@
       <c r="K293" s="6"/>
       <c r="L293" s="6"/>
     </row>
-    <row r="294" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="294" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A294" s="6"/>
       <c r="B294" s="6"/>
       <c r="C294" s="6"/>
@@ -5100,7 +5110,7 @@
       <c r="K294" s="6"/>
       <c r="L294" s="6"/>
     </row>
-    <row r="295" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="295" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A295" s="6"/>
       <c r="B295" s="6"/>
       <c r="C295" s="6"/>
@@ -5114,7 +5124,7 @@
       <c r="K295" s="6"/>
       <c r="L295" s="6"/>
     </row>
-    <row r="296" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="296" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A296" s="6"/>
       <c r="B296" s="6"/>
       <c r="C296" s="6"/>
@@ -5128,7 +5138,7 @@
       <c r="K296" s="6"/>
       <c r="L296" s="6"/>
     </row>
-    <row r="297" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="297" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A297" s="7"/>
       <c r="B297" s="7"/>
       <c r="C297" s="7"/>
@@ -5142,7 +5152,7 @@
       <c r="K297" s="7"/>
       <c r="L297" s="7"/>
     </row>
-    <row r="298" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="298" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A298" s="7"/>
       <c r="B298" s="7"/>
       <c r="C298" s="7"/>
@@ -5156,7 +5166,7 @@
       <c r="K298" s="7"/>
       <c r="L298" s="7"/>
     </row>
-    <row r="299" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="299" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A299" s="7"/>
       <c r="B299" s="7"/>
       <c r="C299" s="7"/>
@@ -5170,7 +5180,7 @@
       <c r="K299" s="7"/>
       <c r="L299" s="7"/>
     </row>
-    <row r="300" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="300" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A300" s="7"/>
       <c r="B300" s="7"/>
       <c r="C300" s="7"/>
@@ -5184,7 +5194,7 @@
       <c r="K300" s="7"/>
       <c r="L300" s="7"/>
     </row>
-    <row r="301" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="301" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A301" s="7"/>
       <c r="B301" s="7"/>
       <c r="C301" s="7"/>
@@ -5198,7 +5208,7 @@
       <c r="K301" s="7"/>
       <c r="L301" s="7"/>
     </row>
-    <row r="302" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="302" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A302" s="7"/>
       <c r="B302" s="7"/>
       <c r="C302" s="7"/>
@@ -5212,7 +5222,7 @@
       <c r="K302" s="7"/>
       <c r="L302" s="7"/>
     </row>
-    <row r="303" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="303" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A303" s="7"/>
       <c r="B303" s="7"/>
       <c r="C303" s="7"/>
@@ -5226,7 +5236,7 @@
       <c r="K303" s="7"/>
       <c r="L303" s="7"/>
     </row>
-    <row r="304" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="304" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A304" s="7"/>
       <c r="B304" s="7"/>
       <c r="C304" s="7"/>
@@ -5240,7 +5250,7 @@
       <c r="K304" s="7"/>
       <c r="L304" s="7"/>
     </row>
-    <row r="305" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="305" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A305" s="6"/>
       <c r="B305" s="6"/>
       <c r="C305" s="6"/>
@@ -5254,7 +5264,7 @@
       <c r="K305" s="6"/>
       <c r="L305" s="6"/>
     </row>
-    <row r="306" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="306" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A306" s="6"/>
       <c r="B306" s="6"/>
       <c r="C306" s="6"/>
@@ -5268,7 +5278,7 @@
       <c r="K306" s="6"/>
       <c r="L306" s="6"/>
     </row>
-    <row r="307" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="307" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A307" s="7"/>
       <c r="B307" s="7"/>
       <c r="C307" s="7"/>
@@ -5282,7 +5292,7 @@
       <c r="K307" s="7"/>
       <c r="L307" s="7"/>
     </row>
-    <row r="308" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="308" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A308" s="7"/>
       <c r="B308" s="7"/>
       <c r="C308" s="7"/>
@@ -5296,7 +5306,7 @@
       <c r="K308" s="7"/>
       <c r="L308" s="7"/>
     </row>
-    <row r="309" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="309" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A309" s="7"/>
       <c r="B309" s="7"/>
       <c r="C309" s="7"/>
@@ -5310,7 +5320,7 @@
       <c r="K309" s="7"/>
       <c r="L309" s="7"/>
     </row>
-    <row r="310" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="310" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A310" s="7"/>
       <c r="B310" s="7"/>
       <c r="C310" s="7"/>
@@ -5324,7 +5334,7 @@
       <c r="K310" s="7"/>
       <c r="L310" s="7"/>
     </row>
-    <row r="311" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="311" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A311" s="7"/>
       <c r="B311" s="7"/>
       <c r="C311" s="7"/>
@@ -5338,7 +5348,7 @@
       <c r="K311" s="7"/>
       <c r="L311" s="7"/>
     </row>
-    <row r="312" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="312" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A312" s="6"/>
       <c r="B312" s="6"/>
       <c r="C312" s="6"/>
@@ -5352,7 +5362,7 @@
       <c r="K312" s="6"/>
       <c r="L312" s="6"/>
     </row>
-    <row r="313" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="313" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A313" s="6"/>
       <c r="B313" s="6"/>
       <c r="C313" s="6"/>
@@ -5366,7 +5376,7 @@
       <c r="K313" s="6"/>
       <c r="L313" s="6"/>
     </row>
-    <row r="314" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="314" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A314" s="6"/>
       <c r="B314" s="6"/>
       <c r="C314" s="6"/>
@@ -5380,7 +5390,7 @@
       <c r="K314" s="6"/>
       <c r="L314" s="6"/>
     </row>
-    <row r="315" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="315" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A315" s="6"/>
       <c r="B315" s="6"/>
       <c r="C315" s="6"/>
@@ -5394,7 +5404,7 @@
       <c r="K315" s="6"/>
       <c r="L315" s="6"/>
     </row>
-    <row r="316" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="316" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A316" s="7"/>
       <c r="B316" s="7"/>
       <c r="C316" s="7"/>
@@ -5408,7 +5418,7 @@
       <c r="K316" s="7"/>
       <c r="L316" s="7"/>
     </row>
-    <row r="317" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="317" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A317" s="7"/>
       <c r="B317" s="7"/>
       <c r="C317" s="7"/>
@@ -5422,7 +5432,7 @@
       <c r="K317" s="7"/>
       <c r="L317" s="7"/>
     </row>
-    <row r="318" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="318" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A318" s="7"/>
       <c r="B318" s="7"/>
       <c r="C318" s="7"/>
@@ -5436,7 +5446,7 @@
       <c r="K318" s="7"/>
       <c r="L318" s="7"/>
     </row>
-    <row r="319" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="319" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A319" s="6"/>
       <c r="B319" s="6"/>
       <c r="C319" s="6"/>
@@ -5450,7 +5460,7 @@
       <c r="K319" s="6"/>
       <c r="L319" s="6"/>
     </row>
-    <row r="320" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="320" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A320" s="6"/>
       <c r="B320" s="6"/>
       <c r="C320" s="6"/>
@@ -5464,7 +5474,7 @@
       <c r="K320" s="6"/>
       <c r="L320" s="6"/>
     </row>
-    <row r="321" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="321" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A321" s="6"/>
       <c r="B321" s="6"/>
       <c r="C321" s="6"/>
@@ -5478,7 +5488,7 @@
       <c r="K321" s="6"/>
       <c r="L321" s="6"/>
     </row>
-    <row r="322" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="322" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A322" s="6"/>
       <c r="B322" s="6"/>
       <c r="C322" s="6"/>
@@ -5492,7 +5502,7 @@
       <c r="K322" s="6"/>
       <c r="L322" s="6"/>
     </row>
-    <row r="323" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="323" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A323" s="6"/>
       <c r="B323" s="6"/>
       <c r="C323" s="6"/>
@@ -5506,7 +5516,7 @@
       <c r="K323" s="6"/>
       <c r="L323" s="6"/>
     </row>
-    <row r="324" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="324" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A324" s="6"/>
       <c r="B324" s="6"/>
       <c r="C324" s="6"/>
@@ -5520,7 +5530,7 @@
       <c r="K324" s="6"/>
       <c r="L324" s="6"/>
     </row>
-    <row r="325" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="325" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A325" s="7"/>
       <c r="B325" s="7"/>
       <c r="C325" s="7"/>
@@ -5534,7 +5544,7 @@
       <c r="K325" s="7"/>
       <c r="L325" s="7"/>
     </row>
-    <row r="326" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="326" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A326" s="7"/>
       <c r="B326" s="7"/>
       <c r="C326" s="7"/>
@@ -5548,7 +5558,7 @@
       <c r="K326" s="7"/>
       <c r="L326" s="7"/>
     </row>
-    <row r="327" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="327" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A327" s="7"/>
       <c r="B327" s="7"/>
       <c r="C327" s="7"/>
@@ -5562,7 +5572,7 @@
       <c r="K327" s="7"/>
       <c r="L327" s="7"/>
     </row>
-    <row r="328" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="328" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A328" s="7"/>
       <c r="B328" s="7"/>
       <c r="C328" s="7"/>
@@ -5576,7 +5586,7 @@
       <c r="K328" s="7"/>
       <c r="L328" s="7"/>
     </row>
-    <row r="329" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="329" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A329" s="7"/>
       <c r="B329" s="7"/>
       <c r="C329" s="7"/>
@@ -5590,7 +5600,7 @@
       <c r="K329" s="7"/>
       <c r="L329" s="7"/>
     </row>
-    <row r="330" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="330" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A330" s="7"/>
       <c r="B330" s="7"/>
       <c r="C330" s="7"/>
@@ -5604,7 +5614,7 @@
       <c r="K330" s="7"/>
       <c r="L330" s="7"/>
     </row>
-    <row r="331" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="331" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A331" s="7"/>
       <c r="B331" s="7"/>
       <c r="C331" s="7"/>
@@ -5618,7 +5628,7 @@
       <c r="K331" s="7"/>
       <c r="L331" s="7"/>
     </row>
-    <row r="332" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="332" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A332" s="6"/>
       <c r="B332" s="6"/>
       <c r="C332" s="6"/>
@@ -5632,7 +5642,7 @@
       <c r="K332" s="6"/>
       <c r="L332" s="6"/>
     </row>
-    <row r="333" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="333" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A333" s="6"/>
       <c r="B333" s="6"/>
       <c r="C333" s="6"/>
@@ -5646,7 +5656,7 @@
       <c r="K333" s="6"/>
       <c r="L333" s="6"/>
     </row>
-    <row r="334" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="334" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A334" s="6"/>
       <c r="B334" s="6"/>
       <c r="C334" s="6"/>
@@ -5669,22 +5679,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:H61"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C13" sqref="C13"/>
+      <selection pane="bottomLeft" activeCell="H3" sqref="H3:H61"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="26.44140625" customWidth="1"/>
+    <col min="1" max="1" width="26.5" customWidth="1"/>
     <col min="2" max="3" width="13" customWidth="1"/>
-    <col min="4" max="4" width="29.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="29.5" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="70" customWidth="1"/>
-    <col min="6" max="7" width="13" hidden="1" customWidth="1"/>
-    <col min="8" max="8" width="70" hidden="1" customWidth="1"/>
+    <col min="6" max="7" width="13" customWidth="1"/>
+    <col min="8" max="8" width="70" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="25.8" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:8" ht="26" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>25</v>
       </c>
@@ -5696,7 +5706,7 @@
       <c r="G1" s="4"/>
       <c r="H1" s="4"/>
     </row>
-    <row r="2" spans="1:8" ht="18" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" ht="19" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>15</v>
       </c>
@@ -5722,315 +5732,316 @@
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>76</v>
+      </c>
+      <c r="D3" t="s">
+        <v>77</v>
+      </c>
+      <c r="H3" s="8" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>78</v>
+      </c>
+      <c r="D4" t="s">
+        <v>76</v>
+      </c>
+      <c r="H4" s="8" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="H5" s="8" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="H6" s="8" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="H7" s="8" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="H8" s="8" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="H9" s="8" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="H10" s="8" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="H11" s="8" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="H12" s="8" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="H13" s="8" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="H14" s="8" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="H15" s="8" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="H16" s="8" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="17" spans="8:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="H17" s="8" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="18" spans="8:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="H18" s="8" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="19" spans="8:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="H19" s="8" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="20" spans="8:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="H20" s="8" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="21" spans="8:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="H21" s="8" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="22" spans="8:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="H22" s="8" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="23" spans="8:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="H23" s="8" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="24" spans="8:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="H24" s="8" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="25" spans="8:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="H25" s="8" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="26" spans="8:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="H26" s="8" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="27" spans="8:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="H27" s="8" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="28" spans="8:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="H28" s="8" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="29" spans="8:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="H29" s="8" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="30" spans="8:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="H30" s="8" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="31" spans="8:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="H31" s="8" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="32" spans="8:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="H32" s="8" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="33" spans="8:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="H33" s="8" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="34" spans="8:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="H34" s="8" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="35" spans="8:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="H35" s="8" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="36" spans="8:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="H36" s="8" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="37" spans="8:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="H37" s="8" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="38" spans="8:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="H38" s="8" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="39" spans="8:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="H39" s="8" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="40" spans="8:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="H40" s="8" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="41" spans="8:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="H41" s="8" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="42" spans="8:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="H42" s="8" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="43" spans="8:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="H43" s="8" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="44" spans="8:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="H44" s="8" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="45" spans="8:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="H45" s="8" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="46" spans="8:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="H46" s="8" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="47" spans="8:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="H47" s="8" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="48" spans="8:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="H48" s="8" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="49" spans="8:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="H49" s="8" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="50" spans="8:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="H50" s="8" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="51" spans="8:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="H51" s="8" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="52" spans="8:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="H52" s="8" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="53" spans="8:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="H53" s="8" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="54" spans="8:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="H54" s="8" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="55" spans="8:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="H55" s="8" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="56" spans="8:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="H56" s="8" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="57" spans="8:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="H57" s="8" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="58" spans="8:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="H58" s="8" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="59" spans="8:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="H59" s="8" t="s">
         <v>135</v>
       </c>
-      <c r="D3" t="s">
+    </row>
+    <row r="60" spans="8:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="H60" s="8" t="s">
         <v>136</v>
       </c>
-      <c r="H3" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+    </row>
+    <row r="61" spans="8:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="H61" s="8" t="s">
         <v>137</v>
-      </c>
-      <c r="D4" t="s">
-        <v>135</v>
-      </c>
-      <c r="H4" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="H5" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="H6" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="H7" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="H8" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="H9" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="H10" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="H11" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="H12" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="H13" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="H14" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="H15" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="H16" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="17" spans="8:8" x14ac:dyDescent="0.3">
-      <c r="H17" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="18" spans="8:8" x14ac:dyDescent="0.3">
-      <c r="H18" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="19" spans="8:8" x14ac:dyDescent="0.3">
-      <c r="H19" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="20" spans="8:8" x14ac:dyDescent="0.3">
-      <c r="H20" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="21" spans="8:8" x14ac:dyDescent="0.3">
-      <c r="H21" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="22" spans="8:8" x14ac:dyDescent="0.3">
-      <c r="H22" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="23" spans="8:8" x14ac:dyDescent="0.3">
-      <c r="H23" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="24" spans="8:8" x14ac:dyDescent="0.3">
-      <c r="H24" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="25" spans="8:8" x14ac:dyDescent="0.3">
-      <c r="H25" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="26" spans="8:8" x14ac:dyDescent="0.3">
-      <c r="H26" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="27" spans="8:8" x14ac:dyDescent="0.3">
-      <c r="H27" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="28" spans="8:8" x14ac:dyDescent="0.3">
-      <c r="H28" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="29" spans="8:8" x14ac:dyDescent="0.3">
-      <c r="H29" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="30" spans="8:8" x14ac:dyDescent="0.3">
-      <c r="H30" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="31" spans="8:8" x14ac:dyDescent="0.3">
-      <c r="H31" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="32" spans="8:8" x14ac:dyDescent="0.3">
-      <c r="H32" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="33" spans="8:8" x14ac:dyDescent="0.3">
-      <c r="H33" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="34" spans="8:8" x14ac:dyDescent="0.3">
-      <c r="H34" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="35" spans="8:8" x14ac:dyDescent="0.3">
-      <c r="H35" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="36" spans="8:8" x14ac:dyDescent="0.3">
-      <c r="H36" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="37" spans="8:8" x14ac:dyDescent="0.3">
-      <c r="H37" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="38" spans="8:8" x14ac:dyDescent="0.3">
-      <c r="H38" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="39" spans="8:8" x14ac:dyDescent="0.3">
-      <c r="H39" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="40" spans="8:8" x14ac:dyDescent="0.3">
-      <c r="H40" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="41" spans="8:8" x14ac:dyDescent="0.3">
-      <c r="H41" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="42" spans="8:8" x14ac:dyDescent="0.3">
-      <c r="H42" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="43" spans="8:8" x14ac:dyDescent="0.3">
-      <c r="H43" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="44" spans="8:8" x14ac:dyDescent="0.3">
-      <c r="H44" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="45" spans="8:8" x14ac:dyDescent="0.3">
-      <c r="H45" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="46" spans="8:8" x14ac:dyDescent="0.3">
-      <c r="H46" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="47" spans="8:8" x14ac:dyDescent="0.3">
-      <c r="H47" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="48" spans="8:8" x14ac:dyDescent="0.3">
-      <c r="H48" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="49" spans="8:8" x14ac:dyDescent="0.3">
-      <c r="H49" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="50" spans="8:8" x14ac:dyDescent="0.3">
-      <c r="H50" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="51" spans="8:8" x14ac:dyDescent="0.3">
-      <c r="H51" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="52" spans="8:8" x14ac:dyDescent="0.3">
-      <c r="H52" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="53" spans="8:8" x14ac:dyDescent="0.3">
-      <c r="H53" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="54" spans="8:8" x14ac:dyDescent="0.3">
-      <c r="H54" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="55" spans="8:8" x14ac:dyDescent="0.3">
-      <c r="H55" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="56" spans="8:8" x14ac:dyDescent="0.3">
-      <c r="H56" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="57" spans="8:8" x14ac:dyDescent="0.3">
-      <c r="H57" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="58" spans="8:8" x14ac:dyDescent="0.3">
-      <c r="H58" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="59" spans="8:8" x14ac:dyDescent="0.3">
-      <c r="H59" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="60" spans="8:8" x14ac:dyDescent="0.3">
-      <c r="H60" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="61" spans="8:8" x14ac:dyDescent="0.3">
-      <c r="H61" t="s">
-        <v>85</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
@@ -6040,186 +6051,186 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="13" customWidth="1"/>
-    <col min="2" max="2" width="48.44140625" customWidth="1"/>
+    <col min="2" max="2" width="48.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>86</v>
+        <v>27</v>
       </c>
       <c r="B1" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>88</v>
+        <v>29</v>
       </c>
       <c r="B2" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>90</v>
+        <v>31</v>
       </c>
       <c r="B3" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>92</v>
+        <v>33</v>
       </c>
       <c r="B4" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>94</v>
+        <v>35</v>
       </c>
       <c r="B5" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>96</v>
+        <v>37</v>
       </c>
       <c r="B6" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>98</v>
+        <v>39</v>
       </c>
       <c r="B7" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>100</v>
+        <v>41</v>
       </c>
       <c r="B8" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>102</v>
+        <v>43</v>
       </c>
       <c r="B9" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>104</v>
+        <v>45</v>
       </c>
       <c r="B10" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>106</v>
+        <v>47</v>
       </c>
       <c r="B11" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>108</v>
+        <v>49</v>
       </c>
       <c r="B12" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
-        <v>110</v>
+        <v>51</v>
       </c>
       <c r="B13" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
-        <v>112</v>
+        <v>53</v>
       </c>
       <c r="B14" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
-        <v>114</v>
+        <v>55</v>
       </c>
       <c r="B15" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
-        <v>116</v>
+        <v>57</v>
       </c>
       <c r="B16" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
-        <v>118</v>
+        <v>59</v>
       </c>
       <c r="B17" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
-        <v>120</v>
+        <v>61</v>
       </c>
       <c r="B18" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
-        <v>122</v>
+        <v>63</v>
       </c>
       <c r="B19" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
-        <v>124</v>
+        <v>65</v>
       </c>
       <c r="B20" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
-        <v>126</v>
+        <v>67</v>
       </c>
       <c r="B21" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
-        <v>128</v>
+        <v>69</v>
       </c>
       <c r="B22" t="s">
-        <v>129</v>
+        <v>70</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
enable conceptual data modeling only
</commit_message>
<xml_diff>
--- a/tests/data/_schema/conceptual/only_concepts.xlsx
+++ b/tests/data/_schema/conceptual/only_concepts.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10512"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10608"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nikola/Repos/neat/tests/data/_schema/conceptual/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nikola/repos/neat/tests/data/_schema/conceptual/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6686FB3-51CC-9A4D-B93E-56A519791CEC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB6B53BE-3F41-2646-B060-DCC390CBA55E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="48520" windowHeight="27500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="860" windowWidth="38400" windowHeight="24000" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Metadata" sheetId="1" r:id="rId1"/>
-    <sheet name="Properties" sheetId="2" r:id="rId2"/>
-    <sheet name="Classes" sheetId="3" r:id="rId3"/>
+    <sheet name="Concepts" sheetId="3" r:id="rId2"/>
+    <sheet name="Properties" sheetId="2" r:id="rId3"/>
     <sheet name="Prefixes" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="0"/>
@@ -70,9 +70,6 @@
     <t>Definition of Properties</t>
   </si>
   <si>
-    <t>Class</t>
-  </si>
-  <si>
     <t>Property</t>
   </si>
   <si>
@@ -100,9 +97,6 @@
     <t>Neat ID</t>
   </si>
   <si>
-    <t>Definition of Classes</t>
-  </si>
-  <si>
     <t>Implements</t>
   </si>
   <si>
@@ -437,6 +431,12 @@
   </si>
   <si>
     <t>http://purl.org/cognite/neat/data-model/verified/conceptual/neat_space/NeatInferredDataModel/v1/ScheduleResourceGeneration</t>
+  </si>
+  <si>
+    <t>Concept</t>
+  </si>
+  <si>
+    <t>Definition of Concepts</t>
   </si>
 </sst>
 </file>
@@ -868,7 +868,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="16" x14ac:dyDescent="0.2">
@@ -876,7 +876,7 @@
         <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="16" x14ac:dyDescent="0.2">
@@ -892,7 +892,7 @@
         <v>6</v>
       </c>
       <c r="B5" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="16" x14ac:dyDescent="0.2">
@@ -900,7 +900,7 @@
         <v>7</v>
       </c>
       <c r="B6" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="16" x14ac:dyDescent="0.2">
@@ -908,7 +908,7 @@
         <v>8</v>
       </c>
       <c r="B7" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="16" x14ac:dyDescent="0.2">
@@ -948,12 +948,382 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:H61"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D16" sqref="D16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="26.5" customWidth="1"/>
+    <col min="2" max="3" width="13" customWidth="1"/>
+    <col min="4" max="4" width="29.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="70" customWidth="1"/>
+    <col min="6" max="7" width="13" customWidth="1"/>
+    <col min="8" max="8" width="70" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" ht="26" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
+      <c r="H1" s="4"/>
+    </row>
+    <row r="2" spans="1:8" ht="19" x14ac:dyDescent="0.25">
+      <c r="A2" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="H2" s="5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>74</v>
+      </c>
+      <c r="D3" t="s">
+        <v>75</v>
+      </c>
+      <c r="H3" s="8" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>76</v>
+      </c>
+      <c r="D4" t="s">
+        <v>74</v>
+      </c>
+      <c r="H4" s="8" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="H5" s="8" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="H6" s="8" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="H7" s="8" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="H8" s="8" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="H9" s="8" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="H10" s="8" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="H11" s="8" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="H12" s="8" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="H13" s="8" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="H14" s="8" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="H15" s="8" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="H16" s="8" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="17" spans="8:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="H17" s="8" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="18" spans="8:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="H18" s="8" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="19" spans="8:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="H19" s="8" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="20" spans="8:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="H20" s="8" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="21" spans="8:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="H21" s="8" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="22" spans="8:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="H22" s="8" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="23" spans="8:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="H23" s="8" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="24" spans="8:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="H24" s="8" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="25" spans="8:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="H25" s="8" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="26" spans="8:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="H26" s="8" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="27" spans="8:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="H27" s="8" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="28" spans="8:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="H28" s="8" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="29" spans="8:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="H29" s="8" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="30" spans="8:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="H30" s="8" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="31" spans="8:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="H31" s="8" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="32" spans="8:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="H32" s="8" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="33" spans="8:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="H33" s="8" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="34" spans="8:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="H34" s="8" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="35" spans="8:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="H35" s="8" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="36" spans="8:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="H36" s="8" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="37" spans="8:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="H37" s="8" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="38" spans="8:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="H38" s="8" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="39" spans="8:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="H39" s="8" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="40" spans="8:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="H40" s="8" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="41" spans="8:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="H41" s="8" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="42" spans="8:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="H42" s="8" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="43" spans="8:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="H43" s="8" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="44" spans="8:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="H44" s="8" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="45" spans="8:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="H45" s="8" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="46" spans="8:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="H46" s="8" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="47" spans="8:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="H47" s="8" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="48" spans="8:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="H48" s="8" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="49" spans="8:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="H49" s="8" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="50" spans="8:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="H50" s="8" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="51" spans="8:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="H51" s="8" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="52" spans="8:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="H52" s="8" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="53" spans="8:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="H53" s="8" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="54" spans="8:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="H54" s="8" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="55" spans="8:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="H55" s="8" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="56" spans="8:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="H56" s="8" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="57" spans="8:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="H57" s="8" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="58" spans="8:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="H58" s="8" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="59" spans="8:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="H59" s="8" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="60" spans="8:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="H60" s="8" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="61" spans="8:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="H61" s="8" t="s">
+        <v>135</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:L334"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F20" sqref="F20"/>
+      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -986,31 +1356,31 @@
     </row>
     <row r="2" spans="1:12" ht="19" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="B2" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="C2" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="D2" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="E2" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="F2" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="G2" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="G2" s="5" t="s">
+      <c r="H2" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="H2" s="5" t="s">
+      <c r="I2" s="5" t="s">
         <v>22</v>
-      </c>
-      <c r="I2" s="5" t="s">
-        <v>23</v>
       </c>
       <c r="J2" s="5" t="s">
         <v>12</v>
@@ -1019,7 +1389,7 @@
         <v>13</v>
       </c>
       <c r="L2" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.2">
@@ -5672,376 +6042,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:H61"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H3" sqref="H3:H61"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="26.5" customWidth="1"/>
-    <col min="2" max="3" width="13" customWidth="1"/>
-    <col min="4" max="4" width="29.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="70" customWidth="1"/>
-    <col min="6" max="7" width="13" customWidth="1"/>
-    <col min="8" max="8" width="70" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:8" ht="26" x14ac:dyDescent="0.3">
-      <c r="A1" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="B1" s="4"/>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
-      <c r="G1" s="4"/>
-      <c r="H1" s="4"/>
-    </row>
-    <row r="2" spans="1:8" ht="19" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="E2" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="F2" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="G2" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="H2" s="5" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" ht="16" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>76</v>
-      </c>
-      <c r="D3" t="s">
-        <v>77</v>
-      </c>
-      <c r="H3" s="8" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" ht="16" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>78</v>
-      </c>
-      <c r="D4" t="s">
-        <v>76</v>
-      </c>
-      <c r="H4" s="8" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" ht="16" x14ac:dyDescent="0.2">
-      <c r="H5" s="8" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" ht="16" x14ac:dyDescent="0.2">
-      <c r="H6" s="8" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" ht="16" x14ac:dyDescent="0.2">
-      <c r="H7" s="8" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" ht="16" x14ac:dyDescent="0.2">
-      <c r="H8" s="8" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" ht="16" x14ac:dyDescent="0.2">
-      <c r="H9" s="8" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" ht="16" x14ac:dyDescent="0.2">
-      <c r="H10" s="8" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" ht="16" x14ac:dyDescent="0.2">
-      <c r="H11" s="8" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" ht="16" x14ac:dyDescent="0.2">
-      <c r="H12" s="8" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" ht="16" x14ac:dyDescent="0.2">
-      <c r="H13" s="8" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" ht="16" x14ac:dyDescent="0.2">
-      <c r="H14" s="8" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" ht="16" x14ac:dyDescent="0.2">
-      <c r="H15" s="8" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" ht="16" x14ac:dyDescent="0.2">
-      <c r="H16" s="8" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="17" spans="8:8" ht="16" x14ac:dyDescent="0.2">
-      <c r="H17" s="8" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="18" spans="8:8" ht="16" x14ac:dyDescent="0.2">
-      <c r="H18" s="8" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="19" spans="8:8" ht="16" x14ac:dyDescent="0.2">
-      <c r="H19" s="8" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="20" spans="8:8" ht="16" x14ac:dyDescent="0.2">
-      <c r="H20" s="8" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="21" spans="8:8" ht="16" x14ac:dyDescent="0.2">
-      <c r="H21" s="8" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="22" spans="8:8" ht="16" x14ac:dyDescent="0.2">
-      <c r="H22" s="8" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="23" spans="8:8" ht="16" x14ac:dyDescent="0.2">
-      <c r="H23" s="8" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="24" spans="8:8" ht="16" x14ac:dyDescent="0.2">
-      <c r="H24" s="8" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="25" spans="8:8" ht="16" x14ac:dyDescent="0.2">
-      <c r="H25" s="8" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="26" spans="8:8" ht="16" x14ac:dyDescent="0.2">
-      <c r="H26" s="8" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="27" spans="8:8" ht="16" x14ac:dyDescent="0.2">
-      <c r="H27" s="8" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="28" spans="8:8" ht="16" x14ac:dyDescent="0.2">
-      <c r="H28" s="8" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="29" spans="8:8" ht="16" x14ac:dyDescent="0.2">
-      <c r="H29" s="8" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="30" spans="8:8" ht="16" x14ac:dyDescent="0.2">
-      <c r="H30" s="8" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="31" spans="8:8" ht="16" x14ac:dyDescent="0.2">
-      <c r="H31" s="8" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="32" spans="8:8" ht="16" x14ac:dyDescent="0.2">
-      <c r="H32" s="8" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="33" spans="8:8" ht="16" x14ac:dyDescent="0.2">
-      <c r="H33" s="8" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="34" spans="8:8" ht="16" x14ac:dyDescent="0.2">
-      <c r="H34" s="8" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="35" spans="8:8" ht="16" x14ac:dyDescent="0.2">
-      <c r="H35" s="8" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="36" spans="8:8" ht="16" x14ac:dyDescent="0.2">
-      <c r="H36" s="8" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="37" spans="8:8" ht="16" x14ac:dyDescent="0.2">
-      <c r="H37" s="8" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="38" spans="8:8" ht="16" x14ac:dyDescent="0.2">
-      <c r="H38" s="8" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="39" spans="8:8" ht="16" x14ac:dyDescent="0.2">
-      <c r="H39" s="8" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="40" spans="8:8" ht="16" x14ac:dyDescent="0.2">
-      <c r="H40" s="8" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="41" spans="8:8" ht="16" x14ac:dyDescent="0.2">
-      <c r="H41" s="8" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="42" spans="8:8" ht="16" x14ac:dyDescent="0.2">
-      <c r="H42" s="8" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="43" spans="8:8" ht="16" x14ac:dyDescent="0.2">
-      <c r="H43" s="8" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="44" spans="8:8" ht="16" x14ac:dyDescent="0.2">
-      <c r="H44" s="8" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="45" spans="8:8" ht="16" x14ac:dyDescent="0.2">
-      <c r="H45" s="8" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="46" spans="8:8" ht="16" x14ac:dyDescent="0.2">
-      <c r="H46" s="8" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="47" spans="8:8" ht="16" x14ac:dyDescent="0.2">
-      <c r="H47" s="8" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="48" spans="8:8" ht="16" x14ac:dyDescent="0.2">
-      <c r="H48" s="8" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="49" spans="8:8" ht="16" x14ac:dyDescent="0.2">
-      <c r="H49" s="8" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="50" spans="8:8" ht="16" x14ac:dyDescent="0.2">
-      <c r="H50" s="8" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="51" spans="8:8" ht="16" x14ac:dyDescent="0.2">
-      <c r="H51" s="8" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="52" spans="8:8" ht="16" x14ac:dyDescent="0.2">
-      <c r="H52" s="8" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="53" spans="8:8" ht="16" x14ac:dyDescent="0.2">
-      <c r="H53" s="8" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="54" spans="8:8" ht="16" x14ac:dyDescent="0.2">
-      <c r="H54" s="8" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="55" spans="8:8" ht="16" x14ac:dyDescent="0.2">
-      <c r="H55" s="8" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="56" spans="8:8" ht="16" x14ac:dyDescent="0.2">
-      <c r="H56" s="8" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="57" spans="8:8" ht="16" x14ac:dyDescent="0.2">
-      <c r="H57" s="8" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="58" spans="8:8" ht="16" x14ac:dyDescent="0.2">
-      <c r="H58" s="8" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="59" spans="8:8" ht="16" x14ac:dyDescent="0.2">
-      <c r="H59" s="8" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="60" spans="8:8" ht="16" x14ac:dyDescent="0.2">
-      <c r="H60" s="8" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="61" spans="8:8" ht="16" x14ac:dyDescent="0.2">
-      <c r="H61" s="8" t="s">
-        <v>137</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
@@ -6059,178 +6059,178 @@
   <sheetData>
     <row r="1" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B3" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B4" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B5" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B6" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B7" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B8" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B9" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B10" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B11" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B12" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B13" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B14" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B15" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B16" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B17" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B18" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B19" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B20" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B21" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B22" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Enable concept only conceptual data models (#1247)
# Description

This enables conceptual data models to consist of only concepts. It
raises nice warning.

Risk reviewers: This is stacked PR on top of
[1246](https://github.com/cognitedata/neat/pull/1246)

## Bump

- [x] Patch
- [ ] Minor
- [ ] Skip

## Changelog
### Improved

- Concept only conceptual data models are now allowed

---------

Co-authored-by: Nikola Vasiljevic <nikola@Nikolas-MacBook-Air.local>
</commit_message>
<xml_diff>
--- a/tests/data/_schema/conceptual/only_concepts.xlsx
+++ b/tests/data/_schema/conceptual/only_concepts.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10512"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10608"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nikola/Repos/neat/tests/data/_schema/conceptual/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nikola/repos/neat/tests/data/_schema/conceptual/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6686FB3-51CC-9A4D-B93E-56A519791CEC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB6B53BE-3F41-2646-B060-DCC390CBA55E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="48520" windowHeight="27500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="860" windowWidth="38400" windowHeight="24000" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Metadata" sheetId="1" r:id="rId1"/>
-    <sheet name="Properties" sheetId="2" r:id="rId2"/>
-    <sheet name="Classes" sheetId="3" r:id="rId3"/>
+    <sheet name="Concepts" sheetId="3" r:id="rId2"/>
+    <sheet name="Properties" sheetId="2" r:id="rId3"/>
     <sheet name="Prefixes" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="0"/>
@@ -70,9 +70,6 @@
     <t>Definition of Properties</t>
   </si>
   <si>
-    <t>Class</t>
-  </si>
-  <si>
     <t>Property</t>
   </si>
   <si>
@@ -100,9 +97,6 @@
     <t>Neat ID</t>
   </si>
   <si>
-    <t>Definition of Classes</t>
-  </si>
-  <si>
     <t>Implements</t>
   </si>
   <si>
@@ -437,6 +431,12 @@
   </si>
   <si>
     <t>http://purl.org/cognite/neat/data-model/verified/conceptual/neat_space/NeatInferredDataModel/v1/ScheduleResourceGeneration</t>
+  </si>
+  <si>
+    <t>Concept</t>
+  </si>
+  <si>
+    <t>Definition of Concepts</t>
   </si>
 </sst>
 </file>
@@ -868,7 +868,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="16" x14ac:dyDescent="0.2">
@@ -876,7 +876,7 @@
         <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="16" x14ac:dyDescent="0.2">
@@ -892,7 +892,7 @@
         <v>6</v>
       </c>
       <c r="B5" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="16" x14ac:dyDescent="0.2">
@@ -900,7 +900,7 @@
         <v>7</v>
       </c>
       <c r="B6" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="16" x14ac:dyDescent="0.2">
@@ -908,7 +908,7 @@
         <v>8</v>
       </c>
       <c r="B7" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="16" x14ac:dyDescent="0.2">
@@ -948,12 +948,382 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:H61"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D16" sqref="D16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="26.5" customWidth="1"/>
+    <col min="2" max="3" width="13" customWidth="1"/>
+    <col min="4" max="4" width="29.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="70" customWidth="1"/>
+    <col min="6" max="7" width="13" customWidth="1"/>
+    <col min="8" max="8" width="70" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" ht="26" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
+      <c r="H1" s="4"/>
+    </row>
+    <row r="2" spans="1:8" ht="19" x14ac:dyDescent="0.25">
+      <c r="A2" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="H2" s="5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>74</v>
+      </c>
+      <c r="D3" t="s">
+        <v>75</v>
+      </c>
+      <c r="H3" s="8" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>76</v>
+      </c>
+      <c r="D4" t="s">
+        <v>74</v>
+      </c>
+      <c r="H4" s="8" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="H5" s="8" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="H6" s="8" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="H7" s="8" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="H8" s="8" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="H9" s="8" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="H10" s="8" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="H11" s="8" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="H12" s="8" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="H13" s="8" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="H14" s="8" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="H15" s="8" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="H16" s="8" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="17" spans="8:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="H17" s="8" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="18" spans="8:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="H18" s="8" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="19" spans="8:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="H19" s="8" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="20" spans="8:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="H20" s="8" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="21" spans="8:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="H21" s="8" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="22" spans="8:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="H22" s="8" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="23" spans="8:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="H23" s="8" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="24" spans="8:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="H24" s="8" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="25" spans="8:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="H25" s="8" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="26" spans="8:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="H26" s="8" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="27" spans="8:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="H27" s="8" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="28" spans="8:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="H28" s="8" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="29" spans="8:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="H29" s="8" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="30" spans="8:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="H30" s="8" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="31" spans="8:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="H31" s="8" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="32" spans="8:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="H32" s="8" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="33" spans="8:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="H33" s="8" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="34" spans="8:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="H34" s="8" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="35" spans="8:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="H35" s="8" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="36" spans="8:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="H36" s="8" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="37" spans="8:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="H37" s="8" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="38" spans="8:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="H38" s="8" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="39" spans="8:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="H39" s="8" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="40" spans="8:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="H40" s="8" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="41" spans="8:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="H41" s="8" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="42" spans="8:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="H42" s="8" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="43" spans="8:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="H43" s="8" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="44" spans="8:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="H44" s="8" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="45" spans="8:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="H45" s="8" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="46" spans="8:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="H46" s="8" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="47" spans="8:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="H47" s="8" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="48" spans="8:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="H48" s="8" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="49" spans="8:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="H49" s="8" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="50" spans="8:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="H50" s="8" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="51" spans="8:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="H51" s="8" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="52" spans="8:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="H52" s="8" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="53" spans="8:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="H53" s="8" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="54" spans="8:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="H54" s="8" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="55" spans="8:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="H55" s="8" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="56" spans="8:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="H56" s="8" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="57" spans="8:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="H57" s="8" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="58" spans="8:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="H58" s="8" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="59" spans="8:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="H59" s="8" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="60" spans="8:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="H60" s="8" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="61" spans="8:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="H61" s="8" t="s">
+        <v>135</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:L334"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F20" sqref="F20"/>
+      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -986,31 +1356,31 @@
     </row>
     <row r="2" spans="1:12" ht="19" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="B2" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="C2" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="D2" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="E2" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="F2" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="G2" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="G2" s="5" t="s">
+      <c r="H2" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="H2" s="5" t="s">
+      <c r="I2" s="5" t="s">
         <v>22</v>
-      </c>
-      <c r="I2" s="5" t="s">
-        <v>23</v>
       </c>
       <c r="J2" s="5" t="s">
         <v>12</v>
@@ -1019,7 +1389,7 @@
         <v>13</v>
       </c>
       <c r="L2" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.2">
@@ -5672,376 +6042,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:H61"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H3" sqref="H3:H61"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="26.5" customWidth="1"/>
-    <col min="2" max="3" width="13" customWidth="1"/>
-    <col min="4" max="4" width="29.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="70" customWidth="1"/>
-    <col min="6" max="7" width="13" customWidth="1"/>
-    <col min="8" max="8" width="70" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:8" ht="26" x14ac:dyDescent="0.3">
-      <c r="A1" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="B1" s="4"/>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
-      <c r="G1" s="4"/>
-      <c r="H1" s="4"/>
-    </row>
-    <row r="2" spans="1:8" ht="19" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="E2" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="F2" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="G2" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="H2" s="5" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" ht="16" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>76</v>
-      </c>
-      <c r="D3" t="s">
-        <v>77</v>
-      </c>
-      <c r="H3" s="8" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" ht="16" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>78</v>
-      </c>
-      <c r="D4" t="s">
-        <v>76</v>
-      </c>
-      <c r="H4" s="8" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" ht="16" x14ac:dyDescent="0.2">
-      <c r="H5" s="8" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" ht="16" x14ac:dyDescent="0.2">
-      <c r="H6" s="8" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" ht="16" x14ac:dyDescent="0.2">
-      <c r="H7" s="8" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" ht="16" x14ac:dyDescent="0.2">
-      <c r="H8" s="8" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" ht="16" x14ac:dyDescent="0.2">
-      <c r="H9" s="8" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" ht="16" x14ac:dyDescent="0.2">
-      <c r="H10" s="8" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" ht="16" x14ac:dyDescent="0.2">
-      <c r="H11" s="8" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" ht="16" x14ac:dyDescent="0.2">
-      <c r="H12" s="8" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" ht="16" x14ac:dyDescent="0.2">
-      <c r="H13" s="8" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" ht="16" x14ac:dyDescent="0.2">
-      <c r="H14" s="8" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" ht="16" x14ac:dyDescent="0.2">
-      <c r="H15" s="8" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" ht="16" x14ac:dyDescent="0.2">
-      <c r="H16" s="8" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="17" spans="8:8" ht="16" x14ac:dyDescent="0.2">
-      <c r="H17" s="8" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="18" spans="8:8" ht="16" x14ac:dyDescent="0.2">
-      <c r="H18" s="8" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="19" spans="8:8" ht="16" x14ac:dyDescent="0.2">
-      <c r="H19" s="8" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="20" spans="8:8" ht="16" x14ac:dyDescent="0.2">
-      <c r="H20" s="8" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="21" spans="8:8" ht="16" x14ac:dyDescent="0.2">
-      <c r="H21" s="8" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="22" spans="8:8" ht="16" x14ac:dyDescent="0.2">
-      <c r="H22" s="8" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="23" spans="8:8" ht="16" x14ac:dyDescent="0.2">
-      <c r="H23" s="8" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="24" spans="8:8" ht="16" x14ac:dyDescent="0.2">
-      <c r="H24" s="8" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="25" spans="8:8" ht="16" x14ac:dyDescent="0.2">
-      <c r="H25" s="8" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="26" spans="8:8" ht="16" x14ac:dyDescent="0.2">
-      <c r="H26" s="8" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="27" spans="8:8" ht="16" x14ac:dyDescent="0.2">
-      <c r="H27" s="8" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="28" spans="8:8" ht="16" x14ac:dyDescent="0.2">
-      <c r="H28" s="8" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="29" spans="8:8" ht="16" x14ac:dyDescent="0.2">
-      <c r="H29" s="8" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="30" spans="8:8" ht="16" x14ac:dyDescent="0.2">
-      <c r="H30" s="8" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="31" spans="8:8" ht="16" x14ac:dyDescent="0.2">
-      <c r="H31" s="8" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="32" spans="8:8" ht="16" x14ac:dyDescent="0.2">
-      <c r="H32" s="8" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="33" spans="8:8" ht="16" x14ac:dyDescent="0.2">
-      <c r="H33" s="8" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="34" spans="8:8" ht="16" x14ac:dyDescent="0.2">
-      <c r="H34" s="8" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="35" spans="8:8" ht="16" x14ac:dyDescent="0.2">
-      <c r="H35" s="8" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="36" spans="8:8" ht="16" x14ac:dyDescent="0.2">
-      <c r="H36" s="8" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="37" spans="8:8" ht="16" x14ac:dyDescent="0.2">
-      <c r="H37" s="8" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="38" spans="8:8" ht="16" x14ac:dyDescent="0.2">
-      <c r="H38" s="8" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="39" spans="8:8" ht="16" x14ac:dyDescent="0.2">
-      <c r="H39" s="8" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="40" spans="8:8" ht="16" x14ac:dyDescent="0.2">
-      <c r="H40" s="8" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="41" spans="8:8" ht="16" x14ac:dyDescent="0.2">
-      <c r="H41" s="8" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="42" spans="8:8" ht="16" x14ac:dyDescent="0.2">
-      <c r="H42" s="8" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="43" spans="8:8" ht="16" x14ac:dyDescent="0.2">
-      <c r="H43" s="8" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="44" spans="8:8" ht="16" x14ac:dyDescent="0.2">
-      <c r="H44" s="8" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="45" spans="8:8" ht="16" x14ac:dyDescent="0.2">
-      <c r="H45" s="8" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="46" spans="8:8" ht="16" x14ac:dyDescent="0.2">
-      <c r="H46" s="8" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="47" spans="8:8" ht="16" x14ac:dyDescent="0.2">
-      <c r="H47" s="8" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="48" spans="8:8" ht="16" x14ac:dyDescent="0.2">
-      <c r="H48" s="8" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="49" spans="8:8" ht="16" x14ac:dyDescent="0.2">
-      <c r="H49" s="8" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="50" spans="8:8" ht="16" x14ac:dyDescent="0.2">
-      <c r="H50" s="8" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="51" spans="8:8" ht="16" x14ac:dyDescent="0.2">
-      <c r="H51" s="8" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="52" spans="8:8" ht="16" x14ac:dyDescent="0.2">
-      <c r="H52" s="8" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="53" spans="8:8" ht="16" x14ac:dyDescent="0.2">
-      <c r="H53" s="8" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="54" spans="8:8" ht="16" x14ac:dyDescent="0.2">
-      <c r="H54" s="8" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="55" spans="8:8" ht="16" x14ac:dyDescent="0.2">
-      <c r="H55" s="8" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="56" spans="8:8" ht="16" x14ac:dyDescent="0.2">
-      <c r="H56" s="8" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="57" spans="8:8" ht="16" x14ac:dyDescent="0.2">
-      <c r="H57" s="8" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="58" spans="8:8" ht="16" x14ac:dyDescent="0.2">
-      <c r="H58" s="8" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="59" spans="8:8" ht="16" x14ac:dyDescent="0.2">
-      <c r="H59" s="8" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="60" spans="8:8" ht="16" x14ac:dyDescent="0.2">
-      <c r="H60" s="8" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="61" spans="8:8" ht="16" x14ac:dyDescent="0.2">
-      <c r="H61" s="8" t="s">
-        <v>137</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
@@ -6059,178 +6059,178 @@
   <sheetData>
     <row r="1" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B3" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B4" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B5" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B6" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B7" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B8" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B9" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B10" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B11" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B12" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B13" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B14" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B15" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B16" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B17" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B18" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B19" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B20" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B21" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B22" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
   </sheetData>

</xml_diff>